<commit_message>
Added writing tips from HJ
</commit_message>
<xml_diff>
--- a/read-and-write-kana/Note Types/Read & Write Kana/Read & Write Kana - Data Sheet.xlsx
+++ b/read-and-write-kana/Note Types/Read & Write Kana/Read & Write Kana - Data Sheet.xlsx
@@ -9,12 +9,12 @@
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="122211"/>
+  <calcPr calcId="152511"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="745" uniqueCount="531">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="929" uniqueCount="715">
   <si>
     <t>あ</t>
   </si>
@@ -1607,6 +1607,558 @@
   </si>
   <si>
     <t>zwi, zi</t>
+  </si>
+  <si>
+    <t>In &lt;i&gt;a&lt;/i&gt;, it&amp;rsquo;s important that the last stroke intersects the two places I have circled on the left. Notice, also, that the very end of the last stroke is &amp;ldquo;trying&amp;rdquo; to finish a complete circle. In other words, don&amp;rsquo;t make it pointing down or some other direction.</t>
+  </si>
+  <si>
+    <t>Writing Tip</t>
+  </si>
+  <si>
+    <t>Writing Tip Illustration</t>
+  </si>
+  <si>
+    <t>Your main concern with &lt;i&gt;i&lt;/i&gt; should be including the &lt;i&gt;hane&lt;/i&gt;. Create it with a light flick of your pencil, much like you might make a check mark. Also notice that the second stroke is not as long as the first.</t>
+  </si>
+  <si>
+    <t>With &lt;i&gt;u&lt;/i&gt;, be sure you angle the first stroke back, not making it a vertical line. Also, make sure that you start stroke two by veering northeast.</t>
+  </si>
+  <si>
+    <t>To make &lt;i&gt;e&lt;/i&gt; look good, be sure to get the wave in at the end.</t>
+  </si>
+  <si>
+    <t>When you write &lt;i&gt;ka&lt;/i&gt;, try to keep it balanced inside a triangle formed by the second and third strokes. The first stroke comes down in the center of the triangle, parallel to the next stroke.</t>
+  </si>
+  <si>
+    <t>You can place the last stroke correctly in &lt;i&gt;ki&lt;/i&gt; if you imagine an oval sitting inside as shown here.</t>
+  </si>
+  <si>
+    <t>With &lt;i&gt;ku&lt;/i&gt;, just keep the angle to about 90 degrees, perhaps a bit more, and you&amp;rsquo;ll be good.</t>
+  </si>
+  <si>
+    <t>In &lt;i&gt;ke&lt;/i&gt;, be sure to include a good &lt;i&gt;hane&lt;/i&gt; at the end of stroke one. Also, notice that this character looks very good if you veer to the left at the end of stroke three, as shown here by the arrow.</t>
+  </si>
+  <si>
+    <t>Your main concern with &lt;i&gt;ko&lt;/i&gt; should be to keep it from looking like an equals sign. You can do this by honoring the &lt;i&gt;hane&lt;/i&gt; at the end of the first stroke and by keeping the two strokes far enough apart to imagine a square sitting between them.</t>
+  </si>
+  <si>
+    <t>As with &lt;i&gt;ki&lt;/i&gt;, imagine an oval sitting inside &lt;i&gt;sa&lt;/i&gt; to help place the final stroke.</t>
+  </si>
+  <si>
+    <t>Don&amp;rsquo;t make &lt;i&gt;shi&lt;/i&gt; look like a fishhook. You can avoid this by making the end of it point off at a 45-degree angle, not straight up.</t>
+  </si>
+  <si>
+    <t>Just as in &lt;i&gt;ke&lt;/i&gt;, this character looks the best when the final stroke veers to the left at the end. Also, keep the loop nice and open. Japanese people often exaggerate it, so don&amp;rsquo;t worry about making it too large.</t>
+  </si>
+  <si>
+    <t>Besides being careful about the &lt;i&gt;hane&lt;/i&gt; as always, note that the first stroke runs uphill very slightly.</t>
+  </si>
+  <si>
+    <t>&lt;i&gt;So&lt;/i&gt; can be a hard character to write nicely. One thing that can really make a difference is opening up that last curve. Imagine there&amp;rsquo;s a plump oval sitting in there.</t>
+  </si>
+  <si>
+    <t>You&amp;rsquo;ll notice that there is a small &lt;i&gt;ko&lt;/i&gt; inside this character. Give the mini-&lt;i&gt;ko&lt;/i&gt; the same &lt;i&gt;hane&lt;/i&gt; it gets in its grown-up version.</t>
+  </si>
+  <si>
+    <t>In &lt;i&gt;chi&lt;/i&gt;, be sure that the round part of the last stroke starts by veering up slightly, as shown by the arrow.</t>
+  </si>
+  <si>
+    <t>&lt;i&gt;Tsu&lt;/i&gt; is easy to remember if you imagine the breaking wave of a &lt;i&gt;tsunami&lt;/i&gt;.</t>
+  </si>
+  <si>
+    <t>Keep &lt;i&gt;te&lt;/i&gt; from looking like a 7 by imagining that a large plump ball is sitting in the curve.</t>
+  </si>
+  <si>
+    <t>I think the standard way to remember &lt;i&gt;to&lt;/i&gt; is to think of someone&amp;rsquo;s big toe. If you keep that second stroke open enough to actually put a toe inside, it will look nice.</t>
+  </si>
+  <si>
+    <t>When writing this character, note that the third stroke veers to the right ever so slightly. If you swing it out just a bit there, it makes a big difference in the balance of the character.</t>
+  </si>
+  <si>
+    <t>&lt;i&gt;Ni&lt;/i&gt; is similar to &lt;i&gt;ta&lt;/i&gt; in that the last two strokes should not be quite parallel. Taking this one simple precaution really helps the look of this character.</t>
+  </si>
+  <si>
+    <t>My main advice for &lt;i&gt;nu&lt;/i&gt; is that you make the first stroke long enough that the second will intersect it and leave a little hanging over, as I&amp;rsquo;ve shown in red.</t>
+  </si>
+  <si>
+    <t>&lt;i&gt;Ne&lt;/i&gt; doesn&amp;rsquo;t look good when people confuse it with &lt;i&gt;nu&lt;/i&gt; and make the first stroke diagonal. Bring it straight down, nice and strong.</t>
+  </si>
+  <si>
+    <t>The main thing to notice in &lt;i&gt;no&lt;/i&gt; is how perfect an oval it is. When you lift up your pencil at the end, you should be able to see little dashed lines in your imagination that close the circle.</t>
+  </si>
+  <si>
+    <t>With &lt;i&gt;ha&lt;/i&gt;, just be sure to get the &lt;i&gt;hane&lt;/i&gt; at the end of stroke 1. Also, when you make the loop at the end of the last stroke, be sure to make it wider than it is tall, as shown here.</t>
+  </si>
+  <si>
+    <t>The biggest problem students have with &lt;i&gt;hi&lt;/i&gt; is they always make the loop too sharp at the bottom. Keep the loop nice and open. Also, notice that the entire character lists to the side. You definitely don&amp;rsquo;t want to make this character look like a U with wings. Lean it slightly to the right.</t>
+  </si>
+  <si>
+    <t>Think of Mount Fuji when writing the character &lt;i&gt;fu&lt;/i&gt;. It should basically fit inside the shape of a triangle.</t>
+  </si>
+  <si>
+    <t>It&amp;rsquo;s pretty hard to go wrong on &lt;i&gt;he&lt;/i&gt;. Just make the downstroke about twice as long as the upstroke.</t>
+  </si>
+  <si>
+    <t>Notice the even spacing of the elements on the right side of &lt;i&gt;ho&lt;/i&gt;. And of course, watch the &lt;i&gt;hane&lt;/i&gt; and the loop as I mentioned for &lt;i&gt;ha&lt;/i&gt;.</t>
+  </si>
+  <si>
+    <t>&lt;i&gt;Mi&lt;/i&gt; looks bad if you don&amp;rsquo;t make the horizontal stroke long enough. Keep the loop open and then draw the arch way over to the right.</t>
+  </si>
+  <si>
+    <t>My comments on &lt;i&gt;ma&lt;/i&gt; are exactly the same as those for &lt;i&gt;ho&lt;/i&gt;. If you take notice again of the even spacing of the elements in this character, you won&amp;rsquo;t make it too elongated.</t>
+  </si>
+  <si>
+    <t>To keep &lt;i&gt;mu&lt;/i&gt; looking sharp, give it a nice wide base, like a travel coffee &lt;b&gt;mu&lt;/b&gt;g.</t>
+  </si>
+  <si>
+    <t>The only thing to watch out for on &lt;i&gt;me&lt;/i&gt; is that the second stroke crosses the first twice, as I&amp;rsquo;ve indicated.</t>
+  </si>
+  <si>
+    <t>Looking at my drawing here, you should be able to see the energy leaving stroke one and pointing toward the first horizontal stroke. &lt;i&gt;Mo&lt;/i&gt; looks great when you veer the end of stroke one off to the northwest as I&amp;rsquo;ve shown.</t>
+  </si>
+  <si>
+    <t>Notice that in &lt;i&gt;ya&lt;/i&gt;, the first and last strokes are perpendicular where they cross. But the cross that is formed is not standing straight up. It&amp;rsquo;s really important to make it lean back like this.</t>
+  </si>
+  <si>
+    <t>&lt;i&gt;Yu&lt;/i&gt; looks really good when you keep fluid as you write it. Notice how the end of stroke one leads right up into the next stroke. Many people even make the whole character into one long stroke by drawing along the path I&amp;rsquo;ve shown here. You may write it whichever way you like.</t>
+  </si>
+  <si>
+    <t>The advice I gave regarding the loops in &lt;i&gt;ha&lt;/i&gt;, &lt;i&gt;ho&lt;/i&gt;, and &lt;i&gt;ma&lt;/i&gt; also holds true here. The only other piece of wisdom I can offer is to make sure that the first stroke and the very end of the second stroke stick out about the same length.</t>
+  </si>
+  <si>
+    <t>My comments on &lt;i&gt;ra&lt;/i&gt; are similar to those for &lt;i&gt;chi&lt;/i&gt;. After you start the second stroke, be sure to come slightly up and over where the arrow shows.</t>
+  </si>
+  <si>
+    <t>With &lt;i&gt;ri&lt;/i&gt;, just watch the &lt;i&gt;hane&lt;/i&gt; at the end of stroke 1.</t>
+  </si>
+  <si>
+    <t>Check out how long the red portion of &lt;i&gt;ru&lt;/i&gt; is here. It comes further to the left than any other part of the character. Be sure to give this line its full value.</t>
+  </si>
+  <si>
+    <t>This character looks an awful lot like &lt;i&gt;ne&lt;/i&gt;, but without the loop. Emphasize the difference by making the final stroke come down strong with a little curl at the end.</t>
+  </si>
+  <si>
+    <t>It&amp;rsquo;s hard to go wrong with this one, but avoid making it look like a 3 by keeping the upper right corner sharp.</t>
+  </si>
+  <si>
+    <t>&lt;i&gt;Wa&lt;/i&gt; looks exactly the same as &lt;i&gt;ne&lt;/i&gt;, only without the final loop. It&amp;rsquo;s also similar in shape to &lt;i&gt;re&lt;/i&gt;. Differentiate it by keeping it nice and open, with plenty of air inside.</t>
+  </si>
+  <si>
+    <t>As strange as this character looks, it&amp;rsquo;s not difficult to write. It might help to imagine it as a hybrid of &lt;i&gt;n&lt;/i&gt; and &lt;i&gt;to&lt;/i&gt;.</t>
+  </si>
+  <si>
+    <t>Don&amp;rsquo;t deny it. I know you&amp;rsquo;re thinking that this looks like an &lt;i&gt;h&lt;/i&gt;. And that&amp;rsquo;s just how you should write it. Just be sure to make it an &lt;u&gt;italic&lt;/u&gt; &lt;i&gt;h&lt;/i&gt;.</t>
+  </si>
+  <si>
+    <t>Keep the angle in stroke one sharp in this character. When you begin stroke two, don&amp;rsquo;t curve it right away. Bring it straight down for a bit before sweeping left.</t>
+  </si>
+  <si>
+    <t>Be sure to bring the second stroke straight down with a solid stop at the bottom. Don&amp;rsquo;t flick your pencil down to make this stroke. Bring it straight down, stop moving the lead, &lt;u&gt;then&lt;/u&gt; pick up your pencil.</t>
+  </si>
+  <si>
+    <t>Notice that the first two strokes and the first part of the third are all perfectly straight. Also, note that the first stroke is centered over the third.</t>
+  </si>
+  <si>
+    <t>Think of a flattened I-beam when you write this one. Notice that the character is slightly wider than it is tall.</t>
+  </si>
+  <si>
+    <t>Notice that the second stroke does not come down through the middle of the first. Keep it slightly off to the right, to make room for stroke three.</t>
+  </si>
+  <si>
+    <t>Your main concerns in this character are the point in the middle of the first stroke and the &lt;i&gt;hane&lt;/i&gt; at the end.</t>
+  </si>
+  <si>
+    <t>Keep this character leaning to the left, reminiscent of its hiragana counterpart. Notice that the last stroke bisects the first two at a 90-degree angle.</t>
+  </si>
+  <si>
+    <t>Here we have two instances of the &amp;ldquo;katakana curve&amp;rdquo; in a single character. If you can master this curve, your characters will look great.</t>
+  </si>
+  <si>
+    <t>Obviously, &lt;i&gt;ke&lt;/i&gt; differs from &lt;i&gt;ku&lt;/i&gt; in that the second stroke is longer. But also notice that the placement of the second stroke is slightly lower, so that it meets the first stroke in the middle, not as high up as in &lt;i&gt;ku&lt;/i&gt;.</t>
+  </si>
+  <si>
+    <t>It&amp;rsquo;s subtle in this font, but in &lt;i&gt;ko&lt;/i&gt;, as in &lt;i&gt;e&lt;/i&gt;, the character is slightly wider than it is tall.</t>
+  </si>
+  <si>
+    <t>In &lt;i&gt;o&lt;/i&gt;, notice how you can see the energy being directed to the final stroke. Follow this flow to keep the character fluid and great-looking.</t>
+  </si>
+  <si>
+    <t>Be careful with &lt;i&gt;sa&lt;/i&gt;, as it looks a lot like the hiragana character &lt;i&gt;se&lt;/i&gt;.</t>
+  </si>
+  <si>
+    <t>The last stroke in this character &lt;strong&gt;must&lt;/strong&gt; be written from the bottom up. Also notice that the angle isn&amp;rsquo;t as steep as in &lt;i&gt;so&lt;/i&gt;, below. The first two strokes point more in the direction of the horizon than the elements of &lt;i&gt;so&lt;/i&gt;.</t>
+  </si>
+  <si>
+    <t>If you find it easier, most people write &lt;i&gt;su&lt;/i&gt; using all straight lines. There&amp;rsquo;s no need to curve the end of the first stroke.</t>
+  </si>
+  <si>
+    <t>Don&amp;rsquo;t skimp on that &lt;i&gt;hane&lt;/i&gt; at the end of the first stroke. Give it the same oomph you might use when finishing off a check mark and you&amp;rsquo;ll have a great looking &lt;i&gt;se&lt;/i&gt;.</t>
+  </si>
+  <si>
+    <t>Make &lt;i&gt;so&lt;/i&gt; look different from &lt;i&gt;shi&lt;/i&gt; by emphasizing the fact that both elements in this character point down to the ground. The second stroke must start from the top.</t>
+  </si>
+  <si>
+    <t>&lt;i&gt;Ta&lt;/i&gt; doesn&amp;rsquo;t present many challenges. Just get that nice &amp;ldquo;katakana curve&amp;rdquo; in there.</t>
+  </si>
+  <si>
+    <t>In &lt;i&gt;chi&lt;/i&gt;, the first stroke starts from the right and goes down and hard to the left, which is very unusual. As a general rule, all strokes go from left to right, and from top to bottom, so you need to remember that this character is special. Also notice that the last stroke pulls straight down, then curves at the end.</t>
+  </si>
+  <si>
+    <t>To remember the difference between &lt;i&gt;tsu&lt;/i&gt; and &lt;i&gt;so&lt;/i&gt;, it might be helpful to remind yourself that &lt;i&gt;tsu&lt;/i&gt; has &amp;ldquo;tsu&amp;rdquo; (two) short strokes at the beginning instead of just one. Like the character &lt;i&gt;so&lt;/i&gt;, the last stroke must come from the top.</t>
+  </si>
+  <si>
+    <t>Keep &lt;i&gt;te&lt;/i&gt; and &lt;i&gt;chi&lt;/i&gt; straight by remembering the two main differences: The first two strokes in &lt;i&gt;te&lt;/i&gt; are parallel, and the third stroke doesn&amp;rsquo;t go all the way through, as it does in &lt;i&gt;chi&lt;/i&gt;.</t>
+  </si>
+  <si>
+    <t>&lt;i&gt;To&lt;/i&gt; is easy. Just keep the first stroke vertical and you&amp;rsquo;ll be fine.</t>
+  </si>
+  <si>
+    <t>Be sure to intersect the first stroke of &lt;i&gt;na&lt;/i&gt; in the center.</t>
+  </si>
+  <si>
+    <t>You can remember &lt;i&gt;ni&lt;/i&gt; because it has two horizontal lines, and &lt;i&gt;ni&lt;/i&gt; is the word for &amp;ldquo;two.&amp;rdquo;</t>
+  </si>
+  <si>
+    <t>This character is basically a &lt;i&gt;ta&lt;/i&gt; without the first stroke.</t>
+  </si>
+  <si>
+    <t>&lt;i&gt;Ne&lt;/i&gt; will look a lot more balanced if you think of the third stroke as a central support pole around which the rest of the character should be distributed evenly.</t>
+  </si>
+  <si>
+    <t>&lt;i&gt;No&lt;/i&gt; is easy to remember because &amp;ldquo;no&amp;rdquo; other lines attach to it.</t>
+  </si>
+  <si>
+    <t>Don&amp;rsquo;t let these strokes connect at the top.</t>
+  </si>
+  <si>
+    <t>Make sure that second stroke forms a solid 90-degree elbow in &lt;i&gt;hi&lt;/i&gt;.</t>
+  </si>
+  <si>
+    <t>It&amp;rsquo;s important with &lt;i&gt;fu&lt;/i&gt; that you don&amp;rsquo;t make the curved part straight. In other words, don&amp;rsquo;t make it look like a 7. It also helps to keep it slightly wider than it is tall.</t>
+  </si>
+  <si>
+    <t>Write this exactly as its cousin.</t>
+  </si>
+  <si>
+    <t>If you learn anything from my notes on the two syllabaries, I hope it&amp;rsquo;s that you should always be sure to include &lt;i&gt;hane&lt;/i&gt; in characters that use them. Here we find a beautiful example at the end of stroke two.</t>
+  </si>
+  <si>
+    <t>When I was learning this syllabary, it helped me to write &lt;i&gt;ma&lt;/i&gt; correctly if I imagined it as a triangular flag on a stick, leaning back at a 45-degree angle.</t>
+  </si>
+  <si>
+    <t>This character might make more sense after you learn another way to say the number three: &lt;i&gt;mittsu&lt;/i&gt;. Just as &lt;i&gt;ni&lt;/i&gt; is composed of &amp;ldquo;two&amp;rdquo; lines, &lt;i&gt;mi&lt;/i&gt; is composed of &amp;ldquo;three.&amp;rdquo;</t>
+  </si>
+  <si>
+    <t>It&amp;rsquo;s hard to go wrong with &lt;i&gt;mu&lt;/i&gt;. Just keep that first stroke to about a 45-degree angle and it&amp;rsquo;ll look great.</t>
+  </si>
+  <si>
+    <t>This one is nice and easy. Just be sure to get that gentle "katakana curve" in, and make the strokes different lengths so it doesn&amp;rsquo;t look like an X, and you&amp;rsquo;ll be fine.</t>
+  </si>
+  <si>
+    <t>&lt;i&gt;Mo&lt;/i&gt; also looks a lot like its cousin. Notice, however, that the stroke order is different. (In the hiragana &lt;i&gt;mo&lt;/i&gt;, the vertical line comes first.)</t>
+  </si>
+  <si>
+    <t>This character looks just like its cousin, except it&amp;rsquo;s more angular and it&amp;rsquo;s missing a stroke. Notice that what used to be an open curve at the end of the first stroke has been reduced to a &lt;i&gt;hane&lt;/i&gt;.</t>
+  </si>
+  <si>
+    <t>Above all else, make sure that the vertical portion of the first stroke in &lt;i&gt;yu&lt;/i&gt; goes straight down or veers a little to the left. It should not go to the right.</t>
+  </si>
+  <si>
+    <t>It&amp;rsquo;s a backwards &amp;ldquo;E.&amp;rdquo; That&amp;rsquo;s all it is. Write it like that and you&amp;rsquo;ll have no problems. Just remember to use the proper stroke order: Each of the two lower arms must be drawn from left to right.</t>
+  </si>
+  <si>
+    <t>This character is simply a &lt;i&gt;fu&lt;/i&gt; with a line on top, but since &lt;i&gt;fu&lt;/i&gt; and &lt;i&gt;ra&lt;/i&gt; should take up the same vertical space, you&amp;rsquo;ll need to compress the &lt;i&gt;fu&lt;/i&gt; part a bit.</t>
+  </si>
+  <si>
+    <t>Notice that with the katakana version of &lt;i&gt;ri&lt;/i&gt;, there is no &lt;i&gt;hane&lt;/i&gt; at the end of stroke one.</t>
+  </si>
+  <si>
+    <t>The end of stroke two in &lt;i&gt;ru&lt;/i&gt; is nothing more than a glorified &lt;i&gt;hane&lt;/i&gt;. Flick the pencil up like you&amp;rsquo;re making a check mark and it&amp;rsquo;ll look perfect.</t>
+  </si>
+  <si>
+    <t>The end of this character is a super-glorified &lt;i&gt;hane&lt;/i&gt;.</t>
+  </si>
+  <si>
+    <t>Be sure to note that the path marked by the red arrow here is actually one large stroke. It&amp;rsquo;s important to write this character correctly, using three strokes, not four.</t>
+  </si>
+  <si>
+    <t>&lt;i&gt;Wa&lt;/i&gt; is the same as &lt;i&gt;u&lt;/i&gt;, only without the line on top.</t>
+  </si>
+  <si>
+    <t>In order to keep this character distinct from the very similar looking &lt;i&gt;so&lt;/i&gt;, be sure that you draw the second stroke up from the bottom, and point it slightly lower than a 45-degree angle.</t>
+  </si>
+  <si>
+    <t>&lt;img src="7biey7947yx7iz074op63ck7x_tips_hiragana_a.png"&gt;</t>
+  </si>
+  <si>
+    <t>&lt;img src="7biey7947yx7iz074op63ck7x_tips_hiragana_i.png"&gt;</t>
+  </si>
+  <si>
+    <t>&lt;img src="7biey7947yx7iz074op63ck7x_tips_hiragana_u.png"&gt;</t>
+  </si>
+  <si>
+    <t>&lt;img src="7biey7947yx7iz074op63ck7x_tips_hiragana_e.png"&gt;</t>
+  </si>
+  <si>
+    <t>&lt;img src="7biey7947yx7iz074op63ck7x_tips_hiragana_o.png"&gt;</t>
+  </si>
+  <si>
+    <t>&lt;img src="7biey7947yx7iz074op63ck7x_tips_hiragana_ka.png"&gt;</t>
+  </si>
+  <si>
+    <t>&lt;img src="7biey7947yx7iz074op63ck7x_tips_hiragana_ki.png"&gt;</t>
+  </si>
+  <si>
+    <t>&lt;img src="7biey7947yx7iz074op63ck7x_tips_hiragana_ku.png"&gt;</t>
+  </si>
+  <si>
+    <t>&lt;img src="7biey7947yx7iz074op63ck7x_tips_hiragana_ke.png"&gt;</t>
+  </si>
+  <si>
+    <t>&lt;img src="7biey7947yx7iz074op63ck7x_tips_hiragana_ko.png"&gt;</t>
+  </si>
+  <si>
+    <t>&lt;img src="7biey7947yx7iz074op63ck7x_tips_hiragana_sa.png"&gt;</t>
+  </si>
+  <si>
+    <t>&lt;img src="7biey7947yx7iz074op63ck7x_tips_hiragana_shi.png"&gt;</t>
+  </si>
+  <si>
+    <t>&lt;img src="7biey7947yx7iz074op63ck7x_tips_hiragana_su.png"&gt;</t>
+  </si>
+  <si>
+    <t>&lt;img src="7biey7947yx7iz074op63ck7x_tips_hiragana_se.png"&gt;</t>
+  </si>
+  <si>
+    <t>&lt;img src="7biey7947yx7iz074op63ck7x_tips_hiragana_so.png"&gt;</t>
+  </si>
+  <si>
+    <t>&lt;img src="7biey7947yx7iz074op63ck7x_tips_hiragana_ta.png"&gt;</t>
+  </si>
+  <si>
+    <t>&lt;img src="7biey7947yx7iz074op63ck7x_tips_hiragana_chi.png"&gt;</t>
+  </si>
+  <si>
+    <t>&lt;img src="7biey7947yx7iz074op63ck7x_tips_hiragana_tsu.png"&gt;</t>
+  </si>
+  <si>
+    <t>&lt;img src="7biey7947yx7iz074op63ck7x_tips_hiragana_te.png"&gt;</t>
+  </si>
+  <si>
+    <t>&lt;img src="7biey7947yx7iz074op63ck7x_tips_hiragana_to.png"&gt;</t>
+  </si>
+  <si>
+    <t>&lt;img src="7biey7947yx7iz074op63ck7x_tips_hiragana_na.png"&gt;</t>
+  </si>
+  <si>
+    <t>&lt;img src="7biey7947yx7iz074op63ck7x_tips_hiragana_ni.png"&gt;</t>
+  </si>
+  <si>
+    <t>&lt;img src="7biey7947yx7iz074op63ck7x_tips_hiragana_nu.png"&gt;</t>
+  </si>
+  <si>
+    <t>&lt;img src="7biey7947yx7iz074op63ck7x_tips_hiragana_ne.png"&gt;</t>
+  </si>
+  <si>
+    <t>&lt;img src="7biey7947yx7iz074op63ck7x_tips_hiragana_no.png"&gt;</t>
+  </si>
+  <si>
+    <t>&lt;img src="7biey7947yx7iz074op63ck7x_tips_hiragana_ha.png"&gt;</t>
+  </si>
+  <si>
+    <t>&lt;img src="7biey7947yx7iz074op63ck7x_tips_hiragana_hi.png"&gt;</t>
+  </si>
+  <si>
+    <t>&lt;img src="7biey7947yx7iz074op63ck7x_tips_hiragana_fu.png"&gt;</t>
+  </si>
+  <si>
+    <t>&lt;img src="7biey7947yx7iz074op63ck7x_tips_hiragana_he.png"&gt;</t>
+  </si>
+  <si>
+    <t>&lt;img src="7biey7947yx7iz074op63ck7x_tips_hiragana_ho.png"&gt;</t>
+  </si>
+  <si>
+    <t>&lt;img src="7biey7947yx7iz074op63ck7x_tips_hiragana_ma.png"&gt;</t>
+  </si>
+  <si>
+    <t>&lt;img src="7biey7947yx7iz074op63ck7x_tips_hiragana_mi.png"&gt;</t>
+  </si>
+  <si>
+    <t>&lt;img src="7biey7947yx7iz074op63ck7x_tips_hiragana_mu.png"&gt;</t>
+  </si>
+  <si>
+    <t>&lt;img src="7biey7947yx7iz074op63ck7x_tips_hiragana_me.png"&gt;</t>
+  </si>
+  <si>
+    <t>&lt;img src="7biey7947yx7iz074op63ck7x_tips_hiragana_mo.png"&gt;</t>
+  </si>
+  <si>
+    <t>&lt;img src="7biey7947yx7iz074op63ck7x_tips_hiragana_ya.png"&gt;</t>
+  </si>
+  <si>
+    <t>&lt;img src="7biey7947yx7iz074op63ck7x_tips_hiragana_yu.png"&gt;</t>
+  </si>
+  <si>
+    <t>&lt;img src="7biey7947yx7iz074op63ck7x_tips_hiragana_yo.png"&gt;</t>
+  </si>
+  <si>
+    <t>&lt;img src="7biey7947yx7iz074op63ck7x_tips_hiragana_ra.png"&gt;</t>
+  </si>
+  <si>
+    <t>&lt;img src="7biey7947yx7iz074op63ck7x_tips_hiragana_ri.png"&gt;</t>
+  </si>
+  <si>
+    <t>&lt;img src="7biey7947yx7iz074op63ck7x_tips_hiragana_ru.png"&gt;</t>
+  </si>
+  <si>
+    <t>&lt;img src="7biey7947yx7iz074op63ck7x_tips_hiragana_re.png"&gt;</t>
+  </si>
+  <si>
+    <t>&lt;img src="7biey7947yx7iz074op63ck7x_tips_hiragana_ro.png"&gt;</t>
+  </si>
+  <si>
+    <t>&lt;img src="7biey7947yx7iz074op63ck7x_tips_hiragana_wa.png"&gt;</t>
+  </si>
+  <si>
+    <t>&lt;img src="7biey7947yx7iz074op63ck7x_tips_hiragana_wo.png"&gt;</t>
+  </si>
+  <si>
+    <t>&lt;img src="7biey7947yx7iz074op63ck7x_tips_hiragana_n.png"&gt;</t>
+  </si>
+  <si>
+    <t>&lt;img src="7biey7947yx7iz074op63ck7x_tips_katakana_a.png"&gt;</t>
+  </si>
+  <si>
+    <t>&lt;img src="7biey7947yx7iz074op63ck7x_tips_katakana_i.png"&gt;</t>
+  </si>
+  <si>
+    <t>&lt;img src="7biey7947yx7iz074op63ck7x_tips_katakana_u.png"&gt;</t>
+  </si>
+  <si>
+    <t>&lt;img src="7biey7947yx7iz074op63ck7x_tips_katakana_e.png"&gt;</t>
+  </si>
+  <si>
+    <t>&lt;img src="7biey7947yx7iz074op63ck7x_tips_katakana_o.png"&gt;</t>
+  </si>
+  <si>
+    <t>&lt;img src="7biey7947yx7iz074op63ck7x_tips_katakana_ka.png"&gt;</t>
+  </si>
+  <si>
+    <t>&lt;img src="7biey7947yx7iz074op63ck7x_tips_katakana_ki.png"&gt;</t>
+  </si>
+  <si>
+    <t>&lt;img src="7biey7947yx7iz074op63ck7x_tips_katakana_ku.png"&gt;</t>
+  </si>
+  <si>
+    <t>&lt;img src="7biey7947yx7iz074op63ck7x_tips_katakana_ke.png"&gt;</t>
+  </si>
+  <si>
+    <t>&lt;img src="7biey7947yx7iz074op63ck7x_tips_katakana_ko.png"&gt;</t>
+  </si>
+  <si>
+    <t>&lt;img src="7biey7947yx7iz074op63ck7x_tips_katakana_sa.png"&gt;</t>
+  </si>
+  <si>
+    <t>&lt;img src="7biey7947yx7iz074op63ck7x_tips_katakana_shi.png"&gt;</t>
+  </si>
+  <si>
+    <t>&lt;img src="7biey7947yx7iz074op63ck7x_tips_katakana_su.png"&gt;</t>
+  </si>
+  <si>
+    <t>&lt;img src="7biey7947yx7iz074op63ck7x_tips_katakana_se.png"&gt;</t>
+  </si>
+  <si>
+    <t>&lt;img src="7biey7947yx7iz074op63ck7x_tips_katakana_so.png"&gt;</t>
+  </si>
+  <si>
+    <t>&lt;img src="7biey7947yx7iz074op63ck7x_tips_katakana_ta.png"&gt;</t>
+  </si>
+  <si>
+    <t>&lt;img src="7biey7947yx7iz074op63ck7x_tips_katakana_chi.png"&gt;</t>
+  </si>
+  <si>
+    <t>&lt;img src="7biey7947yx7iz074op63ck7x_tips_katakana_tsu.png"&gt;</t>
+  </si>
+  <si>
+    <t>&lt;img src="7biey7947yx7iz074op63ck7x_tips_katakana_te.png"&gt;</t>
+  </si>
+  <si>
+    <t>&lt;img src="7biey7947yx7iz074op63ck7x_tips_katakana_to.png"&gt;</t>
+  </si>
+  <si>
+    <t>&lt;img src="7biey7947yx7iz074op63ck7x_tips_katakana_na.png"&gt;</t>
+  </si>
+  <si>
+    <t>&lt;img src="7biey7947yx7iz074op63ck7x_tips_katakana_ni.png"&gt;</t>
+  </si>
+  <si>
+    <t>&lt;img src="7biey7947yx7iz074op63ck7x_tips_katakana_nu.png"&gt;</t>
+  </si>
+  <si>
+    <t>&lt;img src="7biey7947yx7iz074op63ck7x_tips_katakana_ne.png"&gt;</t>
+  </si>
+  <si>
+    <t>&lt;img src="7biey7947yx7iz074op63ck7x_tips_katakana_no.png"&gt;</t>
+  </si>
+  <si>
+    <t>&lt;img src="7biey7947yx7iz074op63ck7x_tips_katakana_ha.png"&gt;</t>
+  </si>
+  <si>
+    <t>&lt;img src="7biey7947yx7iz074op63ck7x_tips_katakana_hi.png"&gt;</t>
+  </si>
+  <si>
+    <t>&lt;img src="7biey7947yx7iz074op63ck7x_tips_katakana_fu.png"&gt;</t>
+  </si>
+  <si>
+    <t>&lt;img src="7biey7947yx7iz074op63ck7x_tips_katakana_he.png"&gt;</t>
+  </si>
+  <si>
+    <t>&lt;img src="7biey7947yx7iz074op63ck7x_tips_katakana_ho.png"&gt;</t>
+  </si>
+  <si>
+    <t>&lt;img src="7biey7947yx7iz074op63ck7x_tips_katakana_ma.png"&gt;</t>
+  </si>
+  <si>
+    <t>&lt;img src="7biey7947yx7iz074op63ck7x_tips_katakana_mi.png"&gt;</t>
+  </si>
+  <si>
+    <t>&lt;img src="7biey7947yx7iz074op63ck7x_tips_katakana_mu.png"&gt;</t>
+  </si>
+  <si>
+    <t>&lt;img src="7biey7947yx7iz074op63ck7x_tips_katakana_me.png"&gt;</t>
+  </si>
+  <si>
+    <t>&lt;img src="7biey7947yx7iz074op63ck7x_tips_katakana_mo.png"&gt;</t>
+  </si>
+  <si>
+    <t>&lt;img src="7biey7947yx7iz074op63ck7x_tips_katakana_ya.png"&gt;</t>
+  </si>
+  <si>
+    <t>&lt;img src="7biey7947yx7iz074op63ck7x_tips_katakana_yu.png"&gt;</t>
+  </si>
+  <si>
+    <t>&lt;img src="7biey7947yx7iz074op63ck7x_tips_katakana_yo.png"&gt;</t>
+  </si>
+  <si>
+    <t>&lt;img src="7biey7947yx7iz074op63ck7x_tips_katakana_ra.png"&gt;</t>
+  </si>
+  <si>
+    <t>&lt;img src="7biey7947yx7iz074op63ck7x_tips_katakana_ri.png"&gt;</t>
+  </si>
+  <si>
+    <t>&lt;img src="7biey7947yx7iz074op63ck7x_tips_katakana_ru.png"&gt;</t>
+  </si>
+  <si>
+    <t>&lt;img src="7biey7947yx7iz074op63ck7x_tips_katakana_re.png"&gt;</t>
+  </si>
+  <si>
+    <t>&lt;img src="7biey7947yx7iz074op63ck7x_tips_katakana_ro.png"&gt;</t>
+  </si>
+  <si>
+    <t>&lt;img src="7biey7947yx7iz074op63ck7x_tips_katakana_wa.png"&gt;</t>
+  </si>
+  <si>
+    <t>&lt;img src="7biey7947yx7iz074op63ck7x_tips_katakana_n.png"&gt;</t>
   </si>
 </sst>
 </file>
@@ -1948,7 +2500,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D256"/>
+  <dimension ref="A1:F256"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -1957,9 +2509,11 @@
     <col min="2" max="2" width="44" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="23.5703125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="22.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="41.7109375" customWidth="1"/>
+    <col min="6" max="6" width="58.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>401</v>
       </c>
@@ -1972,8 +2526,14 @@
       <c r="D1" t="s">
         <v>404</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E1" t="s">
+        <v>532</v>
+      </c>
+      <c r="F1" t="s">
+        <v>533</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -1983,8 +2543,14 @@
       <c r="C2" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E2" t="s">
+        <v>531</v>
+      </c>
+      <c r="F2" t="s">
+        <v>624</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -1994,8 +2560,14 @@
       <c r="C3" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E3" t="s">
+        <v>534</v>
+      </c>
+      <c r="F3" t="s">
+        <v>625</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>4</v>
       </c>
@@ -2005,8 +2577,14 @@
       <c r="C4" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E4" t="s">
+        <v>535</v>
+      </c>
+      <c r="F4" t="s">
+        <v>626</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>6</v>
       </c>
@@ -2016,8 +2594,14 @@
       <c r="C5" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E5" t="s">
+        <v>536</v>
+      </c>
+      <c r="F5" t="s">
+        <v>627</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>8</v>
       </c>
@@ -2027,8 +2611,14 @@
       <c r="C6" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E6" t="s">
+        <v>588</v>
+      </c>
+      <c r="F6" t="s">
+        <v>628</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>10</v>
       </c>
@@ -2038,8 +2628,14 @@
       <c r="C7" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E7" t="s">
+        <v>537</v>
+      </c>
+      <c r="F7" t="s">
+        <v>629</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>12</v>
       </c>
@@ -2049,8 +2645,14 @@
       <c r="C8" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E8" t="s">
+        <v>538</v>
+      </c>
+      <c r="F8" t="s">
+        <v>630</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>14</v>
       </c>
@@ -2060,8 +2662,14 @@
       <c r="C9" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E9" t="s">
+        <v>539</v>
+      </c>
+      <c r="F9" t="s">
+        <v>631</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>16</v>
       </c>
@@ -2071,8 +2679,14 @@
       <c r="C10" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E10" t="s">
+        <v>540</v>
+      </c>
+      <c r="F10" t="s">
+        <v>632</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>18</v>
       </c>
@@ -2082,8 +2696,14 @@
       <c r="C11" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E11" t="s">
+        <v>541</v>
+      </c>
+      <c r="F11" t="s">
+        <v>633</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>20</v>
       </c>
@@ -2093,8 +2713,14 @@
       <c r="C12" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E12" t="s">
+        <v>542</v>
+      </c>
+      <c r="F12" t="s">
+        <v>634</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>22</v>
       </c>
@@ -2104,8 +2730,14 @@
       <c r="C13" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E13" t="s">
+        <v>543</v>
+      </c>
+      <c r="F13" t="s">
+        <v>635</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>24</v>
       </c>
@@ -2115,8 +2747,14 @@
       <c r="C14" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E14" t="s">
+        <v>544</v>
+      </c>
+      <c r="F14" t="s">
+        <v>636</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>26</v>
       </c>
@@ -2126,8 +2764,14 @@
       <c r="C15" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E15" t="s">
+        <v>545</v>
+      </c>
+      <c r="F15" t="s">
+        <v>637</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>28</v>
       </c>
@@ -2137,8 +2781,14 @@
       <c r="C16" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E16" t="s">
+        <v>546</v>
+      </c>
+      <c r="F16" t="s">
+        <v>638</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>30</v>
       </c>
@@ -2148,8 +2798,14 @@
       <c r="C17" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E17" t="s">
+        <v>547</v>
+      </c>
+      <c r="F17" t="s">
+        <v>639</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>32</v>
       </c>
@@ -2159,8 +2815,14 @@
       <c r="C18" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E18" t="s">
+        <v>548</v>
+      </c>
+      <c r="F18" t="s">
+        <v>640</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>34</v>
       </c>
@@ -2170,8 +2832,14 @@
       <c r="C19" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E19" t="s">
+        <v>549</v>
+      </c>
+      <c r="F19" t="s">
+        <v>641</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>36</v>
       </c>
@@ -2181,8 +2849,14 @@
       <c r="C20" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E20" t="s">
+        <v>550</v>
+      </c>
+      <c r="F20" t="s">
+        <v>642</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>38</v>
       </c>
@@ -2192,8 +2866,14 @@
       <c r="C21" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E21" t="s">
+        <v>551</v>
+      </c>
+      <c r="F21" t="s">
+        <v>643</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>40</v>
       </c>
@@ -2203,8 +2883,14 @@
       <c r="C22" t="s">
         <v>41</v>
       </c>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E22" t="s">
+        <v>552</v>
+      </c>
+      <c r="F22" t="s">
+        <v>644</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>42</v>
       </c>
@@ -2214,8 +2900,14 @@
       <c r="C23" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E23" t="s">
+        <v>553</v>
+      </c>
+      <c r="F23" t="s">
+        <v>645</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>44</v>
       </c>
@@ -2225,8 +2917,14 @@
       <c r="C24" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E24" t="s">
+        <v>554</v>
+      </c>
+      <c r="F24" t="s">
+        <v>646</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>46</v>
       </c>
@@ -2236,8 +2934,14 @@
       <c r="C25" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E25" t="s">
+        <v>555</v>
+      </c>
+      <c r="F25" t="s">
+        <v>647</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>48</v>
       </c>
@@ -2247,8 +2951,14 @@
       <c r="C26" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E26" t="s">
+        <v>556</v>
+      </c>
+      <c r="F26" t="s">
+        <v>648</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>50</v>
       </c>
@@ -2258,8 +2968,14 @@
       <c r="C27" t="s">
         <v>51</v>
       </c>
-    </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E27" t="s">
+        <v>557</v>
+      </c>
+      <c r="F27" t="s">
+        <v>649</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>52</v>
       </c>
@@ -2269,8 +2985,14 @@
       <c r="C28" t="s">
         <v>53</v>
       </c>
-    </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E28" t="s">
+        <v>558</v>
+      </c>
+      <c r="F28" t="s">
+        <v>650</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>54</v>
       </c>
@@ -2280,8 +3002,14 @@
       <c r="C29" t="s">
         <v>55</v>
       </c>
-    </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E29" t="s">
+        <v>559</v>
+      </c>
+      <c r="F29" t="s">
+        <v>651</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>56</v>
       </c>
@@ -2291,8 +3019,14 @@
       <c r="C30" t="s">
         <v>57</v>
       </c>
-    </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E30" t="s">
+        <v>560</v>
+      </c>
+      <c r="F30" t="s">
+        <v>652</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>58</v>
       </c>
@@ -2302,8 +3036,14 @@
       <c r="C31" t="s">
         <v>59</v>
       </c>
-    </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E31" t="s">
+        <v>561</v>
+      </c>
+      <c r="F31" t="s">
+        <v>653</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>60</v>
       </c>
@@ -2313,8 +3053,14 @@
       <c r="C32" t="s">
         <v>61</v>
       </c>
-    </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E32" t="s">
+        <v>563</v>
+      </c>
+      <c r="F32" t="s">
+        <v>654</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>62</v>
       </c>
@@ -2324,8 +3070,14 @@
       <c r="C33" t="s">
         <v>63</v>
       </c>
-    </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E33" t="s">
+        <v>562</v>
+      </c>
+      <c r="F33" t="s">
+        <v>655</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>64</v>
       </c>
@@ -2335,8 +3087,14 @@
       <c r="C34" t="s">
         <v>65</v>
       </c>
-    </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E34" t="s">
+        <v>564</v>
+      </c>
+      <c r="F34" t="s">
+        <v>656</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>66</v>
       </c>
@@ -2346,8 +3104,14 @@
       <c r="C35" t="s">
         <v>67</v>
       </c>
-    </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E35" t="s">
+        <v>565</v>
+      </c>
+      <c r="F35" t="s">
+        <v>657</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>68</v>
       </c>
@@ -2357,8 +3121,14 @@
       <c r="C36" t="s">
         <v>69</v>
       </c>
-    </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E36" t="s">
+        <v>566</v>
+      </c>
+      <c r="F36" t="s">
+        <v>658</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>70</v>
       </c>
@@ -2368,8 +3138,14 @@
       <c r="C37" t="s">
         <v>71</v>
       </c>
-    </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E37" t="s">
+        <v>567</v>
+      </c>
+      <c r="F37" t="s">
+        <v>659</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>72</v>
       </c>
@@ -2379,8 +3155,14 @@
       <c r="C38" t="s">
         <v>73</v>
       </c>
-    </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E38" t="s">
+        <v>568</v>
+      </c>
+      <c r="F38" t="s">
+        <v>660</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>74</v>
       </c>
@@ -2390,8 +3172,14 @@
       <c r="C39" t="s">
         <v>75</v>
       </c>
-    </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E39" t="s">
+        <v>569</v>
+      </c>
+      <c r="F39" t="s">
+        <v>661</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>76</v>
       </c>
@@ -2401,8 +3189,14 @@
       <c r="C40" t="s">
         <v>77</v>
       </c>
-    </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E40" t="s">
+        <v>570</v>
+      </c>
+      <c r="F40" t="s">
+        <v>662</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>78</v>
       </c>
@@ -2412,8 +3206,14 @@
       <c r="C41" t="s">
         <v>79</v>
       </c>
-    </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E41" t="s">
+        <v>571</v>
+      </c>
+      <c r="F41" t="s">
+        <v>663</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>80</v>
       </c>
@@ -2423,8 +3223,14 @@
       <c r="C42" t="s">
         <v>81</v>
       </c>
-    </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E42" t="s">
+        <v>572</v>
+      </c>
+      <c r="F42" t="s">
+        <v>664</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>82</v>
       </c>
@@ -2434,8 +3240,14 @@
       <c r="C43" t="s">
         <v>83</v>
       </c>
-    </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E43" t="s">
+        <v>573</v>
+      </c>
+      <c r="F43" t="s">
+        <v>665</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>84</v>
       </c>
@@ -2445,8 +3257,14 @@
       <c r="C44" t="s">
         <v>85</v>
       </c>
-    </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E44" t="s">
+        <v>574</v>
+      </c>
+      <c r="F44" t="s">
+        <v>666</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>86</v>
       </c>
@@ -2456,8 +3274,14 @@
       <c r="C45" t="s">
         <v>87</v>
       </c>
-    </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E45" t="s">
+        <v>575</v>
+      </c>
+      <c r="F45" t="s">
+        <v>667</v>
+      </c>
+    </row>
+    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>88</v>
       </c>
@@ -2470,8 +3294,14 @@
       <c r="D46">
         <v>1</v>
       </c>
-    </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E46" t="s">
+        <v>576</v>
+      </c>
+      <c r="F46" t="s">
+        <v>668</v>
+      </c>
+    </row>
+    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>90</v>
       </c>
@@ -2481,8 +3311,14 @@
       <c r="C47" t="s">
         <v>91</v>
       </c>
-    </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E47" t="s">
+        <v>577</v>
+      </c>
+      <c r="F47" t="s">
+        <v>669</v>
+      </c>
+    </row>
+    <row r="48" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>92</v>
       </c>
@@ -3036,7 +3872,7 @@
         <v>189</v>
       </c>
     </row>
-    <row r="97" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
         <v>190</v>
       </c>
@@ -3050,7 +3886,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="98" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
         <v>192</v>
       </c>
@@ -3064,7 +3900,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="99" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
         <v>194</v>
       </c>
@@ -3078,7 +3914,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="100" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
         <v>196</v>
       </c>
@@ -3092,7 +3928,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="101" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
         <v>198</v>
       </c>
@@ -3106,7 +3942,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="102" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
         <v>200</v>
       </c>
@@ -3120,7 +3956,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="103" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
         <v>202</v>
       </c>
@@ -3131,7 +3967,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="104" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
         <v>204</v>
       </c>
@@ -3142,7 +3978,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="105" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
         <v>206</v>
       </c>
@@ -3153,7 +3989,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="106" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
         <v>208</v>
       </c>
@@ -3164,7 +4000,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="107" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A107" t="s">
         <v>210</v>
       </c>
@@ -3175,7 +4011,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="108" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A108" t="s">
         <v>212</v>
       </c>
@@ -3186,7 +4022,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="109" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A109" t="s">
         <v>214</v>
       </c>
@@ -3196,8 +4032,14 @@
       <c r="C109" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="110" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E109" t="s">
+        <v>578</v>
+      </c>
+      <c r="F109" t="s">
+        <v>670</v>
+      </c>
+    </row>
+    <row r="110" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A110" t="s">
         <v>215</v>
       </c>
@@ -3207,8 +4049,14 @@
       <c r="C110" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="111" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E110" t="s">
+        <v>579</v>
+      </c>
+      <c r="F110" t="s">
+        <v>671</v>
+      </c>
+    </row>
+    <row r="111" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A111" t="s">
         <v>216</v>
       </c>
@@ -3218,8 +4066,14 @@
       <c r="C111" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="112" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E111" t="s">
+        <v>580</v>
+      </c>
+      <c r="F111" t="s">
+        <v>672</v>
+      </c>
+    </row>
+    <row r="112" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A112" t="s">
         <v>217</v>
       </c>
@@ -3229,8 +4083,14 @@
       <c r="C112" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="113" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E112" t="s">
+        <v>581</v>
+      </c>
+      <c r="F112" t="s">
+        <v>673</v>
+      </c>
+    </row>
+    <row r="113" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A113" t="s">
         <v>218</v>
       </c>
@@ -3240,8 +4100,14 @@
       <c r="C113" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="114" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E113" t="s">
+        <v>582</v>
+      </c>
+      <c r="F113" t="s">
+        <v>674</v>
+      </c>
+    </row>
+    <row r="114" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A114" t="s">
         <v>219</v>
       </c>
@@ -3251,8 +4117,14 @@
       <c r="C114" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="115" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E114" t="s">
+        <v>583</v>
+      </c>
+      <c r="F114" t="s">
+        <v>675</v>
+      </c>
+    </row>
+    <row r="115" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A115" t="s">
         <v>220</v>
       </c>
@@ -3262,8 +4134,14 @@
       <c r="C115" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="116" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E115" t="s">
+        <v>584</v>
+      </c>
+      <c r="F115" t="s">
+        <v>676</v>
+      </c>
+    </row>
+    <row r="116" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A116" t="s">
         <v>221</v>
       </c>
@@ -3273,8 +4151,14 @@
       <c r="C116" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="117" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E116" t="s">
+        <v>585</v>
+      </c>
+      <c r="F116" t="s">
+        <v>677</v>
+      </c>
+    </row>
+    <row r="117" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A117" t="s">
         <v>222</v>
       </c>
@@ -3284,8 +4168,14 @@
       <c r="C117" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="118" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E117" t="s">
+        <v>586</v>
+      </c>
+      <c r="F117" t="s">
+        <v>678</v>
+      </c>
+    </row>
+    <row r="118" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A118" t="s">
         <v>223</v>
       </c>
@@ -3295,8 +4185,14 @@
       <c r="C118" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="119" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E118" t="s">
+        <v>587</v>
+      </c>
+      <c r="F118" t="s">
+        <v>679</v>
+      </c>
+    </row>
+    <row r="119" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A119" t="s">
         <v>224</v>
       </c>
@@ -3306,8 +4202,14 @@
       <c r="C119" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="120" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E119" t="s">
+        <v>589</v>
+      </c>
+      <c r="F119" t="s">
+        <v>680</v>
+      </c>
+    </row>
+    <row r="120" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A120" t="s">
         <v>225</v>
       </c>
@@ -3317,8 +4219,14 @@
       <c r="C120" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="121" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E120" t="s">
+        <v>590</v>
+      </c>
+      <c r="F120" t="s">
+        <v>681</v>
+      </c>
+    </row>
+    <row r="121" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A121" t="s">
         <v>226</v>
       </c>
@@ -3328,8 +4236,14 @@
       <c r="C121" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="122" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E121" t="s">
+        <v>591</v>
+      </c>
+      <c r="F121" t="s">
+        <v>682</v>
+      </c>
+    </row>
+    <row r="122" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A122" t="s">
         <v>227</v>
       </c>
@@ -3339,8 +4253,14 @@
       <c r="C122" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="123" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E122" t="s">
+        <v>592</v>
+      </c>
+      <c r="F122" t="s">
+        <v>683</v>
+      </c>
+    </row>
+    <row r="123" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A123" t="s">
         <v>228</v>
       </c>
@@ -3350,8 +4270,14 @@
       <c r="C123" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="124" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E123" t="s">
+        <v>593</v>
+      </c>
+      <c r="F123" t="s">
+        <v>684</v>
+      </c>
+    </row>
+    <row r="124" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A124" t="s">
         <v>229</v>
       </c>
@@ -3361,8 +4287,14 @@
       <c r="C124" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="125" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E124" t="s">
+        <v>594</v>
+      </c>
+      <c r="F124" t="s">
+        <v>685</v>
+      </c>
+    </row>
+    <row r="125" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A125" t="s">
         <v>230</v>
       </c>
@@ -3372,8 +4304,14 @@
       <c r="C125" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="126" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E125" t="s">
+        <v>595</v>
+      </c>
+      <c r="F125" t="s">
+        <v>686</v>
+      </c>
+    </row>
+    <row r="126" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A126" t="s">
         <v>231</v>
       </c>
@@ -3383,8 +4321,14 @@
       <c r="C126" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="127" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E126" t="s">
+        <v>596</v>
+      </c>
+      <c r="F126" t="s">
+        <v>687</v>
+      </c>
+    </row>
+    <row r="127" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A127" t="s">
         <v>232</v>
       </c>
@@ -3394,8 +4338,14 @@
       <c r="C127" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="128" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E127" t="s">
+        <v>597</v>
+      </c>
+      <c r="F127" t="s">
+        <v>688</v>
+      </c>
+    </row>
+    <row r="128" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A128" t="s">
         <v>233</v>
       </c>
@@ -3405,8 +4355,14 @@
       <c r="C128" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="129" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E128" t="s">
+        <v>598</v>
+      </c>
+      <c r="F128" t="s">
+        <v>689</v>
+      </c>
+    </row>
+    <row r="129" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A129" t="s">
         <v>234</v>
       </c>
@@ -3416,8 +4372,14 @@
       <c r="C129" t="s">
         <v>41</v>
       </c>
-    </row>
-    <row r="130" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E129" t="s">
+        <v>599</v>
+      </c>
+      <c r="F129" t="s">
+        <v>690</v>
+      </c>
+    </row>
+    <row r="130" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A130" t="s">
         <v>235</v>
       </c>
@@ -3427,8 +4389,14 @@
       <c r="C130" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="131" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E130" t="s">
+        <v>600</v>
+      </c>
+      <c r="F130" t="s">
+        <v>691</v>
+      </c>
+    </row>
+    <row r="131" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A131" t="s">
         <v>236</v>
       </c>
@@ -3438,8 +4406,14 @@
       <c r="C131" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="132" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E131" t="s">
+        <v>601</v>
+      </c>
+      <c r="F131" t="s">
+        <v>692</v>
+      </c>
+    </row>
+    <row r="132" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A132" t="s">
         <v>237</v>
       </c>
@@ -3449,8 +4423,14 @@
       <c r="C132" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="133" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E132" t="s">
+        <v>602</v>
+      </c>
+      <c r="F132" t="s">
+        <v>693</v>
+      </c>
+    </row>
+    <row r="133" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A133" t="s">
         <v>238</v>
       </c>
@@ -3460,8 +4440,14 @@
       <c r="C133" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="134" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E133" t="s">
+        <v>603</v>
+      </c>
+      <c r="F133" t="s">
+        <v>694</v>
+      </c>
+    </row>
+    <row r="134" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A134" t="s">
         <v>239</v>
       </c>
@@ -3471,8 +4457,14 @@
       <c r="C134" t="s">
         <v>51</v>
       </c>
-    </row>
-    <row r="135" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E134" t="s">
+        <v>604</v>
+      </c>
+      <c r="F134" t="s">
+        <v>695</v>
+      </c>
+    </row>
+    <row r="135" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A135" t="s">
         <v>240</v>
       </c>
@@ -3482,8 +4474,14 @@
       <c r="C135" t="s">
         <v>53</v>
       </c>
-    </row>
-    <row r="136" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E135" t="s">
+        <v>605</v>
+      </c>
+      <c r="F135" t="s">
+        <v>696</v>
+      </c>
+    </row>
+    <row r="136" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A136" t="s">
         <v>241</v>
       </c>
@@ -3493,8 +4491,14 @@
       <c r="C136" t="s">
         <v>55</v>
       </c>
-    </row>
-    <row r="137" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E136" t="s">
+        <v>606</v>
+      </c>
+      <c r="F136" t="s">
+        <v>697</v>
+      </c>
+    </row>
+    <row r="137" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A137" t="s">
         <v>242</v>
       </c>
@@ -3504,8 +4508,14 @@
       <c r="C137" t="s">
         <v>57</v>
       </c>
-    </row>
-    <row r="138" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E137" t="s">
+        <v>607</v>
+      </c>
+      <c r="F137" t="s">
+        <v>698</v>
+      </c>
+    </row>
+    <row r="138" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A138" t="s">
         <v>243</v>
       </c>
@@ -3515,8 +4525,14 @@
       <c r="C138" t="s">
         <v>59</v>
       </c>
-    </row>
-    <row r="139" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E138" t="s">
+        <v>608</v>
+      </c>
+      <c r="F138" t="s">
+        <v>699</v>
+      </c>
+    </row>
+    <row r="139" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A139" t="s">
         <v>244</v>
       </c>
@@ -3526,8 +4542,14 @@
       <c r="C139" t="s">
         <v>61</v>
       </c>
-    </row>
-    <row r="140" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E139" t="s">
+        <v>609</v>
+      </c>
+      <c r="F139" t="s">
+        <v>700</v>
+      </c>
+    </row>
+    <row r="140" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A140" t="s">
         <v>245</v>
       </c>
@@ -3537,8 +4559,14 @@
       <c r="C140" t="s">
         <v>63</v>
       </c>
-    </row>
-    <row r="141" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E140" t="s">
+        <v>610</v>
+      </c>
+      <c r="F140" t="s">
+        <v>701</v>
+      </c>
+    </row>
+    <row r="141" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A141" t="s">
         <v>246</v>
       </c>
@@ -3548,8 +4576,14 @@
       <c r="C141" t="s">
         <v>65</v>
       </c>
-    </row>
-    <row r="142" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E141" t="s">
+        <v>611</v>
+      </c>
+      <c r="F141" t="s">
+        <v>702</v>
+      </c>
+    </row>
+    <row r="142" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A142" t="s">
         <v>247</v>
       </c>
@@ -3559,8 +4593,14 @@
       <c r="C142" t="s">
         <v>67</v>
       </c>
-    </row>
-    <row r="143" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E142" t="s">
+        <v>612</v>
+      </c>
+      <c r="F142" t="s">
+        <v>703</v>
+      </c>
+    </row>
+    <row r="143" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A143" t="s">
         <v>248</v>
       </c>
@@ -3570,8 +4610,14 @@
       <c r="C143" t="s">
         <v>69</v>
       </c>
-    </row>
-    <row r="144" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E143" t="s">
+        <v>613</v>
+      </c>
+      <c r="F143" t="s">
+        <v>704</v>
+      </c>
+    </row>
+    <row r="144" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A144" t="s">
         <v>249</v>
       </c>
@@ -3581,8 +4627,14 @@
       <c r="C144" t="s">
         <v>71</v>
       </c>
-    </row>
-    <row r="145" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E144" t="s">
+        <v>614</v>
+      </c>
+      <c r="F144" t="s">
+        <v>705</v>
+      </c>
+    </row>
+    <row r="145" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A145" t="s">
         <v>250</v>
       </c>
@@ -3592,8 +4644,14 @@
       <c r="C145" t="s">
         <v>73</v>
       </c>
-    </row>
-    <row r="146" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E145" t="s">
+        <v>615</v>
+      </c>
+      <c r="F145" t="s">
+        <v>706</v>
+      </c>
+    </row>
+    <row r="146" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A146" t="s">
         <v>251</v>
       </c>
@@ -3603,8 +4661,14 @@
       <c r="C146" t="s">
         <v>75</v>
       </c>
-    </row>
-    <row r="147" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E146" t="s">
+        <v>616</v>
+      </c>
+      <c r="F146" t="s">
+        <v>707</v>
+      </c>
+    </row>
+    <row r="147" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A147" t="s">
         <v>252</v>
       </c>
@@ -3614,8 +4678,14 @@
       <c r="C147" t="s">
         <v>77</v>
       </c>
-    </row>
-    <row r="148" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E147" t="s">
+        <v>617</v>
+      </c>
+      <c r="F147" t="s">
+        <v>708</v>
+      </c>
+    </row>
+    <row r="148" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A148" t="s">
         <v>253</v>
       </c>
@@ -3625,8 +4695,14 @@
       <c r="C148" t="s">
         <v>79</v>
       </c>
-    </row>
-    <row r="149" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E148" t="s">
+        <v>618</v>
+      </c>
+      <c r="F148" t="s">
+        <v>709</v>
+      </c>
+    </row>
+    <row r="149" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A149" t="s">
         <v>254</v>
       </c>
@@ -3636,8 +4712,14 @@
       <c r="C149" t="s">
         <v>81</v>
       </c>
-    </row>
-    <row r="150" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E149" t="s">
+        <v>619</v>
+      </c>
+      <c r="F149" t="s">
+        <v>710</v>
+      </c>
+    </row>
+    <row r="150" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A150" t="s">
         <v>255</v>
       </c>
@@ -3647,8 +4729,14 @@
       <c r="C150" t="s">
         <v>83</v>
       </c>
-    </row>
-    <row r="151" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E150" t="s">
+        <v>620</v>
+      </c>
+      <c r="F150" t="s">
+        <v>711</v>
+      </c>
+    </row>
+    <row r="151" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A151" t="s">
         <v>256</v>
       </c>
@@ -3658,8 +4746,14 @@
       <c r="C151" t="s">
         <v>85</v>
       </c>
-    </row>
-    <row r="152" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E151" t="s">
+        <v>621</v>
+      </c>
+      <c r="F151" t="s">
+        <v>712</v>
+      </c>
+    </row>
+    <row r="152" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A152" t="s">
         <v>257</v>
       </c>
@@ -3669,8 +4763,14 @@
       <c r="C152" t="s">
         <v>87</v>
       </c>
-    </row>
-    <row r="153" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E152" t="s">
+        <v>622</v>
+      </c>
+      <c r="F152" t="s">
+        <v>713</v>
+      </c>
+    </row>
+    <row r="153" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A153" t="s">
         <v>258</v>
       </c>
@@ -3684,7 +4784,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="154" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="154" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A154" t="s">
         <v>259</v>
       </c>
@@ -3694,8 +4794,14 @@
       <c r="C154" t="s">
         <v>91</v>
       </c>
-    </row>
-    <row r="155" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E154" t="s">
+        <v>623</v>
+      </c>
+      <c r="F154" t="s">
+        <v>714</v>
+      </c>
+    </row>
+    <row r="155" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A155" t="s">
         <v>260</v>
       </c>
@@ -3706,7 +4812,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="156" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="156" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A156" t="s">
         <v>261</v>
       </c>
@@ -3717,7 +4823,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="157" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="157" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A157" t="s">
         <v>262</v>
       </c>
@@ -3728,7 +4834,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="158" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="158" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A158" t="s">
         <v>263</v>
       </c>
@@ -3739,7 +4845,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="159" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="159" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A159" t="s">
         <v>264</v>
       </c>
@@ -3750,7 +4856,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="160" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="160" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A160" t="s">
         <v>265</v>
       </c>

</xml_diff>

<commit_message>
Tagged with the appropriate syllabary series
</commit_message>
<xml_diff>
--- a/read-and-write-kana/Note Types/Read & Write Kana/Read & Write Kana - Data Sheet.xlsx
+++ b/read-and-write-kana/Note Types/Read & Write Kana/Read & Write Kana - Data Sheet.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1185" uniqueCount="729">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1185" uniqueCount="771">
   <si>
     <t>あ</t>
   </si>
@@ -2164,43 +2164,169 @@
     <t>Tags</t>
   </si>
   <si>
-    <t>hiragana dakuon</t>
-  </si>
-  <si>
-    <t>hiragana dakuon handakuon</t>
-  </si>
-  <si>
-    <t>hiragana yoon</t>
-  </si>
-  <si>
-    <t>hiragana yoon_dakuon</t>
-  </si>
-  <si>
-    <t>hiragana yoon_dakuon yoon_handakuon</t>
-  </si>
-  <si>
-    <t>hiragana gojuon seion</t>
-  </si>
-  <si>
-    <t>katakana gojuon seion</t>
-  </si>
-  <si>
-    <t>katakana dakuon</t>
-  </si>
-  <si>
-    <t>katakana dakuon handakuon</t>
-  </si>
-  <si>
-    <t>katakana yoon</t>
-  </si>
-  <si>
-    <t>katakana yoon_dakuon</t>
-  </si>
-  <si>
-    <t>katakana yoon_dakuon yoon_handakuon</t>
-  </si>
-  <si>
     <t>katakana special foreign</t>
+  </si>
+  <si>
+    <t>hiragana gojuon seion a_series</t>
+  </si>
+  <si>
+    <t>hiragana gojuon seion k_series</t>
+  </si>
+  <si>
+    <t>hiragana gojuon seion s_series</t>
+  </si>
+  <si>
+    <t>hiragana gojuon seion t_series</t>
+  </si>
+  <si>
+    <t>hiragana gojuon seion n_series</t>
+  </si>
+  <si>
+    <t>hiragana gojuon seion h_series</t>
+  </si>
+  <si>
+    <t>hiragana gojuon seion m_series</t>
+  </si>
+  <si>
+    <t>hiragana gojuon seion y_series</t>
+  </si>
+  <si>
+    <t>hiragana gojuon seion r_series</t>
+  </si>
+  <si>
+    <t>hiragana gojuon seion w_series</t>
+  </si>
+  <si>
+    <t>hiragana dakuon k_series g_series</t>
+  </si>
+  <si>
+    <t>hiragana dakuon s_series z_series</t>
+  </si>
+  <si>
+    <t>hiragana dakuon t_series d_series</t>
+  </si>
+  <si>
+    <t>hiragana dakuon h_series b_series</t>
+  </si>
+  <si>
+    <t>hiragana yoon t_series ch_series</t>
+  </si>
+  <si>
+    <t>hiragana yoon k_series ky_series</t>
+  </si>
+  <si>
+    <t>hiragana yoon s_series sh_series</t>
+  </si>
+  <si>
+    <t>hiragana yoon n_series ny_series</t>
+  </si>
+  <si>
+    <t>hiragana yoon h_series hy_series</t>
+  </si>
+  <si>
+    <t>hiragana yoon m_series my_series</t>
+  </si>
+  <si>
+    <t>hiragana yoon r_series ry_series</t>
+  </si>
+  <si>
+    <t>hiragana yoon_dakuon k_series ky_series g_series gy_series</t>
+  </si>
+  <si>
+    <t>hiragana yoon_dakuon s_series sh_series j_series</t>
+  </si>
+  <si>
+    <t>hiragana yoon_dakuon t_series ch_series j_series</t>
+  </si>
+  <si>
+    <t>hiragana dakuon handakuon h_series p_series</t>
+  </si>
+  <si>
+    <t>hiragana yoon_dakuon h_series hy_series b_series by_series</t>
+  </si>
+  <si>
+    <t>hiragana yoon_dakuon yoon_handakuon h_series hy_series p_series py_series</t>
+  </si>
+  <si>
+    <t>katakana gojuon seion a_series</t>
+  </si>
+  <si>
+    <t>katakana gojuon seion k_series</t>
+  </si>
+  <si>
+    <t>katakana gojuon seion s_series</t>
+  </si>
+  <si>
+    <t>katakana gojuon seion t_series</t>
+  </si>
+  <si>
+    <t>katakana gojuon seion n_series</t>
+  </si>
+  <si>
+    <t>katakana gojuon seion h_series</t>
+  </si>
+  <si>
+    <t>katakana gojuon seion m_series</t>
+  </si>
+  <si>
+    <t>katakana gojuon seion y_series</t>
+  </si>
+  <si>
+    <t>katakana gojuon seion r_series</t>
+  </si>
+  <si>
+    <t>katakana gojuon seion w_series</t>
+  </si>
+  <si>
+    <t>katakana dakuon k_series g_series</t>
+  </si>
+  <si>
+    <t>katakana dakuon s_series z_series</t>
+  </si>
+  <si>
+    <t>katakana dakuon t_series d_series</t>
+  </si>
+  <si>
+    <t>katakana dakuon h_series b_series</t>
+  </si>
+  <si>
+    <t>katakana dakuon handakuon h_series p_series</t>
+  </si>
+  <si>
+    <t>katakana yoon k_series ky_series</t>
+  </si>
+  <si>
+    <t>katakana yoon s_series sh_series</t>
+  </si>
+  <si>
+    <t>katakana yoon t_series ch_series</t>
+  </si>
+  <si>
+    <t>katakana yoon n_series ny_series</t>
+  </si>
+  <si>
+    <t>katakana yoon h_series hy_series</t>
+  </si>
+  <si>
+    <t>katakana yoon m_series my_series</t>
+  </si>
+  <si>
+    <t>katakana yoon r_series ry_series</t>
+  </si>
+  <si>
+    <t>katakana yoon_dakuon k_series ky_series g_series gy_series</t>
+  </si>
+  <si>
+    <t>katakana yoon_dakuon s_series sh_series j_series</t>
+  </si>
+  <si>
+    <t>katakana yoon_dakuon t_series ch_series j_series</t>
+  </si>
+  <si>
+    <t>katakana yoon_dakuon h_series hy_series b_series by_series</t>
+  </si>
+  <si>
+    <t>katakana yoon_dakuon yoon_handakuon h_series hy_series p_series py_series</t>
   </si>
 </sst>
 </file>
@@ -2553,7 +2679,7 @@
     <col min="4" max="4" width="22.42578125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="35.140625" customWidth="1"/>
     <col min="6" max="6" width="58.85546875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="37.5703125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="72.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
@@ -2596,7 +2722,7 @@
         <v>624</v>
       </c>
       <c r="G2" t="s">
-        <v>721</v>
+        <v>717</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
@@ -2616,7 +2742,7 @@
         <v>625</v>
       </c>
       <c r="G3" t="s">
-        <v>721</v>
+        <v>717</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
@@ -2636,7 +2762,7 @@
         <v>626</v>
       </c>
       <c r="G4" t="s">
-        <v>721</v>
+        <v>717</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
@@ -2656,7 +2782,7 @@
         <v>627</v>
       </c>
       <c r="G5" t="s">
-        <v>721</v>
+        <v>717</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
@@ -2676,7 +2802,7 @@
         <v>628</v>
       </c>
       <c r="G6" t="s">
-        <v>721</v>
+        <v>717</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
@@ -2696,7 +2822,7 @@
         <v>629</v>
       </c>
       <c r="G7" t="s">
-        <v>721</v>
+        <v>718</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
@@ -2716,7 +2842,7 @@
         <v>630</v>
       </c>
       <c r="G8" t="s">
-        <v>721</v>
+        <v>718</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
@@ -2736,7 +2862,7 @@
         <v>631</v>
       </c>
       <c r="G9" t="s">
-        <v>721</v>
+        <v>718</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
@@ -2756,7 +2882,7 @@
         <v>632</v>
       </c>
       <c r="G10" t="s">
-        <v>721</v>
+        <v>718</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
@@ -2776,7 +2902,7 @@
         <v>633</v>
       </c>
       <c r="G11" t="s">
-        <v>721</v>
+        <v>718</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
@@ -2796,7 +2922,7 @@
         <v>634</v>
       </c>
       <c r="G12" t="s">
-        <v>721</v>
+        <v>719</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
@@ -2816,7 +2942,7 @@
         <v>635</v>
       </c>
       <c r="G13" t="s">
-        <v>721</v>
+        <v>719</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
@@ -2836,7 +2962,7 @@
         <v>636</v>
       </c>
       <c r="G14" t="s">
-        <v>721</v>
+        <v>719</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
@@ -2856,7 +2982,7 @@
         <v>637</v>
       </c>
       <c r="G15" t="s">
-        <v>721</v>
+        <v>719</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
@@ -2876,7 +3002,7 @@
         <v>638</v>
       </c>
       <c r="G16" t="s">
-        <v>721</v>
+        <v>719</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
@@ -2896,7 +3022,7 @@
         <v>639</v>
       </c>
       <c r="G17" t="s">
-        <v>721</v>
+        <v>720</v>
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
@@ -2916,7 +3042,7 @@
         <v>640</v>
       </c>
       <c r="G18" t="s">
-        <v>721</v>
+        <v>720</v>
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.25">
@@ -2936,7 +3062,7 @@
         <v>641</v>
       </c>
       <c r="G19" t="s">
-        <v>721</v>
+        <v>720</v>
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.25">
@@ -2956,7 +3082,7 @@
         <v>642</v>
       </c>
       <c r="G20" t="s">
-        <v>721</v>
+        <v>720</v>
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.25">
@@ -2976,7 +3102,7 @@
         <v>643</v>
       </c>
       <c r="G21" t="s">
-        <v>721</v>
+        <v>720</v>
       </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.25">
@@ -3096,7 +3222,7 @@
         <v>649</v>
       </c>
       <c r="G27" t="s">
-        <v>721</v>
+        <v>722</v>
       </c>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.25">
@@ -3116,7 +3242,7 @@
         <v>650</v>
       </c>
       <c r="G28" t="s">
-        <v>721</v>
+        <v>722</v>
       </c>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.25">
@@ -3136,7 +3262,7 @@
         <v>651</v>
       </c>
       <c r="G29" t="s">
-        <v>721</v>
+        <v>722</v>
       </c>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.25">
@@ -3156,7 +3282,7 @@
         <v>652</v>
       </c>
       <c r="G30" t="s">
-        <v>721</v>
+        <v>722</v>
       </c>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.25">
@@ -3176,7 +3302,7 @@
         <v>653</v>
       </c>
       <c r="G31" t="s">
-        <v>721</v>
+        <v>722</v>
       </c>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.25">
@@ -3196,7 +3322,7 @@
         <v>654</v>
       </c>
       <c r="G32" t="s">
-        <v>721</v>
+        <v>723</v>
       </c>
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.25">
@@ -3216,7 +3342,7 @@
         <v>655</v>
       </c>
       <c r="G33" t="s">
-        <v>721</v>
+        <v>723</v>
       </c>
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.25">
@@ -3236,7 +3362,7 @@
         <v>656</v>
       </c>
       <c r="G34" t="s">
-        <v>721</v>
+        <v>723</v>
       </c>
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.25">
@@ -3256,7 +3382,7 @@
         <v>657</v>
       </c>
       <c r="G35" t="s">
-        <v>721</v>
+        <v>723</v>
       </c>
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.25">
@@ -3276,7 +3402,7 @@
         <v>658</v>
       </c>
       <c r="G36" t="s">
-        <v>721</v>
+        <v>723</v>
       </c>
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.25">
@@ -3296,7 +3422,7 @@
         <v>659</v>
       </c>
       <c r="G37" t="s">
-        <v>721</v>
+        <v>724</v>
       </c>
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.25">
@@ -3316,7 +3442,7 @@
         <v>660</v>
       </c>
       <c r="G38" t="s">
-        <v>721</v>
+        <v>724</v>
       </c>
     </row>
     <row r="39" spans="1:7" x14ac:dyDescent="0.25">
@@ -3336,7 +3462,7 @@
         <v>661</v>
       </c>
       <c r="G39" t="s">
-        <v>721</v>
+        <v>724</v>
       </c>
     </row>
     <row r="40" spans="1:7" x14ac:dyDescent="0.25">
@@ -3356,7 +3482,7 @@
         <v>662</v>
       </c>
       <c r="G40" t="s">
-        <v>721</v>
+        <v>725</v>
       </c>
     </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.25">
@@ -3376,7 +3502,7 @@
         <v>663</v>
       </c>
       <c r="G41" t="s">
-        <v>721</v>
+        <v>725</v>
       </c>
     </row>
     <row r="42" spans="1:7" x14ac:dyDescent="0.25">
@@ -3396,7 +3522,7 @@
         <v>664</v>
       </c>
       <c r="G42" t="s">
-        <v>721</v>
+        <v>725</v>
       </c>
     </row>
     <row r="43" spans="1:7" x14ac:dyDescent="0.25">
@@ -3416,7 +3542,7 @@
         <v>665</v>
       </c>
       <c r="G43" t="s">
-        <v>721</v>
+        <v>725</v>
       </c>
     </row>
     <row r="44" spans="1:7" x14ac:dyDescent="0.25">
@@ -3436,7 +3562,7 @@
         <v>666</v>
       </c>
       <c r="G44" t="s">
-        <v>721</v>
+        <v>725</v>
       </c>
     </row>
     <row r="45" spans="1:7" x14ac:dyDescent="0.25">
@@ -3456,7 +3582,7 @@
         <v>667</v>
       </c>
       <c r="G45" t="s">
-        <v>721</v>
+        <v>726</v>
       </c>
     </row>
     <row r="46" spans="1:7" x14ac:dyDescent="0.25">
@@ -3479,7 +3605,7 @@
         <v>668</v>
       </c>
       <c r="G46" t="s">
-        <v>721</v>
+        <v>726</v>
       </c>
     </row>
     <row r="47" spans="1:7" x14ac:dyDescent="0.25">
@@ -3499,7 +3625,7 @@
         <v>669</v>
       </c>
       <c r="G47" t="s">
-        <v>721</v>
+        <v>726</v>
       </c>
     </row>
     <row r="48" spans="1:7" x14ac:dyDescent="0.25">
@@ -3513,7 +3639,7 @@
         <v>93</v>
       </c>
       <c r="G48" t="s">
-        <v>716</v>
+        <v>727</v>
       </c>
     </row>
     <row r="49" spans="1:7" x14ac:dyDescent="0.25">
@@ -3527,7 +3653,7 @@
         <v>95</v>
       </c>
       <c r="G49" t="s">
-        <v>716</v>
+        <v>727</v>
       </c>
     </row>
     <row r="50" spans="1:7" x14ac:dyDescent="0.25">
@@ -3541,7 +3667,7 @@
         <v>97</v>
       </c>
       <c r="G50" t="s">
-        <v>716</v>
+        <v>727</v>
       </c>
     </row>
     <row r="51" spans="1:7" x14ac:dyDescent="0.25">
@@ -3555,7 +3681,7 @@
         <v>99</v>
       </c>
       <c r="G51" t="s">
-        <v>716</v>
+        <v>727</v>
       </c>
     </row>
     <row r="52" spans="1:7" x14ac:dyDescent="0.25">
@@ -3569,7 +3695,7 @@
         <v>101</v>
       </c>
       <c r="G52" t="s">
-        <v>716</v>
+        <v>727</v>
       </c>
     </row>
     <row r="53" spans="1:7" x14ac:dyDescent="0.25">
@@ -3583,7 +3709,7 @@
         <v>103</v>
       </c>
       <c r="G53" t="s">
-        <v>716</v>
+        <v>728</v>
       </c>
     </row>
     <row r="54" spans="1:7" x14ac:dyDescent="0.25">
@@ -3600,7 +3726,7 @@
         <v>1</v>
       </c>
       <c r="G54" t="s">
-        <v>716</v>
+        <v>728</v>
       </c>
     </row>
     <row r="55" spans="1:7" x14ac:dyDescent="0.25">
@@ -3617,7 +3743,7 @@
         <v>1</v>
       </c>
       <c r="G55" t="s">
-        <v>716</v>
+        <v>728</v>
       </c>
     </row>
     <row r="56" spans="1:7" x14ac:dyDescent="0.25">
@@ -3631,7 +3757,7 @@
         <v>109</v>
       </c>
       <c r="G56" t="s">
-        <v>716</v>
+        <v>728</v>
       </c>
     </row>
     <row r="57" spans="1:7" x14ac:dyDescent="0.25">
@@ -3645,7 +3771,7 @@
         <v>111</v>
       </c>
       <c r="G57" t="s">
-        <v>716</v>
+        <v>728</v>
       </c>
     </row>
     <row r="58" spans="1:7" x14ac:dyDescent="0.25">
@@ -3659,7 +3785,7 @@
         <v>113</v>
       </c>
       <c r="G58" t="s">
-        <v>716</v>
+        <v>729</v>
       </c>
     </row>
     <row r="59" spans="1:7" x14ac:dyDescent="0.25">
@@ -3676,7 +3802,7 @@
         <v>1</v>
       </c>
       <c r="G59" t="s">
-        <v>716</v>
+        <v>729</v>
       </c>
     </row>
     <row r="60" spans="1:7" x14ac:dyDescent="0.25">
@@ -3693,7 +3819,7 @@
         <v>1</v>
       </c>
       <c r="G60" t="s">
-        <v>716</v>
+        <v>729</v>
       </c>
     </row>
     <row r="61" spans="1:7" x14ac:dyDescent="0.25">
@@ -3707,7 +3833,7 @@
         <v>119</v>
       </c>
       <c r="G61" t="s">
-        <v>716</v>
+        <v>729</v>
       </c>
     </row>
     <row r="62" spans="1:7" x14ac:dyDescent="0.25">
@@ -3721,7 +3847,7 @@
         <v>121</v>
       </c>
       <c r="G62" t="s">
-        <v>716</v>
+        <v>729</v>
       </c>
     </row>
     <row r="63" spans="1:7" x14ac:dyDescent="0.25">
@@ -3735,7 +3861,7 @@
         <v>123</v>
       </c>
       <c r="G63" t="s">
-        <v>716</v>
+        <v>730</v>
       </c>
     </row>
     <row r="64" spans="1:7" x14ac:dyDescent="0.25">
@@ -3749,7 +3875,7 @@
         <v>125</v>
       </c>
       <c r="G64" t="s">
-        <v>716</v>
+        <v>730</v>
       </c>
     </row>
     <row r="65" spans="1:7" x14ac:dyDescent="0.25">
@@ -3763,7 +3889,7 @@
         <v>127</v>
       </c>
       <c r="G65" t="s">
-        <v>716</v>
+        <v>730</v>
       </c>
     </row>
     <row r="66" spans="1:7" x14ac:dyDescent="0.25">
@@ -3777,7 +3903,7 @@
         <v>129</v>
       </c>
       <c r="G66" t="s">
-        <v>716</v>
+        <v>730</v>
       </c>
     </row>
     <row r="67" spans="1:7" x14ac:dyDescent="0.25">
@@ -3791,7 +3917,7 @@
         <v>131</v>
       </c>
       <c r="G67" t="s">
-        <v>716</v>
+        <v>730</v>
       </c>
     </row>
     <row r="68" spans="1:7" x14ac:dyDescent="0.25">
@@ -3805,7 +3931,7 @@
         <v>133</v>
       </c>
       <c r="G68" t="s">
-        <v>717</v>
+        <v>741</v>
       </c>
     </row>
     <row r="69" spans="1:7" x14ac:dyDescent="0.25">
@@ -3819,7 +3945,7 @@
         <v>135</v>
       </c>
       <c r="G69" t="s">
-        <v>717</v>
+        <v>741</v>
       </c>
     </row>
     <row r="70" spans="1:7" x14ac:dyDescent="0.25">
@@ -3833,7 +3959,7 @@
         <v>137</v>
       </c>
       <c r="G70" t="s">
-        <v>717</v>
+        <v>741</v>
       </c>
     </row>
     <row r="71" spans="1:7" x14ac:dyDescent="0.25">
@@ -3847,7 +3973,7 @@
         <v>139</v>
       </c>
       <c r="G71" t="s">
-        <v>717</v>
+        <v>741</v>
       </c>
     </row>
     <row r="72" spans="1:7" x14ac:dyDescent="0.25">
@@ -3861,7 +3987,7 @@
         <v>141</v>
       </c>
       <c r="G72" t="s">
-        <v>717</v>
+        <v>741</v>
       </c>
     </row>
     <row r="73" spans="1:7" x14ac:dyDescent="0.25">
@@ -3875,7 +4001,7 @@
         <v>143</v>
       </c>
       <c r="G73" t="s">
-        <v>718</v>
+        <v>732</v>
       </c>
     </row>
     <row r="74" spans="1:7" x14ac:dyDescent="0.25">
@@ -3889,7 +4015,7 @@
         <v>145</v>
       </c>
       <c r="G74" t="s">
-        <v>718</v>
+        <v>732</v>
       </c>
     </row>
     <row r="75" spans="1:7" x14ac:dyDescent="0.25">
@@ -3903,7 +4029,7 @@
         <v>147</v>
       </c>
       <c r="G75" t="s">
-        <v>718</v>
+        <v>732</v>
       </c>
     </row>
     <row r="76" spans="1:7" x14ac:dyDescent="0.25">
@@ -3917,7 +4043,7 @@
         <v>149</v>
       </c>
       <c r="G76" t="s">
-        <v>718</v>
+        <v>733</v>
       </c>
     </row>
     <row r="77" spans="1:7" x14ac:dyDescent="0.25">
@@ -3931,7 +4057,7 @@
         <v>151</v>
       </c>
       <c r="G77" t="s">
-        <v>718</v>
+        <v>733</v>
       </c>
     </row>
     <row r="78" spans="1:7" x14ac:dyDescent="0.25">
@@ -3945,7 +4071,7 @@
         <v>153</v>
       </c>
       <c r="G78" t="s">
-        <v>718</v>
+        <v>733</v>
       </c>
     </row>
     <row r="79" spans="1:7" x14ac:dyDescent="0.25">
@@ -3959,7 +4085,7 @@
         <v>155</v>
       </c>
       <c r="G79" t="s">
-        <v>718</v>
+        <v>731</v>
       </c>
     </row>
     <row r="80" spans="1:7" x14ac:dyDescent="0.25">
@@ -3973,7 +4099,7 @@
         <v>157</v>
       </c>
       <c r="G80" t="s">
-        <v>718</v>
+        <v>731</v>
       </c>
     </row>
     <row r="81" spans="1:7" x14ac:dyDescent="0.25">
@@ -3987,7 +4113,7 @@
         <v>159</v>
       </c>
       <c r="G81" t="s">
-        <v>718</v>
+        <v>731</v>
       </c>
     </row>
     <row r="82" spans="1:7" x14ac:dyDescent="0.25">
@@ -4001,7 +4127,7 @@
         <v>161</v>
       </c>
       <c r="G82" t="s">
-        <v>718</v>
+        <v>734</v>
       </c>
     </row>
     <row r="83" spans="1:7" x14ac:dyDescent="0.25">
@@ -4015,7 +4141,7 @@
         <v>163</v>
       </c>
       <c r="G83" t="s">
-        <v>718</v>
+        <v>734</v>
       </c>
     </row>
     <row r="84" spans="1:7" x14ac:dyDescent="0.25">
@@ -4029,7 +4155,7 @@
         <v>165</v>
       </c>
       <c r="G84" t="s">
-        <v>718</v>
+        <v>734</v>
       </c>
     </row>
     <row r="85" spans="1:7" x14ac:dyDescent="0.25">
@@ -4043,7 +4169,7 @@
         <v>167</v>
       </c>
       <c r="G85" t="s">
-        <v>718</v>
+        <v>735</v>
       </c>
     </row>
     <row r="86" spans="1:7" x14ac:dyDescent="0.25">
@@ -4057,7 +4183,7 @@
         <v>169</v>
       </c>
       <c r="G86" t="s">
-        <v>718</v>
+        <v>735</v>
       </c>
     </row>
     <row r="87" spans="1:7" x14ac:dyDescent="0.25">
@@ -4071,7 +4197,7 @@
         <v>171</v>
       </c>
       <c r="G87" t="s">
-        <v>718</v>
+        <v>735</v>
       </c>
     </row>
     <row r="88" spans="1:7" x14ac:dyDescent="0.25">
@@ -4085,7 +4211,7 @@
         <v>173</v>
       </c>
       <c r="G88" t="s">
-        <v>718</v>
+        <v>736</v>
       </c>
     </row>
     <row r="89" spans="1:7" x14ac:dyDescent="0.25">
@@ -4099,7 +4225,7 @@
         <v>175</v>
       </c>
       <c r="G89" t="s">
-        <v>718</v>
+        <v>736</v>
       </c>
     </row>
     <row r="90" spans="1:7" x14ac:dyDescent="0.25">
@@ -4113,7 +4239,7 @@
         <v>177</v>
       </c>
       <c r="G90" t="s">
-        <v>718</v>
+        <v>736</v>
       </c>
     </row>
     <row r="91" spans="1:7" x14ac:dyDescent="0.25">
@@ -4127,7 +4253,7 @@
         <v>179</v>
       </c>
       <c r="G91" t="s">
-        <v>718</v>
+        <v>737</v>
       </c>
     </row>
     <row r="92" spans="1:7" x14ac:dyDescent="0.25">
@@ -4144,7 +4270,7 @@
         <v>1</v>
       </c>
       <c r="G92" t="s">
-        <v>718</v>
+        <v>737</v>
       </c>
     </row>
     <row r="93" spans="1:7" x14ac:dyDescent="0.25">
@@ -4158,7 +4284,7 @@
         <v>183</v>
       </c>
       <c r="G93" t="s">
-        <v>718</v>
+        <v>737</v>
       </c>
     </row>
     <row r="94" spans="1:7" x14ac:dyDescent="0.25">
@@ -4172,7 +4298,7 @@
         <v>185</v>
       </c>
       <c r="G94" t="s">
-        <v>719</v>
+        <v>738</v>
       </c>
     </row>
     <row r="95" spans="1:7" x14ac:dyDescent="0.25">
@@ -4186,7 +4312,7 @@
         <v>187</v>
       </c>
       <c r="G95" t="s">
-        <v>719</v>
+        <v>738</v>
       </c>
     </row>
     <row r="96" spans="1:7" x14ac:dyDescent="0.25">
@@ -4200,7 +4326,7 @@
         <v>189</v>
       </c>
       <c r="G96" t="s">
-        <v>719</v>
+        <v>738</v>
       </c>
     </row>
     <row r="97" spans="1:7" x14ac:dyDescent="0.25">
@@ -4217,7 +4343,7 @@
         <v>1</v>
       </c>
       <c r="G97" t="s">
-        <v>719</v>
+        <v>739</v>
       </c>
     </row>
     <row r="98" spans="1:7" x14ac:dyDescent="0.25">
@@ -4234,7 +4360,7 @@
         <v>1</v>
       </c>
       <c r="G98" t="s">
-        <v>719</v>
+        <v>739</v>
       </c>
     </row>
     <row r="99" spans="1:7" x14ac:dyDescent="0.25">
@@ -4251,7 +4377,7 @@
         <v>1</v>
       </c>
       <c r="G99" t="s">
-        <v>719</v>
+        <v>739</v>
       </c>
     </row>
     <row r="100" spans="1:7" x14ac:dyDescent="0.25">
@@ -4268,7 +4394,7 @@
         <v>1</v>
       </c>
       <c r="G100" t="s">
-        <v>719</v>
+        <v>740</v>
       </c>
     </row>
     <row r="101" spans="1:7" x14ac:dyDescent="0.25">
@@ -4285,7 +4411,7 @@
         <v>1</v>
       </c>
       <c r="G101" t="s">
-        <v>719</v>
+        <v>740</v>
       </c>
     </row>
     <row r="102" spans="1:7" x14ac:dyDescent="0.25">
@@ -4302,7 +4428,7 @@
         <v>1</v>
       </c>
       <c r="G102" t="s">
-        <v>719</v>
+        <v>740</v>
       </c>
     </row>
     <row r="103" spans="1:7" x14ac:dyDescent="0.25">
@@ -4316,7 +4442,7 @@
         <v>203</v>
       </c>
       <c r="G103" t="s">
-        <v>719</v>
+        <v>742</v>
       </c>
     </row>
     <row r="104" spans="1:7" x14ac:dyDescent="0.25">
@@ -4330,7 +4456,7 @@
         <v>205</v>
       </c>
       <c r="G104" t="s">
-        <v>719</v>
+        <v>742</v>
       </c>
     </row>
     <row r="105" spans="1:7" x14ac:dyDescent="0.25">
@@ -4344,7 +4470,7 @@
         <v>207</v>
       </c>
       <c r="G105" t="s">
-        <v>719</v>
+        <v>742</v>
       </c>
     </row>
     <row r="106" spans="1:7" x14ac:dyDescent="0.25">
@@ -4358,7 +4484,7 @@
         <v>209</v>
       </c>
       <c r="G106" t="s">
-        <v>720</v>
+        <v>743</v>
       </c>
     </row>
     <row r="107" spans="1:7" x14ac:dyDescent="0.25">
@@ -4372,7 +4498,7 @@
         <v>211</v>
       </c>
       <c r="G107" t="s">
-        <v>720</v>
+        <v>743</v>
       </c>
     </row>
     <row r="108" spans="1:7" x14ac:dyDescent="0.25">
@@ -4386,7 +4512,7 @@
         <v>213</v>
       </c>
       <c r="G108" t="s">
-        <v>720</v>
+        <v>743</v>
       </c>
     </row>
     <row r="109" spans="1:7" x14ac:dyDescent="0.25">
@@ -4406,7 +4532,7 @@
         <v>670</v>
       </c>
       <c r="G109" t="s">
-        <v>722</v>
+        <v>744</v>
       </c>
     </row>
     <row r="110" spans="1:7" x14ac:dyDescent="0.25">
@@ -4426,7 +4552,7 @@
         <v>671</v>
       </c>
       <c r="G110" t="s">
-        <v>722</v>
+        <v>744</v>
       </c>
     </row>
     <row r="111" spans="1:7" x14ac:dyDescent="0.25">
@@ -4446,7 +4572,7 @@
         <v>672</v>
       </c>
       <c r="G111" t="s">
-        <v>722</v>
+        <v>744</v>
       </c>
     </row>
     <row r="112" spans="1:7" x14ac:dyDescent="0.25">
@@ -4466,7 +4592,7 @@
         <v>673</v>
       </c>
       <c r="G112" t="s">
-        <v>722</v>
+        <v>744</v>
       </c>
     </row>
     <row r="113" spans="1:7" x14ac:dyDescent="0.25">
@@ -4486,7 +4612,7 @@
         <v>674</v>
       </c>
       <c r="G113" t="s">
-        <v>722</v>
+        <v>744</v>
       </c>
     </row>
     <row r="114" spans="1:7" x14ac:dyDescent="0.25">
@@ -4506,7 +4632,7 @@
         <v>675</v>
       </c>
       <c r="G114" t="s">
-        <v>722</v>
+        <v>745</v>
       </c>
     </row>
     <row r="115" spans="1:7" x14ac:dyDescent="0.25">
@@ -4526,7 +4652,7 @@
         <v>676</v>
       </c>
       <c r="G115" t="s">
-        <v>722</v>
+        <v>745</v>
       </c>
     </row>
     <row r="116" spans="1:7" x14ac:dyDescent="0.25">
@@ -4546,7 +4672,7 @@
         <v>677</v>
       </c>
       <c r="G116" t="s">
-        <v>722</v>
+        <v>745</v>
       </c>
     </row>
     <row r="117" spans="1:7" x14ac:dyDescent="0.25">
@@ -4566,7 +4692,7 @@
         <v>678</v>
       </c>
       <c r="G117" t="s">
-        <v>722</v>
+        <v>745</v>
       </c>
     </row>
     <row r="118" spans="1:7" x14ac:dyDescent="0.25">
@@ -4586,7 +4712,7 @@
         <v>679</v>
       </c>
       <c r="G118" t="s">
-        <v>722</v>
+        <v>745</v>
       </c>
     </row>
     <row r="119" spans="1:7" x14ac:dyDescent="0.25">
@@ -4606,7 +4732,7 @@
         <v>680</v>
       </c>
       <c r="G119" t="s">
-        <v>722</v>
+        <v>746</v>
       </c>
     </row>
     <row r="120" spans="1:7" x14ac:dyDescent="0.25">
@@ -4626,7 +4752,7 @@
         <v>681</v>
       </c>
       <c r="G120" t="s">
-        <v>722</v>
+        <v>746</v>
       </c>
     </row>
     <row r="121" spans="1:7" x14ac:dyDescent="0.25">
@@ -4646,7 +4772,7 @@
         <v>682</v>
       </c>
       <c r="G121" t="s">
-        <v>722</v>
+        <v>746</v>
       </c>
     </row>
     <row r="122" spans="1:7" x14ac:dyDescent="0.25">
@@ -4666,7 +4792,7 @@
         <v>683</v>
       </c>
       <c r="G122" t="s">
-        <v>722</v>
+        <v>746</v>
       </c>
     </row>
     <row r="123" spans="1:7" x14ac:dyDescent="0.25">
@@ -4686,7 +4812,7 @@
         <v>684</v>
       </c>
       <c r="G123" t="s">
-        <v>722</v>
+        <v>746</v>
       </c>
     </row>
     <row r="124" spans="1:7" x14ac:dyDescent="0.25">
@@ -4706,7 +4832,7 @@
         <v>685</v>
       </c>
       <c r="G124" t="s">
-        <v>722</v>
+        <v>747</v>
       </c>
     </row>
     <row r="125" spans="1:7" x14ac:dyDescent="0.25">
@@ -4726,7 +4852,7 @@
         <v>686</v>
       </c>
       <c r="G125" t="s">
-        <v>722</v>
+        <v>747</v>
       </c>
     </row>
     <row r="126" spans="1:7" x14ac:dyDescent="0.25">
@@ -4746,7 +4872,7 @@
         <v>687</v>
       </c>
       <c r="G126" t="s">
-        <v>722</v>
+        <v>747</v>
       </c>
     </row>
     <row r="127" spans="1:7" x14ac:dyDescent="0.25">
@@ -4766,7 +4892,7 @@
         <v>688</v>
       </c>
       <c r="G127" t="s">
-        <v>722</v>
+        <v>747</v>
       </c>
     </row>
     <row r="128" spans="1:7" x14ac:dyDescent="0.25">
@@ -4786,7 +4912,7 @@
         <v>689</v>
       </c>
       <c r="G128" t="s">
-        <v>722</v>
+        <v>747</v>
       </c>
     </row>
     <row r="129" spans="1:7" x14ac:dyDescent="0.25">
@@ -4806,7 +4932,7 @@
         <v>690</v>
       </c>
       <c r="G129" t="s">
-        <v>722</v>
+        <v>748</v>
       </c>
     </row>
     <row r="130" spans="1:7" x14ac:dyDescent="0.25">
@@ -4826,7 +4952,7 @@
         <v>691</v>
       </c>
       <c r="G130" t="s">
-        <v>722</v>
+        <v>748</v>
       </c>
     </row>
     <row r="131" spans="1:7" x14ac:dyDescent="0.25">
@@ -4846,7 +4972,7 @@
         <v>692</v>
       </c>
       <c r="G131" t="s">
-        <v>722</v>
+        <v>748</v>
       </c>
     </row>
     <row r="132" spans="1:7" x14ac:dyDescent="0.25">
@@ -4866,7 +4992,7 @@
         <v>693</v>
       </c>
       <c r="G132" t="s">
-        <v>722</v>
+        <v>748</v>
       </c>
     </row>
     <row r="133" spans="1:7" x14ac:dyDescent="0.25">
@@ -4886,7 +5012,7 @@
         <v>694</v>
       </c>
       <c r="G133" t="s">
-        <v>722</v>
+        <v>748</v>
       </c>
     </row>
     <row r="134" spans="1:7" x14ac:dyDescent="0.25">
@@ -4906,7 +5032,7 @@
         <v>695</v>
       </c>
       <c r="G134" t="s">
-        <v>722</v>
+        <v>749</v>
       </c>
     </row>
     <row r="135" spans="1:7" x14ac:dyDescent="0.25">
@@ -4926,7 +5052,7 @@
         <v>696</v>
       </c>
       <c r="G135" t="s">
-        <v>722</v>
+        <v>749</v>
       </c>
     </row>
     <row r="136" spans="1:7" x14ac:dyDescent="0.25">
@@ -4946,7 +5072,7 @@
         <v>697</v>
       </c>
       <c r="G136" t="s">
-        <v>722</v>
+        <v>749</v>
       </c>
     </row>
     <row r="137" spans="1:7" x14ac:dyDescent="0.25">
@@ -4966,7 +5092,7 @@
         <v>698</v>
       </c>
       <c r="G137" t="s">
-        <v>722</v>
+        <v>749</v>
       </c>
     </row>
     <row r="138" spans="1:7" x14ac:dyDescent="0.25">
@@ -4986,7 +5112,7 @@
         <v>699</v>
       </c>
       <c r="G138" t="s">
-        <v>722</v>
+        <v>749</v>
       </c>
     </row>
     <row r="139" spans="1:7" x14ac:dyDescent="0.25">
@@ -5006,7 +5132,7 @@
         <v>700</v>
       </c>
       <c r="G139" t="s">
-        <v>722</v>
+        <v>750</v>
       </c>
     </row>
     <row r="140" spans="1:7" x14ac:dyDescent="0.25">
@@ -5026,7 +5152,7 @@
         <v>701</v>
       </c>
       <c r="G140" t="s">
-        <v>722</v>
+        <v>750</v>
       </c>
     </row>
     <row r="141" spans="1:7" x14ac:dyDescent="0.25">
@@ -5046,7 +5172,7 @@
         <v>702</v>
       </c>
       <c r="G141" t="s">
-        <v>722</v>
+        <v>750</v>
       </c>
     </row>
     <row r="142" spans="1:7" x14ac:dyDescent="0.25">
@@ -5066,7 +5192,7 @@
         <v>703</v>
       </c>
       <c r="G142" t="s">
-        <v>722</v>
+        <v>750</v>
       </c>
     </row>
     <row r="143" spans="1:7" x14ac:dyDescent="0.25">
@@ -5086,7 +5212,7 @@
         <v>704</v>
       </c>
       <c r="G143" t="s">
-        <v>722</v>
+        <v>750</v>
       </c>
     </row>
     <row r="144" spans="1:7" x14ac:dyDescent="0.25">
@@ -5106,7 +5232,7 @@
         <v>705</v>
       </c>
       <c r="G144" t="s">
-        <v>722</v>
+        <v>751</v>
       </c>
     </row>
     <row r="145" spans="1:7" x14ac:dyDescent="0.25">
@@ -5126,7 +5252,7 @@
         <v>706</v>
       </c>
       <c r="G145" t="s">
-        <v>722</v>
+        <v>751</v>
       </c>
     </row>
     <row r="146" spans="1:7" x14ac:dyDescent="0.25">
@@ -5146,7 +5272,7 @@
         <v>707</v>
       </c>
       <c r="G146" t="s">
-        <v>722</v>
+        <v>751</v>
       </c>
     </row>
     <row r="147" spans="1:7" x14ac:dyDescent="0.25">
@@ -5166,7 +5292,7 @@
         <v>708</v>
       </c>
       <c r="G147" t="s">
-        <v>722</v>
+        <v>752</v>
       </c>
     </row>
     <row r="148" spans="1:7" x14ac:dyDescent="0.25">
@@ -5186,7 +5312,7 @@
         <v>709</v>
       </c>
       <c r="G148" t="s">
-        <v>722</v>
+        <v>752</v>
       </c>
     </row>
     <row r="149" spans="1:7" x14ac:dyDescent="0.25">
@@ -5206,7 +5332,7 @@
         <v>710</v>
       </c>
       <c r="G149" t="s">
-        <v>722</v>
+        <v>752</v>
       </c>
     </row>
     <row r="150" spans="1:7" x14ac:dyDescent="0.25">
@@ -5226,7 +5352,7 @@
         <v>711</v>
       </c>
       <c r="G150" t="s">
-        <v>722</v>
+        <v>752</v>
       </c>
     </row>
     <row r="151" spans="1:7" x14ac:dyDescent="0.25">
@@ -5246,7 +5372,7 @@
         <v>712</v>
       </c>
       <c r="G151" t="s">
-        <v>722</v>
+        <v>752</v>
       </c>
     </row>
     <row r="152" spans="1:7" x14ac:dyDescent="0.25">
@@ -5266,7 +5392,7 @@
         <v>713</v>
       </c>
       <c r="G152" t="s">
-        <v>722</v>
+        <v>753</v>
       </c>
     </row>
     <row r="153" spans="1:7" x14ac:dyDescent="0.25">
@@ -5283,7 +5409,7 @@
         <v>1</v>
       </c>
       <c r="G153" t="s">
-        <v>722</v>
+        <v>753</v>
       </c>
     </row>
     <row r="154" spans="1:7" x14ac:dyDescent="0.25">
@@ -5303,7 +5429,7 @@
         <v>714</v>
       </c>
       <c r="G154" t="s">
-        <v>722</v>
+        <v>753</v>
       </c>
     </row>
     <row r="155" spans="1:7" x14ac:dyDescent="0.25">
@@ -5317,7 +5443,7 @@
         <v>93</v>
       </c>
       <c r="G155" t="s">
-        <v>723</v>
+        <v>754</v>
       </c>
     </row>
     <row r="156" spans="1:7" x14ac:dyDescent="0.25">
@@ -5331,7 +5457,7 @@
         <v>95</v>
       </c>
       <c r="G156" t="s">
-        <v>723</v>
+        <v>754</v>
       </c>
     </row>
     <row r="157" spans="1:7" x14ac:dyDescent="0.25">
@@ -5345,7 +5471,7 @@
         <v>97</v>
       </c>
       <c r="G157" t="s">
-        <v>723</v>
+        <v>754</v>
       </c>
     </row>
     <row r="158" spans="1:7" x14ac:dyDescent="0.25">
@@ -5359,7 +5485,7 @@
         <v>99</v>
       </c>
       <c r="G158" t="s">
-        <v>723</v>
+        <v>754</v>
       </c>
     </row>
     <row r="159" spans="1:7" x14ac:dyDescent="0.25">
@@ -5373,7 +5499,7 @@
         <v>101</v>
       </c>
       <c r="G159" t="s">
-        <v>723</v>
+        <v>754</v>
       </c>
     </row>
     <row r="160" spans="1:7" x14ac:dyDescent="0.25">
@@ -5387,7 +5513,7 @@
         <v>103</v>
       </c>
       <c r="G160" t="s">
-        <v>723</v>
+        <v>755</v>
       </c>
     </row>
     <row r="161" spans="1:7" x14ac:dyDescent="0.25">
@@ -5404,7 +5530,7 @@
         <v>1</v>
       </c>
       <c r="G161" t="s">
-        <v>723</v>
+        <v>755</v>
       </c>
     </row>
     <row r="162" spans="1:7" x14ac:dyDescent="0.25">
@@ -5421,7 +5547,7 @@
         <v>1</v>
       </c>
       <c r="G162" t="s">
-        <v>723</v>
+        <v>755</v>
       </c>
     </row>
     <row r="163" spans="1:7" x14ac:dyDescent="0.25">
@@ -5435,7 +5561,7 @@
         <v>109</v>
       </c>
       <c r="G163" t="s">
-        <v>723</v>
+        <v>755</v>
       </c>
     </row>
     <row r="164" spans="1:7" x14ac:dyDescent="0.25">
@@ -5449,7 +5575,7 @@
         <v>111</v>
       </c>
       <c r="G164" t="s">
-        <v>723</v>
+        <v>755</v>
       </c>
     </row>
     <row r="165" spans="1:7" x14ac:dyDescent="0.25">
@@ -5463,7 +5589,7 @@
         <v>113</v>
       </c>
       <c r="G165" t="s">
-        <v>723</v>
+        <v>756</v>
       </c>
     </row>
     <row r="166" spans="1:7" x14ac:dyDescent="0.25">
@@ -5480,7 +5606,7 @@
         <v>1</v>
       </c>
       <c r="G166" t="s">
-        <v>723</v>
+        <v>756</v>
       </c>
     </row>
     <row r="167" spans="1:7" x14ac:dyDescent="0.25">
@@ -5497,7 +5623,7 @@
         <v>1</v>
       </c>
       <c r="G167" t="s">
-        <v>723</v>
+        <v>756</v>
       </c>
     </row>
     <row r="168" spans="1:7" x14ac:dyDescent="0.25">
@@ -5511,7 +5637,7 @@
         <v>119</v>
       </c>
       <c r="G168" t="s">
-        <v>723</v>
+        <v>756</v>
       </c>
     </row>
     <row r="169" spans="1:7" x14ac:dyDescent="0.25">
@@ -5525,7 +5651,7 @@
         <v>121</v>
       </c>
       <c r="G169" t="s">
-        <v>723</v>
+        <v>756</v>
       </c>
     </row>
     <row r="170" spans="1:7" x14ac:dyDescent="0.25">
@@ -5539,7 +5665,7 @@
         <v>123</v>
       </c>
       <c r="G170" t="s">
-        <v>723</v>
+        <v>757</v>
       </c>
     </row>
     <row r="171" spans="1:7" x14ac:dyDescent="0.25">
@@ -5553,7 +5679,7 @@
         <v>125</v>
       </c>
       <c r="G171" t="s">
-        <v>723</v>
+        <v>757</v>
       </c>
     </row>
     <row r="172" spans="1:7" x14ac:dyDescent="0.25">
@@ -5567,7 +5693,7 @@
         <v>127</v>
       </c>
       <c r="G172" t="s">
-        <v>723</v>
+        <v>757</v>
       </c>
     </row>
     <row r="173" spans="1:7" x14ac:dyDescent="0.25">
@@ -5581,7 +5707,7 @@
         <v>129</v>
       </c>
       <c r="G173" t="s">
-        <v>723</v>
+        <v>757</v>
       </c>
     </row>
     <row r="174" spans="1:7" x14ac:dyDescent="0.25">
@@ -5595,7 +5721,7 @@
         <v>131</v>
       </c>
       <c r="G174" t="s">
-        <v>723</v>
+        <v>757</v>
       </c>
     </row>
     <row r="175" spans="1:7" x14ac:dyDescent="0.25">
@@ -5609,7 +5735,7 @@
         <v>133</v>
       </c>
       <c r="G175" t="s">
-        <v>724</v>
+        <v>758</v>
       </c>
     </row>
     <row r="176" spans="1:7" x14ac:dyDescent="0.25">
@@ -5623,7 +5749,7 @@
         <v>135</v>
       </c>
       <c r="G176" t="s">
-        <v>724</v>
+        <v>758</v>
       </c>
     </row>
     <row r="177" spans="1:7" x14ac:dyDescent="0.25">
@@ -5637,7 +5763,7 @@
         <v>137</v>
       </c>
       <c r="G177" t="s">
-        <v>724</v>
+        <v>758</v>
       </c>
     </row>
     <row r="178" spans="1:7" x14ac:dyDescent="0.25">
@@ -5651,7 +5777,7 @@
         <v>139</v>
       </c>
       <c r="G178" t="s">
-        <v>724</v>
+        <v>758</v>
       </c>
     </row>
     <row r="179" spans="1:7" x14ac:dyDescent="0.25">
@@ -5665,7 +5791,7 @@
         <v>141</v>
       </c>
       <c r="G179" t="s">
-        <v>724</v>
+        <v>758</v>
       </c>
     </row>
     <row r="180" spans="1:7" x14ac:dyDescent="0.25">
@@ -5679,7 +5805,7 @@
         <v>143</v>
       </c>
       <c r="G180" t="s">
-        <v>725</v>
+        <v>759</v>
       </c>
     </row>
     <row r="181" spans="1:7" x14ac:dyDescent="0.25">
@@ -5693,7 +5819,7 @@
         <v>145</v>
       </c>
       <c r="G181" t="s">
-        <v>725</v>
+        <v>759</v>
       </c>
     </row>
     <row r="182" spans="1:7" x14ac:dyDescent="0.25">
@@ -5707,7 +5833,7 @@
         <v>147</v>
       </c>
       <c r="G182" t="s">
-        <v>725</v>
+        <v>759</v>
       </c>
     </row>
     <row r="183" spans="1:7" x14ac:dyDescent="0.25">
@@ -5721,7 +5847,7 @@
         <v>149</v>
       </c>
       <c r="G183" t="s">
-        <v>725</v>
+        <v>760</v>
       </c>
     </row>
     <row r="184" spans="1:7" x14ac:dyDescent="0.25">
@@ -5735,7 +5861,7 @@
         <v>151</v>
       </c>
       <c r="G184" t="s">
-        <v>725</v>
+        <v>760</v>
       </c>
     </row>
     <row r="185" spans="1:7" x14ac:dyDescent="0.25">
@@ -5749,7 +5875,7 @@
         <v>153</v>
       </c>
       <c r="G185" t="s">
-        <v>725</v>
+        <v>760</v>
       </c>
     </row>
     <row r="186" spans="1:7" x14ac:dyDescent="0.25">
@@ -5763,7 +5889,7 @@
         <v>155</v>
       </c>
       <c r="G186" t="s">
-        <v>725</v>
+        <v>761</v>
       </c>
     </row>
     <row r="187" spans="1:7" x14ac:dyDescent="0.25">
@@ -5777,7 +5903,7 @@
         <v>157</v>
       </c>
       <c r="G187" t="s">
-        <v>725</v>
+        <v>761</v>
       </c>
     </row>
     <row r="188" spans="1:7" x14ac:dyDescent="0.25">
@@ -5791,7 +5917,7 @@
         <v>159</v>
       </c>
       <c r="G188" t="s">
-        <v>725</v>
+        <v>761</v>
       </c>
     </row>
     <row r="189" spans="1:7" x14ac:dyDescent="0.25">
@@ -5805,7 +5931,7 @@
         <v>161</v>
       </c>
       <c r="G189" t="s">
-        <v>725</v>
+        <v>762</v>
       </c>
     </row>
     <row r="190" spans="1:7" x14ac:dyDescent="0.25">
@@ -5819,7 +5945,7 @@
         <v>163</v>
       </c>
       <c r="G190" t="s">
-        <v>725</v>
+        <v>762</v>
       </c>
     </row>
     <row r="191" spans="1:7" x14ac:dyDescent="0.25">
@@ -5833,7 +5959,7 @@
         <v>165</v>
       </c>
       <c r="G191" t="s">
-        <v>725</v>
+        <v>762</v>
       </c>
     </row>
     <row r="192" spans="1:7" x14ac:dyDescent="0.25">
@@ -5847,7 +5973,7 @@
         <v>167</v>
       </c>
       <c r="G192" t="s">
-        <v>725</v>
+        <v>763</v>
       </c>
     </row>
     <row r="193" spans="1:7" x14ac:dyDescent="0.25">
@@ -5861,7 +5987,7 @@
         <v>169</v>
       </c>
       <c r="G193" t="s">
-        <v>725</v>
+        <v>763</v>
       </c>
     </row>
     <row r="194" spans="1:7" x14ac:dyDescent="0.25">
@@ -5875,7 +6001,7 @@
         <v>171</v>
       </c>
       <c r="G194" t="s">
-        <v>725</v>
+        <v>763</v>
       </c>
     </row>
     <row r="195" spans="1:7" x14ac:dyDescent="0.25">
@@ -5889,7 +6015,7 @@
         <v>173</v>
       </c>
       <c r="G195" t="s">
-        <v>725</v>
+        <v>764</v>
       </c>
     </row>
     <row r="196" spans="1:7" x14ac:dyDescent="0.25">
@@ -5903,7 +6029,7 @@
         <v>175</v>
       </c>
       <c r="G196" t="s">
-        <v>725</v>
+        <v>764</v>
       </c>
     </row>
     <row r="197" spans="1:7" x14ac:dyDescent="0.25">
@@ -5917,7 +6043,7 @@
         <v>177</v>
       </c>
       <c r="G197" t="s">
-        <v>725</v>
+        <v>764</v>
       </c>
     </row>
     <row r="198" spans="1:7" x14ac:dyDescent="0.25">
@@ -5931,7 +6057,7 @@
         <v>179</v>
       </c>
       <c r="G198" t="s">
-        <v>725</v>
+        <v>765</v>
       </c>
     </row>
     <row r="199" spans="1:7" x14ac:dyDescent="0.25">
@@ -5948,7 +6074,7 @@
         <v>1</v>
       </c>
       <c r="G199" t="s">
-        <v>725</v>
+        <v>765</v>
       </c>
     </row>
     <row r="200" spans="1:7" x14ac:dyDescent="0.25">
@@ -5962,7 +6088,7 @@
         <v>183</v>
       </c>
       <c r="G200" t="s">
-        <v>725</v>
+        <v>765</v>
       </c>
     </row>
     <row r="201" spans="1:7" x14ac:dyDescent="0.25">
@@ -5976,7 +6102,7 @@
         <v>185</v>
       </c>
       <c r="G201" t="s">
-        <v>726</v>
+        <v>766</v>
       </c>
     </row>
     <row r="202" spans="1:7" x14ac:dyDescent="0.25">
@@ -5990,7 +6116,7 @@
         <v>187</v>
       </c>
       <c r="G202" t="s">
-        <v>726</v>
+        <v>766</v>
       </c>
     </row>
     <row r="203" spans="1:7" x14ac:dyDescent="0.25">
@@ -6004,7 +6130,7 @@
         <v>189</v>
       </c>
       <c r="G203" t="s">
-        <v>726</v>
+        <v>766</v>
       </c>
     </row>
     <row r="204" spans="1:7" x14ac:dyDescent="0.25">
@@ -6021,7 +6147,7 @@
         <v>1</v>
       </c>
       <c r="G204" t="s">
-        <v>726</v>
+        <v>767</v>
       </c>
     </row>
     <row r="205" spans="1:7" x14ac:dyDescent="0.25">
@@ -6038,7 +6164,7 @@
         <v>1</v>
       </c>
       <c r="G205" t="s">
-        <v>726</v>
+        <v>767</v>
       </c>
     </row>
     <row r="206" spans="1:7" x14ac:dyDescent="0.25">
@@ -6055,7 +6181,7 @@
         <v>1</v>
       </c>
       <c r="G206" t="s">
-        <v>726</v>
+        <v>767</v>
       </c>
     </row>
     <row r="207" spans="1:7" x14ac:dyDescent="0.25">
@@ -6072,7 +6198,7 @@
         <v>1</v>
       </c>
       <c r="G207" t="s">
-        <v>726</v>
+        <v>768</v>
       </c>
     </row>
     <row r="208" spans="1:7" x14ac:dyDescent="0.25">
@@ -6089,7 +6215,7 @@
         <v>1</v>
       </c>
       <c r="G208" t="s">
-        <v>726</v>
+        <v>768</v>
       </c>
     </row>
     <row r="209" spans="1:7" x14ac:dyDescent="0.25">
@@ -6106,7 +6232,7 @@
         <v>1</v>
       </c>
       <c r="G209" t="s">
-        <v>726</v>
+        <v>768</v>
       </c>
     </row>
     <row r="210" spans="1:7" x14ac:dyDescent="0.25">
@@ -6120,7 +6246,7 @@
         <v>203</v>
       </c>
       <c r="G210" t="s">
-        <v>726</v>
+        <v>769</v>
       </c>
     </row>
     <row r="211" spans="1:7" x14ac:dyDescent="0.25">
@@ -6134,7 +6260,7 @@
         <v>205</v>
       </c>
       <c r="G211" t="s">
-        <v>726</v>
+        <v>769</v>
       </c>
     </row>
     <row r="212" spans="1:7" x14ac:dyDescent="0.25">
@@ -6148,7 +6274,7 @@
         <v>207</v>
       </c>
       <c r="G212" t="s">
-        <v>726</v>
+        <v>769</v>
       </c>
     </row>
     <row r="213" spans="1:7" x14ac:dyDescent="0.25">
@@ -6162,7 +6288,7 @@
         <v>209</v>
       </c>
       <c r="G213" t="s">
-        <v>727</v>
+        <v>770</v>
       </c>
     </row>
     <row r="214" spans="1:7" x14ac:dyDescent="0.25">
@@ -6176,7 +6302,7 @@
         <v>211</v>
       </c>
       <c r="G214" t="s">
-        <v>727</v>
+        <v>770</v>
       </c>
     </row>
     <row r="215" spans="1:7" x14ac:dyDescent="0.25">
@@ -6190,7 +6316,7 @@
         <v>213</v>
       </c>
       <c r="G215" t="s">
-        <v>727</v>
+        <v>770</v>
       </c>
     </row>
     <row r="216" spans="1:7" x14ac:dyDescent="0.25">
@@ -6204,7 +6330,7 @@
         <v>1</v>
       </c>
       <c r="G216" t="s">
-        <v>728</v>
+        <v>716</v>
       </c>
     </row>
     <row r="217" spans="1:7" x14ac:dyDescent="0.25">
@@ -6218,7 +6344,7 @@
         <v>1</v>
       </c>
       <c r="G217" t="s">
-        <v>728</v>
+        <v>716</v>
       </c>
     </row>
     <row r="218" spans="1:7" x14ac:dyDescent="0.25">
@@ -6232,7 +6358,7 @@
         <v>1</v>
       </c>
       <c r="G218" t="s">
-        <v>728</v>
+        <v>716</v>
       </c>
     </row>
     <row r="219" spans="1:7" x14ac:dyDescent="0.25">
@@ -6246,7 +6372,7 @@
         <v>1</v>
       </c>
       <c r="G219" t="s">
-        <v>728</v>
+        <v>716</v>
       </c>
     </row>
     <row r="220" spans="1:7" x14ac:dyDescent="0.25">
@@ -6260,7 +6386,7 @@
         <v>1</v>
       </c>
       <c r="G220" t="s">
-        <v>728</v>
+        <v>716</v>
       </c>
     </row>
     <row r="221" spans="1:7" x14ac:dyDescent="0.25">
@@ -6277,7 +6403,7 @@
         <v>1</v>
       </c>
       <c r="G221" t="s">
-        <v>728</v>
+        <v>716</v>
       </c>
     </row>
     <row r="222" spans="1:7" x14ac:dyDescent="0.25">
@@ -6294,7 +6420,7 @@
         <v>1</v>
       </c>
       <c r="G222" t="s">
-        <v>728</v>
+        <v>716</v>
       </c>
     </row>
     <row r="223" spans="1:7" x14ac:dyDescent="0.25">
@@ -6308,7 +6434,7 @@
         <v>1</v>
       </c>
       <c r="G223" t="s">
-        <v>728</v>
+        <v>716</v>
       </c>
     </row>
     <row r="224" spans="1:7" x14ac:dyDescent="0.25">
@@ -6325,7 +6451,7 @@
         <v>1</v>
       </c>
       <c r="G224" t="s">
-        <v>728</v>
+        <v>716</v>
       </c>
     </row>
     <row r="225" spans="1:7" x14ac:dyDescent="0.25">
@@ -6342,7 +6468,7 @@
         <v>1</v>
       </c>
       <c r="G225" t="s">
-        <v>728</v>
+        <v>716</v>
       </c>
     </row>
     <row r="226" spans="1:7" x14ac:dyDescent="0.25">
@@ -6356,7 +6482,7 @@
         <v>1</v>
       </c>
       <c r="G226" t="s">
-        <v>728</v>
+        <v>716</v>
       </c>
     </row>
     <row r="227" spans="1:7" x14ac:dyDescent="0.25">
@@ -6373,7 +6499,7 @@
         <v>1</v>
       </c>
       <c r="G227" t="s">
-        <v>728</v>
+        <v>716</v>
       </c>
     </row>
     <row r="228" spans="1:7" x14ac:dyDescent="0.25">
@@ -6387,7 +6513,7 @@
         <v>1</v>
       </c>
       <c r="G228" t="s">
-        <v>728</v>
+        <v>716</v>
       </c>
     </row>
     <row r="229" spans="1:7" x14ac:dyDescent="0.25">
@@ -6404,7 +6530,7 @@
         <v>1</v>
       </c>
       <c r="G229" t="s">
-        <v>728</v>
+        <v>716</v>
       </c>
     </row>
     <row r="230" spans="1:7" x14ac:dyDescent="0.25">
@@ -6421,7 +6547,7 @@
         <v>1</v>
       </c>
       <c r="G230" t="s">
-        <v>728</v>
+        <v>716</v>
       </c>
     </row>
     <row r="231" spans="1:7" x14ac:dyDescent="0.25">
@@ -6438,7 +6564,7 @@
         <v>1</v>
       </c>
       <c r="G231" t="s">
-        <v>728</v>
+        <v>716</v>
       </c>
     </row>
     <row r="232" spans="1:7" x14ac:dyDescent="0.25">
@@ -6455,7 +6581,7 @@
         <v>1</v>
       </c>
       <c r="G232" t="s">
-        <v>728</v>
+        <v>716</v>
       </c>
     </row>
     <row r="233" spans="1:7" x14ac:dyDescent="0.25">
@@ -6472,7 +6598,7 @@
         <v>1</v>
       </c>
       <c r="G233" t="s">
-        <v>728</v>
+        <v>716</v>
       </c>
     </row>
     <row r="234" spans="1:7" x14ac:dyDescent="0.25">
@@ -6486,7 +6612,7 @@
         <v>1</v>
       </c>
       <c r="G234" t="s">
-        <v>728</v>
+        <v>716</v>
       </c>
     </row>
     <row r="235" spans="1:7" x14ac:dyDescent="0.25">
@@ -6503,7 +6629,7 @@
         <v>1</v>
       </c>
       <c r="G235" t="s">
-        <v>728</v>
+        <v>716</v>
       </c>
     </row>
     <row r="236" spans="1:7" x14ac:dyDescent="0.25">
@@ -6520,7 +6646,7 @@
         <v>1</v>
       </c>
       <c r="G236" t="s">
-        <v>728</v>
+        <v>716</v>
       </c>
     </row>
     <row r="237" spans="1:7" x14ac:dyDescent="0.25">
@@ -6537,7 +6663,7 @@
         <v>1</v>
       </c>
       <c r="G237" t="s">
-        <v>728</v>
+        <v>716</v>
       </c>
     </row>
     <row r="238" spans="1:7" x14ac:dyDescent="0.25">
@@ -6554,7 +6680,7 @@
         <v>1</v>
       </c>
       <c r="G238" t="s">
-        <v>728</v>
+        <v>716</v>
       </c>
     </row>
     <row r="239" spans="1:7" x14ac:dyDescent="0.25">
@@ -6571,7 +6697,7 @@
         <v>1</v>
       </c>
       <c r="G239" t="s">
-        <v>728</v>
+        <v>716</v>
       </c>
     </row>
     <row r="240" spans="1:7" x14ac:dyDescent="0.25">
@@ -6588,7 +6714,7 @@
         <v>1</v>
       </c>
       <c r="G240" t="s">
-        <v>728</v>
+        <v>716</v>
       </c>
     </row>
     <row r="241" spans="1:7" x14ac:dyDescent="0.25">
@@ -6602,7 +6728,7 @@
         <v>1</v>
       </c>
       <c r="G241" t="s">
-        <v>728</v>
+        <v>716</v>
       </c>
     </row>
     <row r="242" spans="1:7" x14ac:dyDescent="0.25">
@@ -6616,7 +6742,7 @@
         <v>1</v>
       </c>
       <c r="G242" t="s">
-        <v>728</v>
+        <v>716</v>
       </c>
     </row>
     <row r="243" spans="1:7" x14ac:dyDescent="0.25">
@@ -6630,7 +6756,7 @@
         <v>1</v>
       </c>
       <c r="G243" t="s">
-        <v>728</v>
+        <v>716</v>
       </c>
     </row>
     <row r="244" spans="1:7" x14ac:dyDescent="0.25">
@@ -6644,7 +6770,7 @@
         <v>1</v>
       </c>
       <c r="G244" t="s">
-        <v>728</v>
+        <v>716</v>
       </c>
     </row>
     <row r="245" spans="1:7" x14ac:dyDescent="0.25">
@@ -6661,7 +6787,7 @@
         <v>1</v>
       </c>
       <c r="G245" t="s">
-        <v>728</v>
+        <v>716</v>
       </c>
     </row>
     <row r="246" spans="1:7" x14ac:dyDescent="0.25">
@@ -6675,7 +6801,7 @@
         <v>1</v>
       </c>
       <c r="G246" t="s">
-        <v>728</v>
+        <v>716</v>
       </c>
     </row>
     <row r="247" spans="1:7" x14ac:dyDescent="0.25">
@@ -6689,7 +6815,7 @@
         <v>1</v>
       </c>
       <c r="G247" t="s">
-        <v>728</v>
+        <v>716</v>
       </c>
     </row>
     <row r="248" spans="1:7" x14ac:dyDescent="0.25">
@@ -6703,7 +6829,7 @@
         <v>1</v>
       </c>
       <c r="G248" t="s">
-        <v>728</v>
+        <v>716</v>
       </c>
     </row>
     <row r="249" spans="1:7" x14ac:dyDescent="0.25">
@@ -6717,7 +6843,7 @@
         <v>1</v>
       </c>
       <c r="G249" t="s">
-        <v>728</v>
+        <v>716</v>
       </c>
     </row>
     <row r="250" spans="1:7" x14ac:dyDescent="0.25">
@@ -6731,7 +6857,7 @@
         <v>1</v>
       </c>
       <c r="G250" t="s">
-        <v>728</v>
+        <v>716</v>
       </c>
     </row>
     <row r="251" spans="1:7" x14ac:dyDescent="0.25">
@@ -6745,7 +6871,7 @@
         <v>1</v>
       </c>
       <c r="G251" t="s">
-        <v>728</v>
+        <v>716</v>
       </c>
     </row>
     <row r="252" spans="1:7" x14ac:dyDescent="0.25">
@@ -6759,7 +6885,7 @@
         <v>1</v>
       </c>
       <c r="G252" t="s">
-        <v>728</v>
+        <v>716</v>
       </c>
     </row>
     <row r="253" spans="1:7" x14ac:dyDescent="0.25">
@@ -6773,7 +6899,7 @@
         <v>1</v>
       </c>
       <c r="G253" t="s">
-        <v>728</v>
+        <v>716</v>
       </c>
     </row>
     <row r="254" spans="1:7" x14ac:dyDescent="0.25">
@@ -6787,7 +6913,7 @@
         <v>1</v>
       </c>
       <c r="G254" t="s">
-        <v>728</v>
+        <v>716</v>
       </c>
     </row>
     <row r="255" spans="1:7" x14ac:dyDescent="0.25">
@@ -6801,7 +6927,7 @@
         <v>1</v>
       </c>
       <c r="G255" t="s">
-        <v>728</v>
+        <v>716</v>
       </c>
     </row>
     <row r="256" spans="1:7" x14ac:dyDescent="0.25">
@@ -6815,7 +6941,7 @@
         <v>1</v>
       </c>
       <c r="G256" t="s">
-        <v>728</v>
+        <v>716</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Better tags for special katakana
</commit_message>
<xml_diff>
--- a/read-and-write-kana/Note Types/Read & Write Kana/Read & Write Kana - Data Sheet.xlsx
+++ b/read-and-write-kana/Note Types/Read & Write Kana/Read & Write Kana - Data Sheet.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1185" uniqueCount="771">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1185" uniqueCount="793">
   <si>
     <t>あ</t>
   </si>
@@ -2164,9 +2164,6 @@
     <t>Tags</t>
   </si>
   <si>
-    <t>katakana special foreign</t>
-  </si>
-  <si>
     <t>hiragana gojuon seion a_series</t>
   </si>
   <si>
@@ -2327,6 +2324,75 @@
   </si>
   <si>
     <t>katakana yoon_dakuon yoon_handakuon h_series hy_series p_series py_series</t>
+  </si>
+  <si>
+    <t>katakana gojuon seion h_series f_series</t>
+  </si>
+  <si>
+    <t>katakana special foreign dakuon_sp a_series_sp v_series v_series_x</t>
+  </si>
+  <si>
+    <t>katakana special foreign dakuon_sp s_series_sp s_series_x sh_series_sp sh_series_x j_series_sp j_series_x</t>
+  </si>
+  <si>
+    <t>katakana special foreign dakuon_sp t_series_sp t_series_x d_series_sp d_series_x</t>
+  </si>
+  <si>
+    <t>katakana special foreign gojuon_sp seion_sp a_series_sp y_series_x</t>
+  </si>
+  <si>
+    <t>katakana special foreign gojuon_sp seion_sp a_series_sp w_series_x</t>
+  </si>
+  <si>
+    <t>katakana special foreign gojuon_sp seion_sp s_series_sp s_series_x sh_series_sp sh_series_x</t>
+  </si>
+  <si>
+    <t>katakana special foreign gojuon_sp seion_sp t_series_sp t_series_x ch_series_sp ch_series_x</t>
+  </si>
+  <si>
+    <t>katakana special foreign gojuon_sp seion_sp t_series_sp t_series_x</t>
+  </si>
+  <si>
+    <t>katakana gojuon seion t_series ch_series</t>
+  </si>
+  <si>
+    <t>katakana gojuon seion t_series ts_series</t>
+  </si>
+  <si>
+    <t>katakana gojuon seion s_series sh_series</t>
+  </si>
+  <si>
+    <t>katakana special foreign gojuon_sp seion_sp t_series_sp t_series_x ts_series_sp ts_series_x</t>
+  </si>
+  <si>
+    <t>katakana special foreign gojuon_sp seion_sp h_series_sp f_series_sp f_series_x</t>
+  </si>
+  <si>
+    <t>katakana special foreign yoon_dakuon_sp a_series_sp v_series v_series_x vy_series vy_series_x</t>
+  </si>
+  <si>
+    <t>katakana special foreign yoon_sp t_series_sp ty_series ty_series_x</t>
+  </si>
+  <si>
+    <t>katakana special foreign yoon_dakuon_sp t_series_sp ty_series ty_series_x</t>
+  </si>
+  <si>
+    <t>katakana special foreign yoon_dakuon_sp f_series_sp f_series_x fy_series fy_series_x</t>
+  </si>
+  <si>
+    <t>katakana special foreign gojuon_sp seion_sp s_series_sp sw_series sw_series_x</t>
+  </si>
+  <si>
+    <t>katakana special foreign gojuon_sp seion_sp s_series_sp s_series_x sw_series sw_series_x</t>
+  </si>
+  <si>
+    <t>katakana special foreign dakuon_sp s_series_sp z_series_x zw_series zw_series_x</t>
+  </si>
+  <si>
+    <t>katakana dakuon s_series z_series j_series</t>
+  </si>
+  <si>
+    <t>katakana special foreign dakuon_sp s_series_sp zw_series zw_series_x</t>
   </si>
 </sst>
 </file>
@@ -2679,7 +2745,7 @@
     <col min="4" max="4" width="22.42578125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="35.140625" customWidth="1"/>
     <col min="6" max="6" width="58.85546875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="72.5703125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="97.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
@@ -2722,7 +2788,7 @@
         <v>624</v>
       </c>
       <c r="G2" t="s">
-        <v>717</v>
+        <v>716</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
@@ -2742,7 +2808,7 @@
         <v>625</v>
       </c>
       <c r="G3" t="s">
-        <v>717</v>
+        <v>716</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
@@ -2762,7 +2828,7 @@
         <v>626</v>
       </c>
       <c r="G4" t="s">
-        <v>717</v>
+        <v>716</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
@@ -2782,7 +2848,7 @@
         <v>627</v>
       </c>
       <c r="G5" t="s">
-        <v>717</v>
+        <v>716</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
@@ -2802,7 +2868,7 @@
         <v>628</v>
       </c>
       <c r="G6" t="s">
-        <v>717</v>
+        <v>716</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
@@ -2822,7 +2888,7 @@
         <v>629</v>
       </c>
       <c r="G7" t="s">
-        <v>718</v>
+        <v>717</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
@@ -2842,7 +2908,7 @@
         <v>630</v>
       </c>
       <c r="G8" t="s">
-        <v>718</v>
+        <v>717</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
@@ -2862,7 +2928,7 @@
         <v>631</v>
       </c>
       <c r="G9" t="s">
-        <v>718</v>
+        <v>717</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
@@ -2882,7 +2948,7 @@
         <v>632</v>
       </c>
       <c r="G10" t="s">
-        <v>718</v>
+        <v>717</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
@@ -2902,7 +2968,7 @@
         <v>633</v>
       </c>
       <c r="G11" t="s">
-        <v>718</v>
+        <v>717</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
@@ -2922,7 +2988,7 @@
         <v>634</v>
       </c>
       <c r="G12" t="s">
-        <v>719</v>
+        <v>718</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
@@ -2942,7 +3008,7 @@
         <v>635</v>
       </c>
       <c r="G13" t="s">
-        <v>719</v>
+        <v>718</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
@@ -2962,7 +3028,7 @@
         <v>636</v>
       </c>
       <c r="G14" t="s">
-        <v>719</v>
+        <v>718</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
@@ -2982,7 +3048,7 @@
         <v>637</v>
       </c>
       <c r="G15" t="s">
-        <v>719</v>
+        <v>718</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
@@ -3002,7 +3068,7 @@
         <v>638</v>
       </c>
       <c r="G16" t="s">
-        <v>719</v>
+        <v>718</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
@@ -3022,7 +3088,7 @@
         <v>639</v>
       </c>
       <c r="G17" t="s">
-        <v>720</v>
+        <v>719</v>
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
@@ -3042,7 +3108,7 @@
         <v>640</v>
       </c>
       <c r="G18" t="s">
-        <v>720</v>
+        <v>719</v>
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.25">
@@ -3062,7 +3128,7 @@
         <v>641</v>
       </c>
       <c r="G19" t="s">
-        <v>720</v>
+        <v>719</v>
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.25">
@@ -3082,7 +3148,7 @@
         <v>642</v>
       </c>
       <c r="G20" t="s">
-        <v>720</v>
+        <v>719</v>
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.25">
@@ -3102,7 +3168,7 @@
         <v>643</v>
       </c>
       <c r="G21" t="s">
-        <v>720</v>
+        <v>719</v>
       </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.25">
@@ -3122,7 +3188,7 @@
         <v>644</v>
       </c>
       <c r="G22" t="s">
-        <v>721</v>
+        <v>720</v>
       </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.25">
@@ -3142,7 +3208,7 @@
         <v>645</v>
       </c>
       <c r="G23" t="s">
-        <v>721</v>
+        <v>720</v>
       </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.25">
@@ -3162,7 +3228,7 @@
         <v>646</v>
       </c>
       <c r="G24" t="s">
-        <v>721</v>
+        <v>720</v>
       </c>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.25">
@@ -3182,7 +3248,7 @@
         <v>647</v>
       </c>
       <c r="G25" t="s">
-        <v>721</v>
+        <v>720</v>
       </c>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.25">
@@ -3202,7 +3268,7 @@
         <v>648</v>
       </c>
       <c r="G26" t="s">
-        <v>721</v>
+        <v>720</v>
       </c>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.25">
@@ -3222,7 +3288,7 @@
         <v>649</v>
       </c>
       <c r="G27" t="s">
-        <v>722</v>
+        <v>721</v>
       </c>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.25">
@@ -3242,7 +3308,7 @@
         <v>650</v>
       </c>
       <c r="G28" t="s">
-        <v>722</v>
+        <v>721</v>
       </c>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.25">
@@ -3262,7 +3328,7 @@
         <v>651</v>
       </c>
       <c r="G29" t="s">
-        <v>722</v>
+        <v>721</v>
       </c>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.25">
@@ -3282,7 +3348,7 @@
         <v>652</v>
       </c>
       <c r="G30" t="s">
-        <v>722</v>
+        <v>721</v>
       </c>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.25">
@@ -3302,7 +3368,7 @@
         <v>653</v>
       </c>
       <c r="G31" t="s">
-        <v>722</v>
+        <v>721</v>
       </c>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.25">
@@ -3322,7 +3388,7 @@
         <v>654</v>
       </c>
       <c r="G32" t="s">
-        <v>723</v>
+        <v>722</v>
       </c>
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.25">
@@ -3342,7 +3408,7 @@
         <v>655</v>
       </c>
       <c r="G33" t="s">
-        <v>723</v>
+        <v>722</v>
       </c>
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.25">
@@ -3362,7 +3428,7 @@
         <v>656</v>
       </c>
       <c r="G34" t="s">
-        <v>723</v>
+        <v>722</v>
       </c>
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.25">
@@ -3382,7 +3448,7 @@
         <v>657</v>
       </c>
       <c r="G35" t="s">
-        <v>723</v>
+        <v>722</v>
       </c>
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.25">
@@ -3402,7 +3468,7 @@
         <v>658</v>
       </c>
       <c r="G36" t="s">
-        <v>723</v>
+        <v>722</v>
       </c>
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.25">
@@ -3422,7 +3488,7 @@
         <v>659</v>
       </c>
       <c r="G37" t="s">
-        <v>724</v>
+        <v>723</v>
       </c>
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.25">
@@ -3442,7 +3508,7 @@
         <v>660</v>
       </c>
       <c r="G38" t="s">
-        <v>724</v>
+        <v>723</v>
       </c>
     </row>
     <row r="39" spans="1:7" x14ac:dyDescent="0.25">
@@ -3462,7 +3528,7 @@
         <v>661</v>
       </c>
       <c r="G39" t="s">
-        <v>724</v>
+        <v>723</v>
       </c>
     </row>
     <row r="40" spans="1:7" x14ac:dyDescent="0.25">
@@ -3482,7 +3548,7 @@
         <v>662</v>
       </c>
       <c r="G40" t="s">
-        <v>725</v>
+        <v>724</v>
       </c>
     </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.25">
@@ -3502,7 +3568,7 @@
         <v>663</v>
       </c>
       <c r="G41" t="s">
-        <v>725</v>
+        <v>724</v>
       </c>
     </row>
     <row r="42" spans="1:7" x14ac:dyDescent="0.25">
@@ -3522,7 +3588,7 @@
         <v>664</v>
       </c>
       <c r="G42" t="s">
-        <v>725</v>
+        <v>724</v>
       </c>
     </row>
     <row r="43" spans="1:7" x14ac:dyDescent="0.25">
@@ -3542,7 +3608,7 @@
         <v>665</v>
       </c>
       <c r="G43" t="s">
-        <v>725</v>
+        <v>724</v>
       </c>
     </row>
     <row r="44" spans="1:7" x14ac:dyDescent="0.25">
@@ -3562,7 +3628,7 @@
         <v>666</v>
       </c>
       <c r="G44" t="s">
-        <v>725</v>
+        <v>724</v>
       </c>
     </row>
     <row r="45" spans="1:7" x14ac:dyDescent="0.25">
@@ -3582,7 +3648,7 @@
         <v>667</v>
       </c>
       <c r="G45" t="s">
-        <v>726</v>
+        <v>725</v>
       </c>
     </row>
     <row r="46" spans="1:7" x14ac:dyDescent="0.25">
@@ -3605,7 +3671,7 @@
         <v>668</v>
       </c>
       <c r="G46" t="s">
-        <v>726</v>
+        <v>725</v>
       </c>
     </row>
     <row r="47" spans="1:7" x14ac:dyDescent="0.25">
@@ -3625,7 +3691,7 @@
         <v>669</v>
       </c>
       <c r="G47" t="s">
-        <v>726</v>
+        <v>725</v>
       </c>
     </row>
     <row r="48" spans="1:7" x14ac:dyDescent="0.25">
@@ -3639,7 +3705,7 @@
         <v>93</v>
       </c>
       <c r="G48" t="s">
-        <v>727</v>
+        <v>726</v>
       </c>
     </row>
     <row r="49" spans="1:7" x14ac:dyDescent="0.25">
@@ -3653,7 +3719,7 @@
         <v>95</v>
       </c>
       <c r="G49" t="s">
-        <v>727</v>
+        <v>726</v>
       </c>
     </row>
     <row r="50" spans="1:7" x14ac:dyDescent="0.25">
@@ -3667,7 +3733,7 @@
         <v>97</v>
       </c>
       <c r="G50" t="s">
-        <v>727</v>
+        <v>726</v>
       </c>
     </row>
     <row r="51" spans="1:7" x14ac:dyDescent="0.25">
@@ -3681,7 +3747,7 @@
         <v>99</v>
       </c>
       <c r="G51" t="s">
-        <v>727</v>
+        <v>726</v>
       </c>
     </row>
     <row r="52" spans="1:7" x14ac:dyDescent="0.25">
@@ -3695,7 +3761,7 @@
         <v>101</v>
       </c>
       <c r="G52" t="s">
-        <v>727</v>
+        <v>726</v>
       </c>
     </row>
     <row r="53" spans="1:7" x14ac:dyDescent="0.25">
@@ -3709,7 +3775,7 @@
         <v>103</v>
       </c>
       <c r="G53" t="s">
-        <v>728</v>
+        <v>727</v>
       </c>
     </row>
     <row r="54" spans="1:7" x14ac:dyDescent="0.25">
@@ -3726,7 +3792,7 @@
         <v>1</v>
       </c>
       <c r="G54" t="s">
-        <v>728</v>
+        <v>727</v>
       </c>
     </row>
     <row r="55" spans="1:7" x14ac:dyDescent="0.25">
@@ -3743,7 +3809,7 @@
         <v>1</v>
       </c>
       <c r="G55" t="s">
-        <v>728</v>
+        <v>727</v>
       </c>
     </row>
     <row r="56" spans="1:7" x14ac:dyDescent="0.25">
@@ -3757,7 +3823,7 @@
         <v>109</v>
       </c>
       <c r="G56" t="s">
-        <v>728</v>
+        <v>727</v>
       </c>
     </row>
     <row r="57" spans="1:7" x14ac:dyDescent="0.25">
@@ -3771,7 +3837,7 @@
         <v>111</v>
       </c>
       <c r="G57" t="s">
-        <v>728</v>
+        <v>727</v>
       </c>
     </row>
     <row r="58" spans="1:7" x14ac:dyDescent="0.25">
@@ -3785,7 +3851,7 @@
         <v>113</v>
       </c>
       <c r="G58" t="s">
-        <v>729</v>
+        <v>728</v>
       </c>
     </row>
     <row r="59" spans="1:7" x14ac:dyDescent="0.25">
@@ -3802,7 +3868,7 @@
         <v>1</v>
       </c>
       <c r="G59" t="s">
-        <v>729</v>
+        <v>728</v>
       </c>
     </row>
     <row r="60" spans="1:7" x14ac:dyDescent="0.25">
@@ -3819,7 +3885,7 @@
         <v>1</v>
       </c>
       <c r="G60" t="s">
-        <v>729</v>
+        <v>728</v>
       </c>
     </row>
     <row r="61" spans="1:7" x14ac:dyDescent="0.25">
@@ -3833,7 +3899,7 @@
         <v>119</v>
       </c>
       <c r="G61" t="s">
-        <v>729</v>
+        <v>728</v>
       </c>
     </row>
     <row r="62" spans="1:7" x14ac:dyDescent="0.25">
@@ -3847,7 +3913,7 @@
         <v>121</v>
       </c>
       <c r="G62" t="s">
-        <v>729</v>
+        <v>728</v>
       </c>
     </row>
     <row r="63" spans="1:7" x14ac:dyDescent="0.25">
@@ -3861,7 +3927,7 @@
         <v>123</v>
       </c>
       <c r="G63" t="s">
-        <v>730</v>
+        <v>729</v>
       </c>
     </row>
     <row r="64" spans="1:7" x14ac:dyDescent="0.25">
@@ -3875,7 +3941,7 @@
         <v>125</v>
       </c>
       <c r="G64" t="s">
-        <v>730</v>
+        <v>729</v>
       </c>
     </row>
     <row r="65" spans="1:7" x14ac:dyDescent="0.25">
@@ -3889,7 +3955,7 @@
         <v>127</v>
       </c>
       <c r="G65" t="s">
-        <v>730</v>
+        <v>729</v>
       </c>
     </row>
     <row r="66" spans="1:7" x14ac:dyDescent="0.25">
@@ -3903,7 +3969,7 @@
         <v>129</v>
       </c>
       <c r="G66" t="s">
-        <v>730</v>
+        <v>729</v>
       </c>
     </row>
     <row r="67" spans="1:7" x14ac:dyDescent="0.25">
@@ -3917,7 +3983,7 @@
         <v>131</v>
       </c>
       <c r="G67" t="s">
-        <v>730</v>
+        <v>729</v>
       </c>
     </row>
     <row r="68" spans="1:7" x14ac:dyDescent="0.25">
@@ -3931,7 +3997,7 @@
         <v>133</v>
       </c>
       <c r="G68" t="s">
-        <v>741</v>
+        <v>740</v>
       </c>
     </row>
     <row r="69" spans="1:7" x14ac:dyDescent="0.25">
@@ -3945,7 +4011,7 @@
         <v>135</v>
       </c>
       <c r="G69" t="s">
-        <v>741</v>
+        <v>740</v>
       </c>
     </row>
     <row r="70" spans="1:7" x14ac:dyDescent="0.25">
@@ -3959,7 +4025,7 @@
         <v>137</v>
       </c>
       <c r="G70" t="s">
-        <v>741</v>
+        <v>740</v>
       </c>
     </row>
     <row r="71" spans="1:7" x14ac:dyDescent="0.25">
@@ -3973,7 +4039,7 @@
         <v>139</v>
       </c>
       <c r="G71" t="s">
-        <v>741</v>
+        <v>740</v>
       </c>
     </row>
     <row r="72" spans="1:7" x14ac:dyDescent="0.25">
@@ -3987,7 +4053,7 @@
         <v>141</v>
       </c>
       <c r="G72" t="s">
-        <v>741</v>
+        <v>740</v>
       </c>
     </row>
     <row r="73" spans="1:7" x14ac:dyDescent="0.25">
@@ -4001,7 +4067,7 @@
         <v>143</v>
       </c>
       <c r="G73" t="s">
-        <v>732</v>
+        <v>731</v>
       </c>
     </row>
     <row r="74" spans="1:7" x14ac:dyDescent="0.25">
@@ -4015,7 +4081,7 @@
         <v>145</v>
       </c>
       <c r="G74" t="s">
-        <v>732</v>
+        <v>731</v>
       </c>
     </row>
     <row r="75" spans="1:7" x14ac:dyDescent="0.25">
@@ -4029,7 +4095,7 @@
         <v>147</v>
       </c>
       <c r="G75" t="s">
-        <v>732</v>
+        <v>731</v>
       </c>
     </row>
     <row r="76" spans="1:7" x14ac:dyDescent="0.25">
@@ -4043,7 +4109,7 @@
         <v>149</v>
       </c>
       <c r="G76" t="s">
-        <v>733</v>
+        <v>732</v>
       </c>
     </row>
     <row r="77" spans="1:7" x14ac:dyDescent="0.25">
@@ -4057,7 +4123,7 @@
         <v>151</v>
       </c>
       <c r="G77" t="s">
-        <v>733</v>
+        <v>732</v>
       </c>
     </row>
     <row r="78" spans="1:7" x14ac:dyDescent="0.25">
@@ -4071,7 +4137,7 @@
         <v>153</v>
       </c>
       <c r="G78" t="s">
-        <v>733</v>
+        <v>732</v>
       </c>
     </row>
     <row r="79" spans="1:7" x14ac:dyDescent="0.25">
@@ -4085,7 +4151,7 @@
         <v>155</v>
       </c>
       <c r="G79" t="s">
-        <v>731</v>
+        <v>730</v>
       </c>
     </row>
     <row r="80" spans="1:7" x14ac:dyDescent="0.25">
@@ -4099,7 +4165,7 @@
         <v>157</v>
       </c>
       <c r="G80" t="s">
-        <v>731</v>
+        <v>730</v>
       </c>
     </row>
     <row r="81" spans="1:7" x14ac:dyDescent="0.25">
@@ -4113,7 +4179,7 @@
         <v>159</v>
       </c>
       <c r="G81" t="s">
-        <v>731</v>
+        <v>730</v>
       </c>
     </row>
     <row r="82" spans="1:7" x14ac:dyDescent="0.25">
@@ -4127,7 +4193,7 @@
         <v>161</v>
       </c>
       <c r="G82" t="s">
-        <v>734</v>
+        <v>733</v>
       </c>
     </row>
     <row r="83" spans="1:7" x14ac:dyDescent="0.25">
@@ -4141,7 +4207,7 @@
         <v>163</v>
       </c>
       <c r="G83" t="s">
-        <v>734</v>
+        <v>733</v>
       </c>
     </row>
     <row r="84" spans="1:7" x14ac:dyDescent="0.25">
@@ -4155,7 +4221,7 @@
         <v>165</v>
       </c>
       <c r="G84" t="s">
-        <v>734</v>
+        <v>733</v>
       </c>
     </row>
     <row r="85" spans="1:7" x14ac:dyDescent="0.25">
@@ -4169,7 +4235,7 @@
         <v>167</v>
       </c>
       <c r="G85" t="s">
-        <v>735</v>
+        <v>734</v>
       </c>
     </row>
     <row r="86" spans="1:7" x14ac:dyDescent="0.25">
@@ -4183,7 +4249,7 @@
         <v>169</v>
       </c>
       <c r="G86" t="s">
-        <v>735</v>
+        <v>734</v>
       </c>
     </row>
     <row r="87" spans="1:7" x14ac:dyDescent="0.25">
@@ -4197,7 +4263,7 @@
         <v>171</v>
       </c>
       <c r="G87" t="s">
-        <v>735</v>
+        <v>734</v>
       </c>
     </row>
     <row r="88" spans="1:7" x14ac:dyDescent="0.25">
@@ -4211,7 +4277,7 @@
         <v>173</v>
       </c>
       <c r="G88" t="s">
-        <v>736</v>
+        <v>735</v>
       </c>
     </row>
     <row r="89" spans="1:7" x14ac:dyDescent="0.25">
@@ -4225,7 +4291,7 @@
         <v>175</v>
       </c>
       <c r="G89" t="s">
-        <v>736</v>
+        <v>735</v>
       </c>
     </row>
     <row r="90" spans="1:7" x14ac:dyDescent="0.25">
@@ -4239,7 +4305,7 @@
         <v>177</v>
       </c>
       <c r="G90" t="s">
-        <v>736</v>
+        <v>735</v>
       </c>
     </row>
     <row r="91" spans="1:7" x14ac:dyDescent="0.25">
@@ -4253,7 +4319,7 @@
         <v>179</v>
       </c>
       <c r="G91" t="s">
-        <v>737</v>
+        <v>736</v>
       </c>
     </row>
     <row r="92" spans="1:7" x14ac:dyDescent="0.25">
@@ -4270,7 +4336,7 @@
         <v>1</v>
       </c>
       <c r="G92" t="s">
-        <v>737</v>
+        <v>736</v>
       </c>
     </row>
     <row r="93" spans="1:7" x14ac:dyDescent="0.25">
@@ -4284,7 +4350,7 @@
         <v>183</v>
       </c>
       <c r="G93" t="s">
-        <v>737</v>
+        <v>736</v>
       </c>
     </row>
     <row r="94" spans="1:7" x14ac:dyDescent="0.25">
@@ -4298,7 +4364,7 @@
         <v>185</v>
       </c>
       <c r="G94" t="s">
-        <v>738</v>
+        <v>737</v>
       </c>
     </row>
     <row r="95" spans="1:7" x14ac:dyDescent="0.25">
@@ -4312,7 +4378,7 @@
         <v>187</v>
       </c>
       <c r="G95" t="s">
-        <v>738</v>
+        <v>737</v>
       </c>
     </row>
     <row r="96" spans="1:7" x14ac:dyDescent="0.25">
@@ -4326,7 +4392,7 @@
         <v>189</v>
       </c>
       <c r="G96" t="s">
-        <v>738</v>
+        <v>737</v>
       </c>
     </row>
     <row r="97" spans="1:7" x14ac:dyDescent="0.25">
@@ -4343,7 +4409,7 @@
         <v>1</v>
       </c>
       <c r="G97" t="s">
-        <v>739</v>
+        <v>738</v>
       </c>
     </row>
     <row r="98" spans="1:7" x14ac:dyDescent="0.25">
@@ -4360,7 +4426,7 @@
         <v>1</v>
       </c>
       <c r="G98" t="s">
-        <v>739</v>
+        <v>738</v>
       </c>
     </row>
     <row r="99" spans="1:7" x14ac:dyDescent="0.25">
@@ -4377,7 +4443,7 @@
         <v>1</v>
       </c>
       <c r="G99" t="s">
-        <v>739</v>
+        <v>738</v>
       </c>
     </row>
     <row r="100" spans="1:7" x14ac:dyDescent="0.25">
@@ -4394,7 +4460,7 @@
         <v>1</v>
       </c>
       <c r="G100" t="s">
-        <v>740</v>
+        <v>739</v>
       </c>
     </row>
     <row r="101" spans="1:7" x14ac:dyDescent="0.25">
@@ -4411,7 +4477,7 @@
         <v>1</v>
       </c>
       <c r="G101" t="s">
-        <v>740</v>
+        <v>739</v>
       </c>
     </row>
     <row r="102" spans="1:7" x14ac:dyDescent="0.25">
@@ -4428,7 +4494,7 @@
         <v>1</v>
       </c>
       <c r="G102" t="s">
-        <v>740</v>
+        <v>739</v>
       </c>
     </row>
     <row r="103" spans="1:7" x14ac:dyDescent="0.25">
@@ -4442,7 +4508,7 @@
         <v>203</v>
       </c>
       <c r="G103" t="s">
-        <v>742</v>
+        <v>741</v>
       </c>
     </row>
     <row r="104" spans="1:7" x14ac:dyDescent="0.25">
@@ -4456,7 +4522,7 @@
         <v>205</v>
       </c>
       <c r="G104" t="s">
-        <v>742</v>
+        <v>741</v>
       </c>
     </row>
     <row r="105" spans="1:7" x14ac:dyDescent="0.25">
@@ -4470,7 +4536,7 @@
         <v>207</v>
       </c>
       <c r="G105" t="s">
-        <v>742</v>
+        <v>741</v>
       </c>
     </row>
     <row r="106" spans="1:7" x14ac:dyDescent="0.25">
@@ -4484,7 +4550,7 @@
         <v>209</v>
       </c>
       <c r="G106" t="s">
-        <v>743</v>
+        <v>742</v>
       </c>
     </row>
     <row r="107" spans="1:7" x14ac:dyDescent="0.25">
@@ -4498,7 +4564,7 @@
         <v>211</v>
       </c>
       <c r="G107" t="s">
-        <v>743</v>
+        <v>742</v>
       </c>
     </row>
     <row r="108" spans="1:7" x14ac:dyDescent="0.25">
@@ -4512,7 +4578,7 @@
         <v>213</v>
       </c>
       <c r="G108" t="s">
-        <v>743</v>
+        <v>742</v>
       </c>
     </row>
     <row r="109" spans="1:7" x14ac:dyDescent="0.25">
@@ -4532,7 +4598,7 @@
         <v>670</v>
       </c>
       <c r="G109" t="s">
-        <v>744</v>
+        <v>743</v>
       </c>
     </row>
     <row r="110" spans="1:7" x14ac:dyDescent="0.25">
@@ -4552,7 +4618,7 @@
         <v>671</v>
       </c>
       <c r="G110" t="s">
-        <v>744</v>
+        <v>743</v>
       </c>
     </row>
     <row r="111" spans="1:7" x14ac:dyDescent="0.25">
@@ -4572,7 +4638,7 @@
         <v>672</v>
       </c>
       <c r="G111" t="s">
-        <v>744</v>
+        <v>743</v>
       </c>
     </row>
     <row r="112" spans="1:7" x14ac:dyDescent="0.25">
@@ -4592,7 +4658,7 @@
         <v>673</v>
       </c>
       <c r="G112" t="s">
-        <v>744</v>
+        <v>743</v>
       </c>
     </row>
     <row r="113" spans="1:7" x14ac:dyDescent="0.25">
@@ -4612,7 +4678,7 @@
         <v>674</v>
       </c>
       <c r="G113" t="s">
-        <v>744</v>
+        <v>743</v>
       </c>
     </row>
     <row r="114" spans="1:7" x14ac:dyDescent="0.25">
@@ -4632,7 +4698,7 @@
         <v>675</v>
       </c>
       <c r="G114" t="s">
-        <v>745</v>
+        <v>744</v>
       </c>
     </row>
     <row r="115" spans="1:7" x14ac:dyDescent="0.25">
@@ -4652,7 +4718,7 @@
         <v>676</v>
       </c>
       <c r="G115" t="s">
-        <v>745</v>
+        <v>744</v>
       </c>
     </row>
     <row r="116" spans="1:7" x14ac:dyDescent="0.25">
@@ -4672,7 +4738,7 @@
         <v>677</v>
       </c>
       <c r="G116" t="s">
-        <v>745</v>
+        <v>744</v>
       </c>
     </row>
     <row r="117" spans="1:7" x14ac:dyDescent="0.25">
@@ -4692,7 +4758,7 @@
         <v>678</v>
       </c>
       <c r="G117" t="s">
-        <v>745</v>
+        <v>744</v>
       </c>
     </row>
     <row r="118" spans="1:7" x14ac:dyDescent="0.25">
@@ -4712,7 +4778,7 @@
         <v>679</v>
       </c>
       <c r="G118" t="s">
-        <v>745</v>
+        <v>744</v>
       </c>
     </row>
     <row r="119" spans="1:7" x14ac:dyDescent="0.25">
@@ -4732,7 +4798,7 @@
         <v>680</v>
       </c>
       <c r="G119" t="s">
-        <v>746</v>
+        <v>745</v>
       </c>
     </row>
     <row r="120" spans="1:7" x14ac:dyDescent="0.25">
@@ -4752,7 +4818,7 @@
         <v>681</v>
       </c>
       <c r="G120" t="s">
-        <v>746</v>
+        <v>781</v>
       </c>
     </row>
     <row r="121" spans="1:7" x14ac:dyDescent="0.25">
@@ -4772,7 +4838,7 @@
         <v>682</v>
       </c>
       <c r="G121" t="s">
-        <v>746</v>
+        <v>745</v>
       </c>
     </row>
     <row r="122" spans="1:7" x14ac:dyDescent="0.25">
@@ -4792,7 +4858,7 @@
         <v>683</v>
       </c>
       <c r="G122" t="s">
-        <v>746</v>
+        <v>745</v>
       </c>
     </row>
     <row r="123" spans="1:7" x14ac:dyDescent="0.25">
@@ -4812,7 +4878,7 @@
         <v>684</v>
       </c>
       <c r="G123" t="s">
-        <v>746</v>
+        <v>745</v>
       </c>
     </row>
     <row r="124" spans="1:7" x14ac:dyDescent="0.25">
@@ -4832,7 +4898,7 @@
         <v>685</v>
       </c>
       <c r="G124" t="s">
-        <v>747</v>
+        <v>746</v>
       </c>
     </row>
     <row r="125" spans="1:7" x14ac:dyDescent="0.25">
@@ -4852,7 +4918,7 @@
         <v>686</v>
       </c>
       <c r="G125" t="s">
-        <v>747</v>
+        <v>779</v>
       </c>
     </row>
     <row r="126" spans="1:7" x14ac:dyDescent="0.25">
@@ -4872,7 +4938,7 @@
         <v>687</v>
       </c>
       <c r="G126" t="s">
-        <v>747</v>
+        <v>780</v>
       </c>
     </row>
     <row r="127" spans="1:7" x14ac:dyDescent="0.25">
@@ -4892,7 +4958,7 @@
         <v>688</v>
       </c>
       <c r="G127" t="s">
-        <v>747</v>
+        <v>746</v>
       </c>
     </row>
     <row r="128" spans="1:7" x14ac:dyDescent="0.25">
@@ -4912,7 +4978,7 @@
         <v>689</v>
       </c>
       <c r="G128" t="s">
-        <v>747</v>
+        <v>746</v>
       </c>
     </row>
     <row r="129" spans="1:7" x14ac:dyDescent="0.25">
@@ -4932,7 +4998,7 @@
         <v>690</v>
       </c>
       <c r="G129" t="s">
-        <v>748</v>
+        <v>747</v>
       </c>
     </row>
     <row r="130" spans="1:7" x14ac:dyDescent="0.25">
@@ -4952,7 +5018,7 @@
         <v>691</v>
       </c>
       <c r="G130" t="s">
-        <v>748</v>
+        <v>747</v>
       </c>
     </row>
     <row r="131" spans="1:7" x14ac:dyDescent="0.25">
@@ -4972,7 +5038,7 @@
         <v>692</v>
       </c>
       <c r="G131" t="s">
-        <v>748</v>
+        <v>747</v>
       </c>
     </row>
     <row r="132" spans="1:7" x14ac:dyDescent="0.25">
@@ -4992,7 +5058,7 @@
         <v>693</v>
       </c>
       <c r="G132" t="s">
-        <v>748</v>
+        <v>747</v>
       </c>
     </row>
     <row r="133" spans="1:7" x14ac:dyDescent="0.25">
@@ -5012,7 +5078,7 @@
         <v>694</v>
       </c>
       <c r="G133" t="s">
-        <v>748</v>
+        <v>747</v>
       </c>
     </row>
     <row r="134" spans="1:7" x14ac:dyDescent="0.25">
@@ -5032,7 +5098,7 @@
         <v>695</v>
       </c>
       <c r="G134" t="s">
-        <v>749</v>
+        <v>748</v>
       </c>
     </row>
     <row r="135" spans="1:7" x14ac:dyDescent="0.25">
@@ -5052,7 +5118,7 @@
         <v>696</v>
       </c>
       <c r="G135" t="s">
-        <v>749</v>
+        <v>748</v>
       </c>
     </row>
     <row r="136" spans="1:7" x14ac:dyDescent="0.25">
@@ -5072,7 +5138,7 @@
         <v>697</v>
       </c>
       <c r="G136" t="s">
-        <v>749</v>
+        <v>770</v>
       </c>
     </row>
     <row r="137" spans="1:7" x14ac:dyDescent="0.25">
@@ -5092,7 +5158,7 @@
         <v>698</v>
       </c>
       <c r="G137" t="s">
-        <v>749</v>
+        <v>748</v>
       </c>
     </row>
     <row r="138" spans="1:7" x14ac:dyDescent="0.25">
@@ -5112,7 +5178,7 @@
         <v>699</v>
       </c>
       <c r="G138" t="s">
-        <v>749</v>
+        <v>748</v>
       </c>
     </row>
     <row r="139" spans="1:7" x14ac:dyDescent="0.25">
@@ -5132,7 +5198,7 @@
         <v>700</v>
       </c>
       <c r="G139" t="s">
-        <v>750</v>
+        <v>749</v>
       </c>
     </row>
     <row r="140" spans="1:7" x14ac:dyDescent="0.25">
@@ -5152,7 +5218,7 @@
         <v>701</v>
       </c>
       <c r="G140" t="s">
-        <v>750</v>
+        <v>749</v>
       </c>
     </row>
     <row r="141" spans="1:7" x14ac:dyDescent="0.25">
@@ -5172,7 +5238,7 @@
         <v>702</v>
       </c>
       <c r="G141" t="s">
-        <v>750</v>
+        <v>749</v>
       </c>
     </row>
     <row r="142" spans="1:7" x14ac:dyDescent="0.25">
@@ -5192,7 +5258,7 @@
         <v>703</v>
       </c>
       <c r="G142" t="s">
-        <v>750</v>
+        <v>749</v>
       </c>
     </row>
     <row r="143" spans="1:7" x14ac:dyDescent="0.25">
@@ -5212,7 +5278,7 @@
         <v>704</v>
       </c>
       <c r="G143" t="s">
-        <v>750</v>
+        <v>749</v>
       </c>
     </row>
     <row r="144" spans="1:7" x14ac:dyDescent="0.25">
@@ -5232,7 +5298,7 @@
         <v>705</v>
       </c>
       <c r="G144" t="s">
-        <v>751</v>
+        <v>750</v>
       </c>
     </row>
     <row r="145" spans="1:7" x14ac:dyDescent="0.25">
@@ -5252,7 +5318,7 @@
         <v>706</v>
       </c>
       <c r="G145" t="s">
-        <v>751</v>
+        <v>750</v>
       </c>
     </row>
     <row r="146" spans="1:7" x14ac:dyDescent="0.25">
@@ -5272,7 +5338,7 @@
         <v>707</v>
       </c>
       <c r="G146" t="s">
-        <v>751</v>
+        <v>750</v>
       </c>
     </row>
     <row r="147" spans="1:7" x14ac:dyDescent="0.25">
@@ -5292,7 +5358,7 @@
         <v>708</v>
       </c>
       <c r="G147" t="s">
-        <v>752</v>
+        <v>751</v>
       </c>
     </row>
     <row r="148" spans="1:7" x14ac:dyDescent="0.25">
@@ -5312,7 +5378,7 @@
         <v>709</v>
       </c>
       <c r="G148" t="s">
-        <v>752</v>
+        <v>751</v>
       </c>
     </row>
     <row r="149" spans="1:7" x14ac:dyDescent="0.25">
@@ -5332,7 +5398,7 @@
         <v>710</v>
       </c>
       <c r="G149" t="s">
-        <v>752</v>
+        <v>751</v>
       </c>
     </row>
     <row r="150" spans="1:7" x14ac:dyDescent="0.25">
@@ -5352,7 +5418,7 @@
         <v>711</v>
       </c>
       <c r="G150" t="s">
-        <v>752</v>
+        <v>751</v>
       </c>
     </row>
     <row r="151" spans="1:7" x14ac:dyDescent="0.25">
@@ -5372,7 +5438,7 @@
         <v>712</v>
       </c>
       <c r="G151" t="s">
-        <v>752</v>
+        <v>751</v>
       </c>
     </row>
     <row r="152" spans="1:7" x14ac:dyDescent="0.25">
@@ -5392,7 +5458,7 @@
         <v>713</v>
       </c>
       <c r="G152" t="s">
-        <v>753</v>
+        <v>752</v>
       </c>
     </row>
     <row r="153" spans="1:7" x14ac:dyDescent="0.25">
@@ -5409,7 +5475,7 @@
         <v>1</v>
       </c>
       <c r="G153" t="s">
-        <v>753</v>
+        <v>752</v>
       </c>
     </row>
     <row r="154" spans="1:7" x14ac:dyDescent="0.25">
@@ -5429,7 +5495,7 @@
         <v>714</v>
       </c>
       <c r="G154" t="s">
-        <v>753</v>
+        <v>752</v>
       </c>
     </row>
     <row r="155" spans="1:7" x14ac:dyDescent="0.25">
@@ -5443,7 +5509,7 @@
         <v>93</v>
       </c>
       <c r="G155" t="s">
-        <v>754</v>
+        <v>753</v>
       </c>
     </row>
     <row r="156" spans="1:7" x14ac:dyDescent="0.25">
@@ -5457,7 +5523,7 @@
         <v>95</v>
       </c>
       <c r="G156" t="s">
-        <v>754</v>
+        <v>753</v>
       </c>
     </row>
     <row r="157" spans="1:7" x14ac:dyDescent="0.25">
@@ -5471,7 +5537,7 @@
         <v>97</v>
       </c>
       <c r="G157" t="s">
-        <v>754</v>
+        <v>753</v>
       </c>
     </row>
     <row r="158" spans="1:7" x14ac:dyDescent="0.25">
@@ -5485,7 +5551,7 @@
         <v>99</v>
       </c>
       <c r="G158" t="s">
-        <v>754</v>
+        <v>753</v>
       </c>
     </row>
     <row r="159" spans="1:7" x14ac:dyDescent="0.25">
@@ -5499,7 +5565,7 @@
         <v>101</v>
       </c>
       <c r="G159" t="s">
-        <v>754</v>
+        <v>753</v>
       </c>
     </row>
     <row r="160" spans="1:7" x14ac:dyDescent="0.25">
@@ -5513,7 +5579,7 @@
         <v>103</v>
       </c>
       <c r="G160" t="s">
-        <v>755</v>
+        <v>754</v>
       </c>
     </row>
     <row r="161" spans="1:7" x14ac:dyDescent="0.25">
@@ -5530,7 +5596,7 @@
         <v>1</v>
       </c>
       <c r="G161" t="s">
-        <v>755</v>
+        <v>791</v>
       </c>
     </row>
     <row r="162" spans="1:7" x14ac:dyDescent="0.25">
@@ -5547,7 +5613,7 @@
         <v>1</v>
       </c>
       <c r="G162" t="s">
-        <v>755</v>
+        <v>754</v>
       </c>
     </row>
     <row r="163" spans="1:7" x14ac:dyDescent="0.25">
@@ -5561,7 +5627,7 @@
         <v>109</v>
       </c>
       <c r="G163" t="s">
-        <v>755</v>
+        <v>754</v>
       </c>
     </row>
     <row r="164" spans="1:7" x14ac:dyDescent="0.25">
@@ -5575,7 +5641,7 @@
         <v>111</v>
       </c>
       <c r="G164" t="s">
-        <v>755</v>
+        <v>754</v>
       </c>
     </row>
     <row r="165" spans="1:7" x14ac:dyDescent="0.25">
@@ -5589,7 +5655,7 @@
         <v>113</v>
       </c>
       <c r="G165" t="s">
-        <v>756</v>
+        <v>755</v>
       </c>
     </row>
     <row r="166" spans="1:7" x14ac:dyDescent="0.25">
@@ -5606,7 +5672,7 @@
         <v>1</v>
       </c>
       <c r="G166" t="s">
-        <v>756</v>
+        <v>755</v>
       </c>
     </row>
     <row r="167" spans="1:7" x14ac:dyDescent="0.25">
@@ -5623,7 +5689,7 @@
         <v>1</v>
       </c>
       <c r="G167" t="s">
-        <v>756</v>
+        <v>755</v>
       </c>
     </row>
     <row r="168" spans="1:7" x14ac:dyDescent="0.25">
@@ -5637,7 +5703,7 @@
         <v>119</v>
       </c>
       <c r="G168" t="s">
-        <v>756</v>
+        <v>755</v>
       </c>
     </row>
     <row r="169" spans="1:7" x14ac:dyDescent="0.25">
@@ -5651,7 +5717,7 @@
         <v>121</v>
       </c>
       <c r="G169" t="s">
-        <v>756</v>
+        <v>755</v>
       </c>
     </row>
     <row r="170" spans="1:7" x14ac:dyDescent="0.25">
@@ -5665,7 +5731,7 @@
         <v>123</v>
       </c>
       <c r="G170" t="s">
-        <v>757</v>
+        <v>756</v>
       </c>
     </row>
     <row r="171" spans="1:7" x14ac:dyDescent="0.25">
@@ -5679,7 +5745,7 @@
         <v>125</v>
       </c>
       <c r="G171" t="s">
-        <v>757</v>
+        <v>756</v>
       </c>
     </row>
     <row r="172" spans="1:7" x14ac:dyDescent="0.25">
@@ -5693,7 +5759,7 @@
         <v>127</v>
       </c>
       <c r="G172" t="s">
-        <v>757</v>
+        <v>756</v>
       </c>
     </row>
     <row r="173" spans="1:7" x14ac:dyDescent="0.25">
@@ -5707,7 +5773,7 @@
         <v>129</v>
       </c>
       <c r="G173" t="s">
-        <v>757</v>
+        <v>756</v>
       </c>
     </row>
     <row r="174" spans="1:7" x14ac:dyDescent="0.25">
@@ -5721,7 +5787,7 @@
         <v>131</v>
       </c>
       <c r="G174" t="s">
-        <v>757</v>
+        <v>756</v>
       </c>
     </row>
     <row r="175" spans="1:7" x14ac:dyDescent="0.25">
@@ -5735,7 +5801,7 @@
         <v>133</v>
       </c>
       <c r="G175" t="s">
-        <v>758</v>
+        <v>757</v>
       </c>
     </row>
     <row r="176" spans="1:7" x14ac:dyDescent="0.25">
@@ -5749,7 +5815,7 @@
         <v>135</v>
       </c>
       <c r="G176" t="s">
-        <v>758</v>
+        <v>757</v>
       </c>
     </row>
     <row r="177" spans="1:7" x14ac:dyDescent="0.25">
@@ -5763,7 +5829,7 @@
         <v>137</v>
       </c>
       <c r="G177" t="s">
-        <v>758</v>
+        <v>757</v>
       </c>
     </row>
     <row r="178" spans="1:7" x14ac:dyDescent="0.25">
@@ -5777,7 +5843,7 @@
         <v>139</v>
       </c>
       <c r="G178" t="s">
-        <v>758</v>
+        <v>757</v>
       </c>
     </row>
     <row r="179" spans="1:7" x14ac:dyDescent="0.25">
@@ -5791,7 +5857,7 @@
         <v>141</v>
       </c>
       <c r="G179" t="s">
-        <v>758</v>
+        <v>757</v>
       </c>
     </row>
     <row r="180" spans="1:7" x14ac:dyDescent="0.25">
@@ -5805,7 +5871,7 @@
         <v>143</v>
       </c>
       <c r="G180" t="s">
-        <v>759</v>
+        <v>758</v>
       </c>
     </row>
     <row r="181" spans="1:7" x14ac:dyDescent="0.25">
@@ -5819,7 +5885,7 @@
         <v>145</v>
       </c>
       <c r="G181" t="s">
-        <v>759</v>
+        <v>758</v>
       </c>
     </row>
     <row r="182" spans="1:7" x14ac:dyDescent="0.25">
@@ -5833,7 +5899,7 @@
         <v>147</v>
       </c>
       <c r="G182" t="s">
-        <v>759</v>
+        <v>758</v>
       </c>
     </row>
     <row r="183" spans="1:7" x14ac:dyDescent="0.25">
@@ -5847,7 +5913,7 @@
         <v>149</v>
       </c>
       <c r="G183" t="s">
-        <v>760</v>
+        <v>759</v>
       </c>
     </row>
     <row r="184" spans="1:7" x14ac:dyDescent="0.25">
@@ -5861,7 +5927,7 @@
         <v>151</v>
       </c>
       <c r="G184" t="s">
-        <v>760</v>
+        <v>759</v>
       </c>
     </row>
     <row r="185" spans="1:7" x14ac:dyDescent="0.25">
@@ -5875,7 +5941,7 @@
         <v>153</v>
       </c>
       <c r="G185" t="s">
-        <v>760</v>
+        <v>759</v>
       </c>
     </row>
     <row r="186" spans="1:7" x14ac:dyDescent="0.25">
@@ -5889,7 +5955,7 @@
         <v>155</v>
       </c>
       <c r="G186" t="s">
-        <v>761</v>
+        <v>760</v>
       </c>
     </row>
     <row r="187" spans="1:7" x14ac:dyDescent="0.25">
@@ -5903,7 +5969,7 @@
         <v>157</v>
       </c>
       <c r="G187" t="s">
-        <v>761</v>
+        <v>760</v>
       </c>
     </row>
     <row r="188" spans="1:7" x14ac:dyDescent="0.25">
@@ -5917,7 +5983,7 @@
         <v>159</v>
       </c>
       <c r="G188" t="s">
-        <v>761</v>
+        <v>760</v>
       </c>
     </row>
     <row r="189" spans="1:7" x14ac:dyDescent="0.25">
@@ -5931,7 +5997,7 @@
         <v>161</v>
       </c>
       <c r="G189" t="s">
-        <v>762</v>
+        <v>761</v>
       </c>
     </row>
     <row r="190" spans="1:7" x14ac:dyDescent="0.25">
@@ -5945,7 +6011,7 @@
         <v>163</v>
       </c>
       <c r="G190" t="s">
-        <v>762</v>
+        <v>761</v>
       </c>
     </row>
     <row r="191" spans="1:7" x14ac:dyDescent="0.25">
@@ -5959,7 +6025,7 @@
         <v>165</v>
       </c>
       <c r="G191" t="s">
-        <v>762</v>
+        <v>761</v>
       </c>
     </row>
     <row r="192" spans="1:7" x14ac:dyDescent="0.25">
@@ -5973,7 +6039,7 @@
         <v>167</v>
       </c>
       <c r="G192" t="s">
-        <v>763</v>
+        <v>762</v>
       </c>
     </row>
     <row r="193" spans="1:7" x14ac:dyDescent="0.25">
@@ -5987,7 +6053,7 @@
         <v>169</v>
       </c>
       <c r="G193" t="s">
-        <v>763</v>
+        <v>762</v>
       </c>
     </row>
     <row r="194" spans="1:7" x14ac:dyDescent="0.25">
@@ -6001,7 +6067,7 @@
         <v>171</v>
       </c>
       <c r="G194" t="s">
-        <v>763</v>
+        <v>762</v>
       </c>
     </row>
     <row r="195" spans="1:7" x14ac:dyDescent="0.25">
@@ -6015,7 +6081,7 @@
         <v>173</v>
       </c>
       <c r="G195" t="s">
-        <v>764</v>
+        <v>763</v>
       </c>
     </row>
     <row r="196" spans="1:7" x14ac:dyDescent="0.25">
@@ -6029,7 +6095,7 @@
         <v>175</v>
       </c>
       <c r="G196" t="s">
-        <v>764</v>
+        <v>763</v>
       </c>
     </row>
     <row r="197" spans="1:7" x14ac:dyDescent="0.25">
@@ -6043,7 +6109,7 @@
         <v>177</v>
       </c>
       <c r="G197" t="s">
-        <v>764</v>
+        <v>763</v>
       </c>
     </row>
     <row r="198" spans="1:7" x14ac:dyDescent="0.25">
@@ -6057,7 +6123,7 @@
         <v>179</v>
       </c>
       <c r="G198" t="s">
-        <v>765</v>
+        <v>764</v>
       </c>
     </row>
     <row r="199" spans="1:7" x14ac:dyDescent="0.25">
@@ -6074,7 +6140,7 @@
         <v>1</v>
       </c>
       <c r="G199" t="s">
-        <v>765</v>
+        <v>764</v>
       </c>
     </row>
     <row r="200" spans="1:7" x14ac:dyDescent="0.25">
@@ -6088,7 +6154,7 @@
         <v>183</v>
       </c>
       <c r="G200" t="s">
-        <v>765</v>
+        <v>764</v>
       </c>
     </row>
     <row r="201" spans="1:7" x14ac:dyDescent="0.25">
@@ -6102,7 +6168,7 @@
         <v>185</v>
       </c>
       <c r="G201" t="s">
-        <v>766</v>
+        <v>765</v>
       </c>
     </row>
     <row r="202" spans="1:7" x14ac:dyDescent="0.25">
@@ -6116,7 +6182,7 @@
         <v>187</v>
       </c>
       <c r="G202" t="s">
-        <v>766</v>
+        <v>765</v>
       </c>
     </row>
     <row r="203" spans="1:7" x14ac:dyDescent="0.25">
@@ -6130,7 +6196,7 @@
         <v>189</v>
       </c>
       <c r="G203" t="s">
-        <v>766</v>
+        <v>765</v>
       </c>
     </row>
     <row r="204" spans="1:7" x14ac:dyDescent="0.25">
@@ -6147,7 +6213,7 @@
         <v>1</v>
       </c>
       <c r="G204" t="s">
-        <v>767</v>
+        <v>766</v>
       </c>
     </row>
     <row r="205" spans="1:7" x14ac:dyDescent="0.25">
@@ -6164,7 +6230,7 @@
         <v>1</v>
       </c>
       <c r="G205" t="s">
-        <v>767</v>
+        <v>766</v>
       </c>
     </row>
     <row r="206" spans="1:7" x14ac:dyDescent="0.25">
@@ -6181,7 +6247,7 @@
         <v>1</v>
       </c>
       <c r="G206" t="s">
-        <v>767</v>
+        <v>766</v>
       </c>
     </row>
     <row r="207" spans="1:7" x14ac:dyDescent="0.25">
@@ -6198,7 +6264,7 @@
         <v>1</v>
       </c>
       <c r="G207" t="s">
-        <v>768</v>
+        <v>767</v>
       </c>
     </row>
     <row r="208" spans="1:7" x14ac:dyDescent="0.25">
@@ -6215,7 +6281,7 @@
         <v>1</v>
       </c>
       <c r="G208" t="s">
-        <v>768</v>
+        <v>767</v>
       </c>
     </row>
     <row r="209" spans="1:7" x14ac:dyDescent="0.25">
@@ -6232,7 +6298,7 @@
         <v>1</v>
       </c>
       <c r="G209" t="s">
-        <v>768</v>
+        <v>767</v>
       </c>
     </row>
     <row r="210" spans="1:7" x14ac:dyDescent="0.25">
@@ -6246,7 +6312,7 @@
         <v>203</v>
       </c>
       <c r="G210" t="s">
-        <v>769</v>
+        <v>768</v>
       </c>
     </row>
     <row r="211" spans="1:7" x14ac:dyDescent="0.25">
@@ -6260,7 +6326,7 @@
         <v>205</v>
       </c>
       <c r="G211" t="s">
-        <v>769</v>
+        <v>768</v>
       </c>
     </row>
     <row r="212" spans="1:7" x14ac:dyDescent="0.25">
@@ -6274,7 +6340,7 @@
         <v>207</v>
       </c>
       <c r="G212" t="s">
-        <v>769</v>
+        <v>768</v>
       </c>
     </row>
     <row r="213" spans="1:7" x14ac:dyDescent="0.25">
@@ -6288,7 +6354,7 @@
         <v>209</v>
       </c>
       <c r="G213" t="s">
-        <v>770</v>
+        <v>769</v>
       </c>
     </row>
     <row r="214" spans="1:7" x14ac:dyDescent="0.25">
@@ -6302,7 +6368,7 @@
         <v>211</v>
       </c>
       <c r="G214" t="s">
-        <v>770</v>
+        <v>769</v>
       </c>
     </row>
     <row r="215" spans="1:7" x14ac:dyDescent="0.25">
@@ -6316,7 +6382,7 @@
         <v>213</v>
       </c>
       <c r="G215" t="s">
-        <v>770</v>
+        <v>769</v>
       </c>
     </row>
     <row r="216" spans="1:7" x14ac:dyDescent="0.25">
@@ -6330,7 +6396,7 @@
         <v>1</v>
       </c>
       <c r="G216" t="s">
-        <v>716</v>
+        <v>774</v>
       </c>
     </row>
     <row r="217" spans="1:7" x14ac:dyDescent="0.25">
@@ -6344,7 +6410,7 @@
         <v>1</v>
       </c>
       <c r="G217" t="s">
-        <v>716</v>
+        <v>774</v>
       </c>
     </row>
     <row r="218" spans="1:7" x14ac:dyDescent="0.25">
@@ -6358,7 +6424,7 @@
         <v>1</v>
       </c>
       <c r="G218" t="s">
-        <v>716</v>
+        <v>775</v>
       </c>
     </row>
     <row r="219" spans="1:7" x14ac:dyDescent="0.25">
@@ -6372,7 +6438,7 @@
         <v>1</v>
       </c>
       <c r="G219" t="s">
-        <v>716</v>
+        <v>775</v>
       </c>
     </row>
     <row r="220" spans="1:7" x14ac:dyDescent="0.25">
@@ -6386,7 +6452,7 @@
         <v>1</v>
       </c>
       <c r="G220" t="s">
-        <v>716</v>
+        <v>775</v>
       </c>
     </row>
     <row r="221" spans="1:7" x14ac:dyDescent="0.25">
@@ -6403,7 +6469,7 @@
         <v>1</v>
       </c>
       <c r="G221" t="s">
-        <v>716</v>
+        <v>771</v>
       </c>
     </row>
     <row r="222" spans="1:7" x14ac:dyDescent="0.25">
@@ -6420,7 +6486,7 @@
         <v>1</v>
       </c>
       <c r="G222" t="s">
-        <v>716</v>
+        <v>771</v>
       </c>
     </row>
     <row r="223" spans="1:7" x14ac:dyDescent="0.25">
@@ -6434,7 +6500,7 @@
         <v>1</v>
       </c>
       <c r="G223" t="s">
-        <v>716</v>
+        <v>771</v>
       </c>
     </row>
     <row r="224" spans="1:7" x14ac:dyDescent="0.25">
@@ -6451,7 +6517,7 @@
         <v>1</v>
       </c>
       <c r="G224" t="s">
-        <v>716</v>
+        <v>771</v>
       </c>
     </row>
     <row r="225" spans="1:7" x14ac:dyDescent="0.25">
@@ -6468,7 +6534,7 @@
         <v>1</v>
       </c>
       <c r="G225" t="s">
-        <v>716</v>
+        <v>771</v>
       </c>
     </row>
     <row r="226" spans="1:7" x14ac:dyDescent="0.25">
@@ -6482,7 +6548,7 @@
         <v>1</v>
       </c>
       <c r="G226" t="s">
-        <v>716</v>
+        <v>776</v>
       </c>
     </row>
     <row r="227" spans="1:7" x14ac:dyDescent="0.25">
@@ -6499,7 +6565,7 @@
         <v>1</v>
       </c>
       <c r="G227" t="s">
-        <v>716</v>
+        <v>772</v>
       </c>
     </row>
     <row r="228" spans="1:7" x14ac:dyDescent="0.25">
@@ -6513,7 +6579,7 @@
         <v>1</v>
       </c>
       <c r="G228" t="s">
-        <v>716</v>
+        <v>777</v>
       </c>
     </row>
     <row r="229" spans="1:7" x14ac:dyDescent="0.25">
@@ -6530,7 +6596,7 @@
         <v>1</v>
       </c>
       <c r="G229" t="s">
-        <v>716</v>
+        <v>778</v>
       </c>
     </row>
     <row r="230" spans="1:7" x14ac:dyDescent="0.25">
@@ -6547,7 +6613,7 @@
         <v>1</v>
       </c>
       <c r="G230" t="s">
-        <v>716</v>
+        <v>778</v>
       </c>
     </row>
     <row r="231" spans="1:7" x14ac:dyDescent="0.25">
@@ -6564,7 +6630,7 @@
         <v>1</v>
       </c>
       <c r="G231" t="s">
-        <v>716</v>
+        <v>773</v>
       </c>
     </row>
     <row r="232" spans="1:7" x14ac:dyDescent="0.25">
@@ -6581,7 +6647,7 @@
         <v>1</v>
       </c>
       <c r="G232" t="s">
-        <v>716</v>
+        <v>773</v>
       </c>
     </row>
     <row r="233" spans="1:7" x14ac:dyDescent="0.25">
@@ -6598,7 +6664,7 @@
         <v>1</v>
       </c>
       <c r="G233" t="s">
-        <v>716</v>
+        <v>782</v>
       </c>
     </row>
     <row r="234" spans="1:7" x14ac:dyDescent="0.25">
@@ -6612,7 +6678,7 @@
         <v>1</v>
       </c>
       <c r="G234" t="s">
-        <v>716</v>
+        <v>782</v>
       </c>
     </row>
     <row r="235" spans="1:7" x14ac:dyDescent="0.25">
@@ -6629,7 +6695,7 @@
         <v>1</v>
       </c>
       <c r="G235" t="s">
-        <v>716</v>
+        <v>782</v>
       </c>
     </row>
     <row r="236" spans="1:7" x14ac:dyDescent="0.25">
@@ -6646,7 +6712,7 @@
         <v>1</v>
       </c>
       <c r="G236" t="s">
-        <v>716</v>
+        <v>782</v>
       </c>
     </row>
     <row r="237" spans="1:7" x14ac:dyDescent="0.25">
@@ -6663,7 +6729,7 @@
         <v>1</v>
       </c>
       <c r="G237" t="s">
-        <v>716</v>
+        <v>783</v>
       </c>
     </row>
     <row r="238" spans="1:7" x14ac:dyDescent="0.25">
@@ -6680,7 +6746,7 @@
         <v>1</v>
       </c>
       <c r="G238" t="s">
-        <v>716</v>
+        <v>783</v>
       </c>
     </row>
     <row r="239" spans="1:7" x14ac:dyDescent="0.25">
@@ -6697,7 +6763,7 @@
         <v>1</v>
       </c>
       <c r="G239" t="s">
-        <v>716</v>
+        <v>783</v>
       </c>
     </row>
     <row r="240" spans="1:7" x14ac:dyDescent="0.25">
@@ -6714,7 +6780,7 @@
         <v>1</v>
       </c>
       <c r="G240" t="s">
-        <v>716</v>
+        <v>783</v>
       </c>
     </row>
     <row r="241" spans="1:7" x14ac:dyDescent="0.25">
@@ -6728,7 +6794,7 @@
         <v>1</v>
       </c>
       <c r="G241" t="s">
-        <v>716</v>
+        <v>784</v>
       </c>
     </row>
     <row r="242" spans="1:7" x14ac:dyDescent="0.25">
@@ -6742,7 +6808,7 @@
         <v>1</v>
       </c>
       <c r="G242" t="s">
-        <v>716</v>
+        <v>784</v>
       </c>
     </row>
     <row r="243" spans="1:7" x14ac:dyDescent="0.25">
@@ -6756,7 +6822,7 @@
         <v>1</v>
       </c>
       <c r="G243" t="s">
-        <v>716</v>
+        <v>784</v>
       </c>
     </row>
     <row r="244" spans="1:7" x14ac:dyDescent="0.25">
@@ -6770,7 +6836,7 @@
         <v>1</v>
       </c>
       <c r="G244" t="s">
-        <v>716</v>
+        <v>785</v>
       </c>
     </row>
     <row r="245" spans="1:7" x14ac:dyDescent="0.25">
@@ -6787,7 +6853,7 @@
         <v>1</v>
       </c>
       <c r="G245" t="s">
-        <v>716</v>
+        <v>786</v>
       </c>
     </row>
     <row r="246" spans="1:7" x14ac:dyDescent="0.25">
@@ -6801,7 +6867,7 @@
         <v>1</v>
       </c>
       <c r="G246" t="s">
-        <v>716</v>
+        <v>787</v>
       </c>
     </row>
     <row r="247" spans="1:7" x14ac:dyDescent="0.25">
@@ -6815,7 +6881,7 @@
         <v>1</v>
       </c>
       <c r="G247" t="s">
-        <v>716</v>
+        <v>788</v>
       </c>
     </row>
     <row r="248" spans="1:7" x14ac:dyDescent="0.25">
@@ -6829,7 +6895,7 @@
         <v>1</v>
       </c>
       <c r="G248" t="s">
-        <v>716</v>
+        <v>789</v>
       </c>
     </row>
     <row r="249" spans="1:7" x14ac:dyDescent="0.25">
@@ -6843,7 +6909,7 @@
         <v>1</v>
       </c>
       <c r="G249" t="s">
-        <v>716</v>
+        <v>788</v>
       </c>
     </row>
     <row r="250" spans="1:7" x14ac:dyDescent="0.25">
@@ -6857,7 +6923,7 @@
         <v>1</v>
       </c>
       <c r="G250" t="s">
-        <v>716</v>
+        <v>788</v>
       </c>
     </row>
     <row r="251" spans="1:7" x14ac:dyDescent="0.25">
@@ -6871,7 +6937,7 @@
         <v>1</v>
       </c>
       <c r="G251" t="s">
-        <v>716</v>
+        <v>788</v>
       </c>
     </row>
     <row r="252" spans="1:7" x14ac:dyDescent="0.25">
@@ -6885,7 +6951,7 @@
         <v>1</v>
       </c>
       <c r="G252" t="s">
-        <v>716</v>
+        <v>792</v>
       </c>
     </row>
     <row r="253" spans="1:7" x14ac:dyDescent="0.25">
@@ -6899,7 +6965,7 @@
         <v>1</v>
       </c>
       <c r="G253" t="s">
-        <v>716</v>
+        <v>790</v>
       </c>
     </row>
     <row r="254" spans="1:7" x14ac:dyDescent="0.25">
@@ -6913,7 +6979,7 @@
         <v>1</v>
       </c>
       <c r="G254" t="s">
-        <v>716</v>
+        <v>792</v>
       </c>
     </row>
     <row r="255" spans="1:7" x14ac:dyDescent="0.25">
@@ -6927,7 +6993,7 @@
         <v>1</v>
       </c>
       <c r="G255" t="s">
-        <v>716</v>
+        <v>792</v>
       </c>
     </row>
     <row r="256" spans="1:7" x14ac:dyDescent="0.25">
@@ -6941,7 +7007,7 @@
         <v>1</v>
       </c>
       <c r="G256" t="s">
-        <v>716</v>
+        <v>792</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Ability to hide extra pronunciation info with the romaji
</commit_message>
<xml_diff>
--- a/read-and-write-kana/Note Types/Read & Write Kana/Read & Write Kana - Data Sheet.xlsx
+++ b/read-and-write-kana/Note Types/Read & Write Kana/Read & Write Kana - Data Sheet.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1206" uniqueCount="798">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1209" uniqueCount="800">
   <si>
     <t>あ</t>
   </si>
@@ -2405,6 +2405,12 @@
   </si>
   <si>
     <t>&lt;b&gt;Pronouncing &lt;i&gt;d&lt;/i&gt;&lt;/b&gt; &amp;ndash; This sound is a bit heavier than in English. The tongue presses hard against the upper teeth and gums. If you were to move your tongue a little lower down, a &lt;i&gt;th&lt;/i&gt; sound would come out.</t>
+  </si>
+  <si>
+    <t>Romaji Extra</t>
+  </si>
+  <si>
+    <t>&lt;small&gt;&lt;small&gt;/ztsa/&lt;/small&gt;&lt;/small&gt;</t>
   </si>
   <si>
     <t>&lt;div style="text-align:left; display:inline-block;"&gt;_x000D_
@@ -2783,7 +2789,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H256"/>
+  <dimension ref="A1:I256"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -2792,13 +2798,14 @@
     <col min="2" max="2" width="44" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="23.5703125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="22.42578125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="35.140625" customWidth="1"/>
-    <col min="6" max="6" width="58.85546875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="35.140625" customWidth="1"/>
-    <col min="8" max="8" width="97.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="22.42578125" customWidth="1"/>
+    <col min="6" max="6" width="35.140625" customWidth="1"/>
+    <col min="7" max="7" width="58.85546875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="35.140625" customWidth="1"/>
+    <col min="9" max="9" width="97.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>401</v>
       </c>
@@ -2812,19 +2819,22 @@
         <v>404</v>
       </c>
       <c r="E1" t="s">
+        <v>797</v>
+      </c>
+      <c r="F1" t="s">
         <v>532</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>533</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>793</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>715</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -2834,17 +2844,17 @@
       <c r="C2" t="s">
         <v>1</v>
       </c>
-      <c r="E2" t="s">
+      <c r="F2" t="s">
         <v>531</v>
       </c>
-      <c r="F2" t="s">
+      <c r="G2" t="s">
         <v>624</v>
       </c>
-      <c r="H2" t="s">
+      <c r="I2" t="s">
         <v>716</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -2854,17 +2864,17 @@
       <c r="C3" t="s">
         <v>3</v>
       </c>
-      <c r="E3" t="s">
+      <c r="F3" t="s">
         <v>534</v>
       </c>
-      <c r="F3" t="s">
+      <c r="G3" t="s">
         <v>625</v>
       </c>
-      <c r="H3" t="s">
+      <c r="I3" t="s">
         <v>716</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>4</v>
       </c>
@@ -2874,17 +2884,17 @@
       <c r="C4" t="s">
         <v>5</v>
       </c>
-      <c r="E4" t="s">
+      <c r="F4" t="s">
         <v>535</v>
       </c>
-      <c r="F4" t="s">
+      <c r="G4" t="s">
         <v>626</v>
       </c>
-      <c r="H4" t="s">
+      <c r="I4" t="s">
         <v>716</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>6</v>
       </c>
@@ -2894,17 +2904,17 @@
       <c r="C5" t="s">
         <v>7</v>
       </c>
-      <c r="E5" t="s">
+      <c r="F5" t="s">
         <v>536</v>
       </c>
-      <c r="F5" t="s">
+      <c r="G5" t="s">
         <v>627</v>
       </c>
-      <c r="H5" t="s">
+      <c r="I5" t="s">
         <v>716</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>8</v>
       </c>
@@ -2914,17 +2924,17 @@
       <c r="C6" t="s">
         <v>9</v>
       </c>
-      <c r="E6" t="s">
+      <c r="F6" t="s">
         <v>588</v>
       </c>
-      <c r="F6" t="s">
+      <c r="G6" t="s">
         <v>628</v>
       </c>
-      <c r="H6" t="s">
+      <c r="I6" t="s">
         <v>716</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>10</v>
       </c>
@@ -2934,17 +2944,17 @@
       <c r="C7" t="s">
         <v>11</v>
       </c>
-      <c r="E7" t="s">
+      <c r="F7" t="s">
         <v>537</v>
       </c>
-      <c r="F7" t="s">
+      <c r="G7" t="s">
         <v>629</v>
       </c>
-      <c r="H7" t="s">
+      <c r="I7" t="s">
         <v>717</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>12</v>
       </c>
@@ -2954,17 +2964,17 @@
       <c r="C8" t="s">
         <v>13</v>
       </c>
-      <c r="E8" t="s">
+      <c r="F8" t="s">
         <v>538</v>
       </c>
-      <c r="F8" t="s">
+      <c r="G8" t="s">
         <v>630</v>
       </c>
-      <c r="H8" t="s">
+      <c r="I8" t="s">
         <v>717</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>14</v>
       </c>
@@ -2974,17 +2984,17 @@
       <c r="C9" t="s">
         <v>15</v>
       </c>
-      <c r="E9" t="s">
+      <c r="F9" t="s">
         <v>539</v>
       </c>
-      <c r="F9" t="s">
+      <c r="G9" t="s">
         <v>631</v>
       </c>
-      <c r="H9" t="s">
+      <c r="I9" t="s">
         <v>717</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>16</v>
       </c>
@@ -2994,17 +3004,17 @@
       <c r="C10" t="s">
         <v>17</v>
       </c>
-      <c r="E10" t="s">
+      <c r="F10" t="s">
         <v>540</v>
       </c>
-      <c r="F10" t="s">
+      <c r="G10" t="s">
         <v>632</v>
       </c>
-      <c r="H10" t="s">
+      <c r="I10" t="s">
         <v>717</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>18</v>
       </c>
@@ -3014,17 +3024,17 @@
       <c r="C11" t="s">
         <v>19</v>
       </c>
-      <c r="E11" t="s">
+      <c r="F11" t="s">
         <v>541</v>
       </c>
-      <c r="F11" t="s">
+      <c r="G11" t="s">
         <v>633</v>
       </c>
-      <c r="H11" t="s">
+      <c r="I11" t="s">
         <v>717</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>20</v>
       </c>
@@ -3034,17 +3044,17 @@
       <c r="C12" t="s">
         <v>21</v>
       </c>
-      <c r="E12" t="s">
+      <c r="F12" t="s">
         <v>542</v>
       </c>
-      <c r="F12" t="s">
+      <c r="G12" t="s">
         <v>634</v>
       </c>
-      <c r="H12" t="s">
+      <c r="I12" t="s">
         <v>718</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>22</v>
       </c>
@@ -3054,17 +3064,17 @@
       <c r="C13" t="s">
         <v>23</v>
       </c>
-      <c r="E13" t="s">
+      <c r="F13" t="s">
         <v>543</v>
       </c>
-      <c r="F13" t="s">
+      <c r="G13" t="s">
         <v>635</v>
       </c>
-      <c r="H13" t="s">
+      <c r="I13" t="s">
         <v>718</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>24</v>
       </c>
@@ -3074,17 +3084,17 @@
       <c r="C14" t="s">
         <v>25</v>
       </c>
-      <c r="E14" t="s">
+      <c r="F14" t="s">
         <v>544</v>
       </c>
-      <c r="F14" t="s">
+      <c r="G14" t="s">
         <v>636</v>
       </c>
-      <c r="H14" t="s">
+      <c r="I14" t="s">
         <v>718</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>26</v>
       </c>
@@ -3094,17 +3104,17 @@
       <c r="C15" t="s">
         <v>27</v>
       </c>
-      <c r="E15" t="s">
+      <c r="F15" t="s">
         <v>545</v>
       </c>
-      <c r="F15" t="s">
+      <c r="G15" t="s">
         <v>637</v>
       </c>
-      <c r="H15" t="s">
+      <c r="I15" t="s">
         <v>718</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>28</v>
       </c>
@@ -3114,17 +3124,17 @@
       <c r="C16" t="s">
         <v>29</v>
       </c>
-      <c r="E16" t="s">
+      <c r="F16" t="s">
         <v>546</v>
       </c>
-      <c r="F16" t="s">
+      <c r="G16" t="s">
         <v>638</v>
       </c>
-      <c r="H16" t="s">
+      <c r="I16" t="s">
         <v>718</v>
       </c>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>30</v>
       </c>
@@ -3134,17 +3144,17 @@
       <c r="C17" t="s">
         <v>31</v>
       </c>
-      <c r="E17" t="s">
+      <c r="F17" t="s">
         <v>547</v>
       </c>
-      <c r="F17" t="s">
+      <c r="G17" t="s">
         <v>639</v>
       </c>
-      <c r="H17" t="s">
+      <c r="I17" t="s">
         <v>719</v>
       </c>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>32</v>
       </c>
@@ -3154,17 +3164,17 @@
       <c r="C18" t="s">
         <v>33</v>
       </c>
-      <c r="E18" t="s">
+      <c r="F18" t="s">
         <v>548</v>
       </c>
-      <c r="F18" t="s">
+      <c r="G18" t="s">
         <v>640</v>
       </c>
-      <c r="H18" t="s">
+      <c r="I18" t="s">
         <v>719</v>
       </c>
     </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>34</v>
       </c>
@@ -3174,17 +3184,17 @@
       <c r="C19" t="s">
         <v>35</v>
       </c>
-      <c r="E19" t="s">
+      <c r="F19" t="s">
         <v>549</v>
       </c>
-      <c r="F19" t="s">
+      <c r="G19" t="s">
         <v>641</v>
       </c>
-      <c r="H19" t="s">
+      <c r="I19" t="s">
         <v>719</v>
       </c>
     </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>36</v>
       </c>
@@ -3194,17 +3204,17 @@
       <c r="C20" t="s">
         <v>37</v>
       </c>
-      <c r="E20" t="s">
+      <c r="F20" t="s">
         <v>550</v>
       </c>
-      <c r="F20" t="s">
+      <c r="G20" t="s">
         <v>642</v>
       </c>
-      <c r="H20" t="s">
+      <c r="I20" t="s">
         <v>719</v>
       </c>
     </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>38</v>
       </c>
@@ -3214,17 +3224,17 @@
       <c r="C21" t="s">
         <v>39</v>
       </c>
-      <c r="E21" t="s">
+      <c r="F21" t="s">
         <v>551</v>
       </c>
-      <c r="F21" t="s">
+      <c r="G21" t="s">
         <v>643</v>
       </c>
-      <c r="H21" t="s">
+      <c r="I21" t="s">
         <v>719</v>
       </c>
     </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>40</v>
       </c>
@@ -3234,17 +3244,17 @@
       <c r="C22" t="s">
         <v>41</v>
       </c>
-      <c r="E22" t="s">
+      <c r="F22" t="s">
         <v>552</v>
       </c>
-      <c r="F22" t="s">
+      <c r="G22" t="s">
         <v>644</v>
       </c>
-      <c r="H22" t="s">
+      <c r="I22" t="s">
         <v>720</v>
       </c>
     </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>42</v>
       </c>
@@ -3254,17 +3264,17 @@
       <c r="C23" t="s">
         <v>43</v>
       </c>
-      <c r="E23" t="s">
+      <c r="F23" t="s">
         <v>553</v>
       </c>
-      <c r="F23" t="s">
+      <c r="G23" t="s">
         <v>645</v>
       </c>
-      <c r="H23" t="s">
+      <c r="I23" t="s">
         <v>720</v>
       </c>
     </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>44</v>
       </c>
@@ -3274,17 +3284,17 @@
       <c r="C24" t="s">
         <v>45</v>
       </c>
-      <c r="E24" t="s">
+      <c r="F24" t="s">
         <v>554</v>
       </c>
-      <c r="F24" t="s">
+      <c r="G24" t="s">
         <v>646</v>
       </c>
-      <c r="H24" t="s">
+      <c r="I24" t="s">
         <v>720</v>
       </c>
     </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>46</v>
       </c>
@@ -3294,17 +3304,17 @@
       <c r="C25" t="s">
         <v>47</v>
       </c>
-      <c r="E25" t="s">
+      <c r="F25" t="s">
         <v>555</v>
       </c>
-      <c r="F25" t="s">
+      <c r="G25" t="s">
         <v>647</v>
       </c>
-      <c r="H25" t="s">
+      <c r="I25" t="s">
         <v>720</v>
       </c>
     </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>48</v>
       </c>
@@ -3314,17 +3324,17 @@
       <c r="C26" t="s">
         <v>49</v>
       </c>
-      <c r="E26" t="s">
+      <c r="F26" t="s">
         <v>556</v>
       </c>
-      <c r="F26" t="s">
+      <c r="G26" t="s">
         <v>648</v>
       </c>
-      <c r="H26" t="s">
+      <c r="I26" t="s">
         <v>720</v>
       </c>
     </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>50</v>
       </c>
@@ -3334,17 +3344,17 @@
       <c r="C27" t="s">
         <v>51</v>
       </c>
-      <c r="E27" t="s">
+      <c r="F27" t="s">
         <v>557</v>
       </c>
-      <c r="F27" t="s">
+      <c r="G27" t="s">
         <v>649</v>
       </c>
-      <c r="H27" t="s">
+      <c r="I27" t="s">
         <v>721</v>
       </c>
     </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>52</v>
       </c>
@@ -3354,17 +3364,17 @@
       <c r="C28" t="s">
         <v>53</v>
       </c>
-      <c r="E28" t="s">
+      <c r="F28" t="s">
         <v>558</v>
       </c>
-      <c r="F28" t="s">
+      <c r="G28" t="s">
         <v>650</v>
       </c>
-      <c r="H28" t="s">
+      <c r="I28" t="s">
         <v>721</v>
       </c>
     </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>54</v>
       </c>
@@ -3374,20 +3384,20 @@
       <c r="C29" t="s">
         <v>55</v>
       </c>
-      <c r="E29" t="s">
+      <c r="F29" t="s">
         <v>559</v>
       </c>
-      <c r="F29" t="s">
+      <c r="G29" t="s">
         <v>651</v>
       </c>
-      <c r="G29" t="s">
+      <c r="H29" t="s">
         <v>794</v>
       </c>
-      <c r="H29" t="s">
+      <c r="I29" t="s">
         <v>721</v>
       </c>
     </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>56</v>
       </c>
@@ -3397,17 +3407,17 @@
       <c r="C30" t="s">
         <v>57</v>
       </c>
-      <c r="E30" t="s">
+      <c r="F30" t="s">
         <v>560</v>
       </c>
-      <c r="F30" t="s">
+      <c r="G30" t="s">
         <v>652</v>
       </c>
-      <c r="H30" t="s">
+      <c r="I30" t="s">
         <v>721</v>
       </c>
     </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>58</v>
       </c>
@@ -3417,17 +3427,17 @@
       <c r="C31" t="s">
         <v>59</v>
       </c>
-      <c r="E31" t="s">
+      <c r="F31" t="s">
         <v>561</v>
       </c>
-      <c r="F31" t="s">
+      <c r="G31" t="s">
         <v>653</v>
       </c>
-      <c r="H31" t="s">
+      <c r="I31" t="s">
         <v>721</v>
       </c>
     </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>60</v>
       </c>
@@ -3437,17 +3447,17 @@
       <c r="C32" t="s">
         <v>61</v>
       </c>
-      <c r="E32" t="s">
+      <c r="F32" t="s">
         <v>563</v>
       </c>
-      <c r="F32" t="s">
+      <c r="G32" t="s">
         <v>654</v>
       </c>
-      <c r="H32" t="s">
+      <c r="I32" t="s">
         <v>722</v>
       </c>
     </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>62</v>
       </c>
@@ -3457,17 +3467,17 @@
       <c r="C33" t="s">
         <v>63</v>
       </c>
-      <c r="E33" t="s">
+      <c r="F33" t="s">
         <v>562</v>
       </c>
-      <c r="F33" t="s">
+      <c r="G33" t="s">
         <v>655</v>
       </c>
-      <c r="H33" t="s">
+      <c r="I33" t="s">
         <v>722</v>
       </c>
     </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>64</v>
       </c>
@@ -3477,17 +3487,17 @@
       <c r="C34" t="s">
         <v>65</v>
       </c>
-      <c r="E34" t="s">
+      <c r="F34" t="s">
         <v>564</v>
       </c>
-      <c r="F34" t="s">
+      <c r="G34" t="s">
         <v>656</v>
       </c>
-      <c r="H34" t="s">
+      <c r="I34" t="s">
         <v>722</v>
       </c>
     </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>66</v>
       </c>
@@ -3497,17 +3507,17 @@
       <c r="C35" t="s">
         <v>67</v>
       </c>
-      <c r="E35" t="s">
+      <c r="F35" t="s">
         <v>565</v>
       </c>
-      <c r="F35" t="s">
+      <c r="G35" t="s">
         <v>657</v>
       </c>
-      <c r="H35" t="s">
+      <c r="I35" t="s">
         <v>722</v>
       </c>
     </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>68</v>
       </c>
@@ -3517,17 +3527,17 @@
       <c r="C36" t="s">
         <v>69</v>
       </c>
-      <c r="E36" t="s">
+      <c r="F36" t="s">
         <v>566</v>
       </c>
-      <c r="F36" t="s">
+      <c r="G36" t="s">
         <v>658</v>
       </c>
-      <c r="H36" t="s">
+      <c r="I36" t="s">
         <v>722</v>
       </c>
     </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>70</v>
       </c>
@@ -3537,17 +3547,17 @@
       <c r="C37" t="s">
         <v>71</v>
       </c>
-      <c r="E37" t="s">
+      <c r="F37" t="s">
         <v>567</v>
       </c>
-      <c r="F37" t="s">
+      <c r="G37" t="s">
         <v>659</v>
       </c>
-      <c r="H37" t="s">
+      <c r="I37" t="s">
         <v>723</v>
       </c>
     </row>
-    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>72</v>
       </c>
@@ -3557,17 +3567,17 @@
       <c r="C38" t="s">
         <v>73</v>
       </c>
-      <c r="E38" t="s">
+      <c r="F38" t="s">
         <v>568</v>
       </c>
-      <c r="F38" t="s">
+      <c r="G38" t="s">
         <v>660</v>
       </c>
-      <c r="H38" t="s">
+      <c r="I38" t="s">
         <v>723</v>
       </c>
     </row>
-    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>74</v>
       </c>
@@ -3577,17 +3587,17 @@
       <c r="C39" t="s">
         <v>75</v>
       </c>
-      <c r="E39" t="s">
+      <c r="F39" t="s">
         <v>569</v>
       </c>
-      <c r="F39" t="s">
+      <c r="G39" t="s">
         <v>661</v>
       </c>
-      <c r="H39" t="s">
+      <c r="I39" t="s">
         <v>723</v>
       </c>
     </row>
-    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>76</v>
       </c>
@@ -3597,20 +3607,20 @@
       <c r="C40" t="s">
         <v>77</v>
       </c>
-      <c r="E40" t="s">
+      <c r="F40" t="s">
         <v>570</v>
       </c>
-      <c r="F40" t="s">
+      <c r="G40" t="s">
         <v>662</v>
       </c>
-      <c r="G40" t="s">
+      <c r="H40" t="s">
         <v>795</v>
       </c>
-      <c r="H40" t="s">
+      <c r="I40" t="s">
         <v>724</v>
       </c>
     </row>
-    <row r="41" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>78</v>
       </c>
@@ -3620,20 +3630,20 @@
       <c r="C41" t="s">
         <v>79</v>
       </c>
-      <c r="E41" t="s">
+      <c r="F41" t="s">
         <v>571</v>
       </c>
-      <c r="F41" t="s">
+      <c r="G41" t="s">
         <v>663</v>
       </c>
-      <c r="G41" t="s">
+      <c r="H41" t="s">
         <v>795</v>
       </c>
-      <c r="H41" t="s">
+      <c r="I41" t="s">
         <v>724</v>
       </c>
     </row>
-    <row r="42" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>80</v>
       </c>
@@ -3643,20 +3653,20 @@
       <c r="C42" t="s">
         <v>81</v>
       </c>
-      <c r="E42" t="s">
+      <c r="F42" t="s">
         <v>572</v>
       </c>
-      <c r="F42" t="s">
+      <c r="G42" t="s">
         <v>664</v>
       </c>
-      <c r="G42" t="s">
+      <c r="H42" t="s">
         <v>795</v>
       </c>
-      <c r="H42" t="s">
+      <c r="I42" t="s">
         <v>724</v>
       </c>
     </row>
-    <row r="43" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>82</v>
       </c>
@@ -3666,20 +3676,20 @@
       <c r="C43" t="s">
         <v>83</v>
       </c>
-      <c r="E43" t="s">
+      <c r="F43" t="s">
         <v>573</v>
       </c>
-      <c r="F43" t="s">
+      <c r="G43" t="s">
         <v>665</v>
       </c>
-      <c r="G43" t="s">
+      <c r="H43" t="s">
         <v>795</v>
       </c>
-      <c r="H43" t="s">
+      <c r="I43" t="s">
         <v>724</v>
       </c>
     </row>
-    <row r="44" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>84</v>
       </c>
@@ -3689,20 +3699,20 @@
       <c r="C44" t="s">
         <v>85</v>
       </c>
-      <c r="E44" t="s">
+      <c r="F44" t="s">
         <v>574</v>
       </c>
-      <c r="F44" t="s">
+      <c r="G44" t="s">
         <v>666</v>
       </c>
-      <c r="G44" t="s">
+      <c r="H44" t="s">
         <v>795</v>
       </c>
-      <c r="H44" t="s">
+      <c r="I44" t="s">
         <v>724</v>
       </c>
     </row>
-    <row r="45" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>86</v>
       </c>
@@ -3712,17 +3722,17 @@
       <c r="C45" t="s">
         <v>87</v>
       </c>
-      <c r="E45" t="s">
+      <c r="F45" t="s">
         <v>575</v>
       </c>
-      <c r="F45" t="s">
+      <c r="G45" t="s">
         <v>667</v>
       </c>
-      <c r="H45" t="s">
+      <c r="I45" t="s">
         <v>725</v>
       </c>
     </row>
-    <row r="46" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>88</v>
       </c>
@@ -3735,17 +3745,17 @@
       <c r="D46">
         <v>1</v>
       </c>
-      <c r="E46" t="s">
+      <c r="F46" t="s">
         <v>576</v>
       </c>
-      <c r="F46" t="s">
+      <c r="G46" t="s">
         <v>668</v>
       </c>
-      <c r="H46" t="s">
+      <c r="I46" t="s">
         <v>725</v>
       </c>
     </row>
-    <row r="47" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>90</v>
       </c>
@@ -3755,20 +3765,20 @@
       <c r="C47" t="s">
         <v>91</v>
       </c>
-      <c r="E47" t="s">
+      <c r="F47" t="s">
         <v>577</v>
       </c>
-      <c r="F47" t="s">
+      <c r="G47" t="s">
         <v>669</v>
       </c>
-      <c r="G47" s="1" t="s">
-        <v>797</v>
-      </c>
-      <c r="H47" t="s">
+      <c r="H47" s="1" t="s">
+        <v>799</v>
+      </c>
+      <c r="I47" t="s">
         <v>725</v>
       </c>
     </row>
-    <row r="48" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>92</v>
       </c>
@@ -3778,11 +3788,11 @@
       <c r="C48" t="s">
         <v>93</v>
       </c>
-      <c r="H48" t="s">
+      <c r="I48" t="s">
         <v>726</v>
       </c>
     </row>
-    <row r="49" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>94</v>
       </c>
@@ -3792,11 +3802,11 @@
       <c r="C49" t="s">
         <v>95</v>
       </c>
-      <c r="H49" t="s">
+      <c r="I49" t="s">
         <v>726</v>
       </c>
     </row>
-    <row r="50" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>96</v>
       </c>
@@ -3806,11 +3816,11 @@
       <c r="C50" t="s">
         <v>97</v>
       </c>
-      <c r="H50" t="s">
+      <c r="I50" t="s">
         <v>726</v>
       </c>
     </row>
-    <row r="51" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>98</v>
       </c>
@@ -3820,11 +3830,11 @@
       <c r="C51" t="s">
         <v>99</v>
       </c>
-      <c r="H51" t="s">
+      <c r="I51" t="s">
         <v>726</v>
       </c>
     </row>
-    <row r="52" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>100</v>
       </c>
@@ -3834,11 +3844,11 @@
       <c r="C52" t="s">
         <v>101</v>
       </c>
-      <c r="H52" t="s">
+      <c r="I52" t="s">
         <v>726</v>
       </c>
     </row>
-    <row r="53" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>102</v>
       </c>
@@ -3848,11 +3858,14 @@
       <c r="C53" t="s">
         <v>103</v>
       </c>
-      <c r="H53" t="s">
+      <c r="E53" t="s">
+        <v>798</v>
+      </c>
+      <c r="I53" t="s">
         <v>727</v>
       </c>
     </row>
-    <row r="54" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>104</v>
       </c>
@@ -3865,11 +3878,11 @@
       <c r="D54">
         <v>1</v>
       </c>
-      <c r="H54" t="s">
+      <c r="I54" t="s">
         <v>727</v>
       </c>
     </row>
-    <row r="55" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>106</v>
       </c>
@@ -3882,11 +3895,11 @@
       <c r="D55">
         <v>1</v>
       </c>
-      <c r="H55" t="s">
+      <c r="I55" t="s">
         <v>727</v>
       </c>
     </row>
-    <row r="56" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
         <v>108</v>
       </c>
@@ -3896,11 +3909,11 @@
       <c r="C56" t="s">
         <v>109</v>
       </c>
-      <c r="H56" t="s">
+      <c r="I56" t="s">
         <v>727</v>
       </c>
     </row>
-    <row r="57" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
         <v>110</v>
       </c>
@@ -3910,11 +3923,11 @@
       <c r="C57" t="s">
         <v>111</v>
       </c>
-      <c r="H57" t="s">
+      <c r="I57" t="s">
         <v>727</v>
       </c>
     </row>
-    <row r="58" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
         <v>112</v>
       </c>
@@ -3924,14 +3937,14 @@
       <c r="C58" t="s">
         <v>113</v>
       </c>
-      <c r="G58" t="s">
+      <c r="H58" t="s">
         <v>796</v>
       </c>
-      <c r="H58" t="s">
+      <c r="I58" t="s">
         <v>728</v>
       </c>
     </row>
-    <row r="59" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
         <v>114</v>
       </c>
@@ -3944,11 +3957,11 @@
       <c r="D59">
         <v>1</v>
       </c>
-      <c r="H59" t="s">
+      <c r="I59" t="s">
         <v>728</v>
       </c>
     </row>
-    <row r="60" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
         <v>116</v>
       </c>
@@ -3961,11 +3974,11 @@
       <c r="D60">
         <v>1</v>
       </c>
-      <c r="H60" t="s">
+      <c r="I60" t="s">
         <v>728</v>
       </c>
     </row>
-    <row r="61" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
         <v>118</v>
       </c>
@@ -3975,14 +3988,14 @@
       <c r="C61" t="s">
         <v>119</v>
       </c>
-      <c r="G61" t="s">
+      <c r="H61" t="s">
         <v>796</v>
       </c>
-      <c r="H61" t="s">
+      <c r="I61" t="s">
         <v>728</v>
       </c>
     </row>
-    <row r="62" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
         <v>120</v>
       </c>
@@ -3992,14 +4005,14 @@
       <c r="C62" t="s">
         <v>121</v>
       </c>
-      <c r="G62" t="s">
+      <c r="H62" t="s">
         <v>796</v>
       </c>
-      <c r="H62" t="s">
+      <c r="I62" t="s">
         <v>728</v>
       </c>
     </row>
-    <row r="63" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
         <v>122</v>
       </c>
@@ -4009,11 +4022,11 @@
       <c r="C63" t="s">
         <v>123</v>
       </c>
-      <c r="H63" t="s">
+      <c r="I63" t="s">
         <v>729</v>
       </c>
     </row>
-    <row r="64" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
         <v>124</v>
       </c>
@@ -4023,11 +4036,11 @@
       <c r="C64" t="s">
         <v>125</v>
       </c>
-      <c r="H64" t="s">
+      <c r="I64" t="s">
         <v>729</v>
       </c>
     </row>
-    <row r="65" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
         <v>126</v>
       </c>
@@ -4037,11 +4050,11 @@
       <c r="C65" t="s">
         <v>127</v>
       </c>
-      <c r="H65" t="s">
+      <c r="I65" t="s">
         <v>729</v>
       </c>
     </row>
-    <row r="66" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
         <v>128</v>
       </c>
@@ -4051,11 +4064,11 @@
       <c r="C66" t="s">
         <v>129</v>
       </c>
-      <c r="H66" t="s">
+      <c r="I66" t="s">
         <v>729</v>
       </c>
     </row>
-    <row r="67" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
         <v>130</v>
       </c>
@@ -4065,11 +4078,11 @@
       <c r="C67" t="s">
         <v>131</v>
       </c>
-      <c r="H67" t="s">
+      <c r="I67" t="s">
         <v>729</v>
       </c>
     </row>
-    <row r="68" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
         <v>132</v>
       </c>
@@ -4079,11 +4092,11 @@
       <c r="C68" t="s">
         <v>133</v>
       </c>
-      <c r="H68" t="s">
+      <c r="I68" t="s">
         <v>740</v>
       </c>
     </row>
-    <row r="69" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
         <v>134</v>
       </c>
@@ -4093,11 +4106,11 @@
       <c r="C69" t="s">
         <v>135</v>
       </c>
-      <c r="H69" t="s">
+      <c r="I69" t="s">
         <v>740</v>
       </c>
     </row>
-    <row r="70" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
         <v>136</v>
       </c>
@@ -4107,11 +4120,11 @@
       <c r="C70" t="s">
         <v>137</v>
       </c>
-      <c r="H70" t="s">
+      <c r="I70" t="s">
         <v>740</v>
       </c>
     </row>
-    <row r="71" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
         <v>138</v>
       </c>
@@ -4121,11 +4134,11 @@
       <c r="C71" t="s">
         <v>139</v>
       </c>
-      <c r="H71" t="s">
+      <c r="I71" t="s">
         <v>740</v>
       </c>
     </row>
-    <row r="72" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
         <v>140</v>
       </c>
@@ -4135,11 +4148,11 @@
       <c r="C72" t="s">
         <v>141</v>
       </c>
-      <c r="H72" t="s">
+      <c r="I72" t="s">
         <v>740</v>
       </c>
     </row>
-    <row r="73" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
         <v>142</v>
       </c>
@@ -4149,11 +4162,11 @@
       <c r="C73" t="s">
         <v>143</v>
       </c>
-      <c r="H73" t="s">
+      <c r="I73" t="s">
         <v>731</v>
       </c>
     </row>
-    <row r="74" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
         <v>144</v>
       </c>
@@ -4163,11 +4176,11 @@
       <c r="C74" t="s">
         <v>145</v>
       </c>
-      <c r="H74" t="s">
+      <c r="I74" t="s">
         <v>731</v>
       </c>
     </row>
-    <row r="75" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
         <v>146</v>
       </c>
@@ -4177,11 +4190,11 @@
       <c r="C75" t="s">
         <v>147</v>
       </c>
-      <c r="H75" t="s">
+      <c r="I75" t="s">
         <v>731</v>
       </c>
     </row>
-    <row r="76" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
         <v>148</v>
       </c>
@@ -4191,11 +4204,11 @@
       <c r="C76" t="s">
         <v>149</v>
       </c>
-      <c r="H76" t="s">
+      <c r="I76" t="s">
         <v>732</v>
       </c>
     </row>
-    <row r="77" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
         <v>150</v>
       </c>
@@ -4205,11 +4218,11 @@
       <c r="C77" t="s">
         <v>151</v>
       </c>
-      <c r="H77" t="s">
+      <c r="I77" t="s">
         <v>732</v>
       </c>
     </row>
-    <row r="78" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
         <v>152</v>
       </c>
@@ -4219,11 +4232,11 @@
       <c r="C78" t="s">
         <v>153</v>
       </c>
-      <c r="H78" t="s">
+      <c r="I78" t="s">
         <v>732</v>
       </c>
     </row>
-    <row r="79" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
         <v>154</v>
       </c>
@@ -4233,11 +4246,11 @@
       <c r="C79" t="s">
         <v>155</v>
       </c>
-      <c r="H79" t="s">
+      <c r="I79" t="s">
         <v>730</v>
       </c>
     </row>
-    <row r="80" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
         <v>156</v>
       </c>
@@ -4247,11 +4260,11 @@
       <c r="C80" t="s">
         <v>157</v>
       </c>
-      <c r="H80" t="s">
+      <c r="I80" t="s">
         <v>730</v>
       </c>
     </row>
-    <row r="81" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
         <v>158</v>
       </c>
@@ -4261,11 +4274,11 @@
       <c r="C81" t="s">
         <v>159</v>
       </c>
-      <c r="H81" t="s">
+      <c r="I81" t="s">
         <v>730</v>
       </c>
     </row>
-    <row r="82" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
         <v>160</v>
       </c>
@@ -4275,11 +4288,11 @@
       <c r="C82" t="s">
         <v>161</v>
       </c>
-      <c r="H82" t="s">
+      <c r="I82" t="s">
         <v>733</v>
       </c>
     </row>
-    <row r="83" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
         <v>162</v>
       </c>
@@ -4289,11 +4302,11 @@
       <c r="C83" t="s">
         <v>163</v>
       </c>
-      <c r="H83" t="s">
+      <c r="I83" t="s">
         <v>733</v>
       </c>
     </row>
-    <row r="84" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
         <v>164</v>
       </c>
@@ -4303,11 +4316,11 @@
       <c r="C84" t="s">
         <v>165</v>
       </c>
-      <c r="H84" t="s">
+      <c r="I84" t="s">
         <v>733</v>
       </c>
     </row>
-    <row r="85" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
         <v>166</v>
       </c>
@@ -4317,11 +4330,11 @@
       <c r="C85" t="s">
         <v>167</v>
       </c>
-      <c r="H85" t="s">
+      <c r="I85" t="s">
         <v>734</v>
       </c>
     </row>
-    <row r="86" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
         <v>168</v>
       </c>
@@ -4331,11 +4344,11 @@
       <c r="C86" t="s">
         <v>169</v>
       </c>
-      <c r="H86" t="s">
+      <c r="I86" t="s">
         <v>734</v>
       </c>
     </row>
-    <row r="87" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
         <v>170</v>
       </c>
@@ -4345,11 +4358,11 @@
       <c r="C87" t="s">
         <v>171</v>
       </c>
-      <c r="H87" t="s">
+      <c r="I87" t="s">
         <v>734</v>
       </c>
     </row>
-    <row r="88" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
         <v>172</v>
       </c>
@@ -4359,11 +4372,11 @@
       <c r="C88" t="s">
         <v>173</v>
       </c>
-      <c r="H88" t="s">
+      <c r="I88" t="s">
         <v>735</v>
       </c>
     </row>
-    <row r="89" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
         <v>174</v>
       </c>
@@ -4373,11 +4386,11 @@
       <c r="C89" t="s">
         <v>175</v>
       </c>
-      <c r="H89" t="s">
+      <c r="I89" t="s">
         <v>735</v>
       </c>
     </row>
-    <row r="90" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
         <v>176</v>
       </c>
@@ -4387,11 +4400,11 @@
       <c r="C90" t="s">
         <v>177</v>
       </c>
-      <c r="H90" t="s">
+      <c r="I90" t="s">
         <v>735</v>
       </c>
     </row>
-    <row r="91" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
         <v>178</v>
       </c>
@@ -4401,11 +4414,11 @@
       <c r="C91" t="s">
         <v>179</v>
       </c>
-      <c r="H91" t="s">
+      <c r="I91" t="s">
         <v>736</v>
       </c>
     </row>
-    <row r="92" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
         <v>180</v>
       </c>
@@ -4418,11 +4431,11 @@
       <c r="D92">
         <v>1</v>
       </c>
-      <c r="H92" t="s">
+      <c r="I92" t="s">
         <v>736</v>
       </c>
     </row>
-    <row r="93" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
         <v>182</v>
       </c>
@@ -4432,11 +4445,11 @@
       <c r="C93" t="s">
         <v>183</v>
       </c>
-      <c r="H93" t="s">
+      <c r="I93" t="s">
         <v>736</v>
       </c>
     </row>
-    <row r="94" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
         <v>184</v>
       </c>
@@ -4446,11 +4459,11 @@
       <c r="C94" t="s">
         <v>185</v>
       </c>
-      <c r="H94" t="s">
+      <c r="I94" t="s">
         <v>737</v>
       </c>
     </row>
-    <row r="95" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
         <v>186</v>
       </c>
@@ -4460,11 +4473,11 @@
       <c r="C95" t="s">
         <v>187</v>
       </c>
-      <c r="H95" t="s">
+      <c r="I95" t="s">
         <v>737</v>
       </c>
     </row>
-    <row r="96" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
         <v>188</v>
       </c>
@@ -4474,11 +4487,11 @@
       <c r="C96" t="s">
         <v>189</v>
       </c>
-      <c r="H96" t="s">
+      <c r="I96" t="s">
         <v>737</v>
       </c>
     </row>
-    <row r="97" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
         <v>190</v>
       </c>
@@ -4491,11 +4504,11 @@
       <c r="D97">
         <v>1</v>
       </c>
-      <c r="H97" t="s">
+      <c r="I97" t="s">
         <v>738</v>
       </c>
     </row>
-    <row r="98" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
         <v>192</v>
       </c>
@@ -4508,11 +4521,11 @@
       <c r="D98">
         <v>1</v>
       </c>
-      <c r="H98" t="s">
+      <c r="I98" t="s">
         <v>738</v>
       </c>
     </row>
-    <row r="99" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
         <v>194</v>
       </c>
@@ -4525,11 +4538,11 @@
       <c r="D99">
         <v>1</v>
       </c>
-      <c r="H99" t="s">
+      <c r="I99" t="s">
         <v>738</v>
       </c>
     </row>
-    <row r="100" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
         <v>196</v>
       </c>
@@ -4542,11 +4555,11 @@
       <c r="D100">
         <v>1</v>
       </c>
-      <c r="H100" t="s">
+      <c r="I100" t="s">
         <v>739</v>
       </c>
     </row>
-    <row r="101" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
         <v>198</v>
       </c>
@@ -4559,11 +4572,11 @@
       <c r="D101">
         <v>1</v>
       </c>
-      <c r="H101" t="s">
+      <c r="I101" t="s">
         <v>739</v>
       </c>
     </row>
-    <row r="102" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
         <v>200</v>
       </c>
@@ -4576,11 +4589,11 @@
       <c r="D102">
         <v>1</v>
       </c>
-      <c r="H102" t="s">
+      <c r="I102" t="s">
         <v>739</v>
       </c>
     </row>
-    <row r="103" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
         <v>202</v>
       </c>
@@ -4590,11 +4603,11 @@
       <c r="C103" t="s">
         <v>203</v>
       </c>
-      <c r="H103" t="s">
+      <c r="I103" t="s">
         <v>741</v>
       </c>
     </row>
-    <row r="104" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
         <v>204</v>
       </c>
@@ -4604,11 +4617,11 @@
       <c r="C104" t="s">
         <v>205</v>
       </c>
-      <c r="H104" t="s">
+      <c r="I104" t="s">
         <v>741</v>
       </c>
     </row>
-    <row r="105" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
         <v>206</v>
       </c>
@@ -4618,11 +4631,11 @@
       <c r="C105" t="s">
         <v>207</v>
       </c>
-      <c r="H105" t="s">
+      <c r="I105" t="s">
         <v>741</v>
       </c>
     </row>
-    <row r="106" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
         <v>208</v>
       </c>
@@ -4632,11 +4645,11 @@
       <c r="C106" t="s">
         <v>209</v>
       </c>
-      <c r="H106" t="s">
+      <c r="I106" t="s">
         <v>742</v>
       </c>
     </row>
-    <row r="107" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A107" t="s">
         <v>210</v>
       </c>
@@ -4646,11 +4659,11 @@
       <c r="C107" t="s">
         <v>211</v>
       </c>
-      <c r="H107" t="s">
+      <c r="I107" t="s">
         <v>742</v>
       </c>
     </row>
-    <row r="108" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A108" t="s">
         <v>212</v>
       </c>
@@ -4660,11 +4673,11 @@
       <c r="C108" t="s">
         <v>213</v>
       </c>
-      <c r="H108" t="s">
+      <c r="I108" t="s">
         <v>742</v>
       </c>
     </row>
-    <row r="109" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A109" t="s">
         <v>214</v>
       </c>
@@ -4674,17 +4687,17 @@
       <c r="C109" t="s">
         <v>1</v>
       </c>
-      <c r="E109" t="s">
+      <c r="F109" t="s">
         <v>578</v>
       </c>
-      <c r="F109" t="s">
+      <c r="G109" t="s">
         <v>670</v>
       </c>
-      <c r="H109" t="s">
+      <c r="I109" t="s">
         <v>743</v>
       </c>
     </row>
-    <row r="110" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A110" t="s">
         <v>215</v>
       </c>
@@ -4694,17 +4707,17 @@
       <c r="C110" t="s">
         <v>3</v>
       </c>
-      <c r="E110" t="s">
+      <c r="F110" t="s">
         <v>579</v>
       </c>
-      <c r="F110" t="s">
+      <c r="G110" t="s">
         <v>671</v>
       </c>
-      <c r="H110" t="s">
+      <c r="I110" t="s">
         <v>743</v>
       </c>
     </row>
-    <row r="111" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A111" t="s">
         <v>216</v>
       </c>
@@ -4714,17 +4727,17 @@
       <c r="C111" t="s">
         <v>5</v>
       </c>
-      <c r="E111" t="s">
+      <c r="F111" t="s">
         <v>580</v>
       </c>
-      <c r="F111" t="s">
+      <c r="G111" t="s">
         <v>672</v>
       </c>
-      <c r="H111" t="s">
+      <c r="I111" t="s">
         <v>743</v>
       </c>
     </row>
-    <row r="112" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A112" t="s">
         <v>217</v>
       </c>
@@ -4734,17 +4747,17 @@
       <c r="C112" t="s">
         <v>7</v>
       </c>
-      <c r="E112" t="s">
+      <c r="F112" t="s">
         <v>581</v>
       </c>
-      <c r="F112" t="s">
+      <c r="G112" t="s">
         <v>673</v>
       </c>
-      <c r="H112" t="s">
+      <c r="I112" t="s">
         <v>743</v>
       </c>
     </row>
-    <row r="113" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A113" t="s">
         <v>218</v>
       </c>
@@ -4754,17 +4767,17 @@
       <c r="C113" t="s">
         <v>9</v>
       </c>
-      <c r="E113" t="s">
+      <c r="F113" t="s">
         <v>582</v>
       </c>
-      <c r="F113" t="s">
+      <c r="G113" t="s">
         <v>674</v>
       </c>
-      <c r="H113" t="s">
+      <c r="I113" t="s">
         <v>743</v>
       </c>
     </row>
-    <row r="114" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A114" t="s">
         <v>219</v>
       </c>
@@ -4774,17 +4787,17 @@
       <c r="C114" t="s">
         <v>11</v>
       </c>
-      <c r="E114" t="s">
+      <c r="F114" t="s">
         <v>583</v>
       </c>
-      <c r="F114" t="s">
+      <c r="G114" t="s">
         <v>675</v>
       </c>
-      <c r="H114" t="s">
+      <c r="I114" t="s">
         <v>744</v>
       </c>
     </row>
-    <row r="115" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A115" t="s">
         <v>220</v>
       </c>
@@ -4794,17 +4807,17 @@
       <c r="C115" t="s">
         <v>13</v>
       </c>
-      <c r="E115" t="s">
+      <c r="F115" t="s">
         <v>584</v>
       </c>
-      <c r="F115" t="s">
+      <c r="G115" t="s">
         <v>676</v>
       </c>
-      <c r="H115" t="s">
+      <c r="I115" t="s">
         <v>744</v>
       </c>
     </row>
-    <row r="116" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A116" t="s">
         <v>221</v>
       </c>
@@ -4814,17 +4827,17 @@
       <c r="C116" t="s">
         <v>15</v>
       </c>
-      <c r="E116" t="s">
+      <c r="F116" t="s">
         <v>585</v>
       </c>
-      <c r="F116" t="s">
+      <c r="G116" t="s">
         <v>677</v>
       </c>
-      <c r="H116" t="s">
+      <c r="I116" t="s">
         <v>744</v>
       </c>
     </row>
-    <row r="117" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A117" t="s">
         <v>222</v>
       </c>
@@ -4834,17 +4847,17 @@
       <c r="C117" t="s">
         <v>17</v>
       </c>
-      <c r="E117" t="s">
+      <c r="F117" t="s">
         <v>586</v>
       </c>
-      <c r="F117" t="s">
+      <c r="G117" t="s">
         <v>678</v>
       </c>
-      <c r="H117" t="s">
+      <c r="I117" t="s">
         <v>744</v>
       </c>
     </row>
-    <row r="118" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A118" t="s">
         <v>223</v>
       </c>
@@ -4854,17 +4867,17 @@
       <c r="C118" t="s">
         <v>19</v>
       </c>
-      <c r="E118" t="s">
+      <c r="F118" t="s">
         <v>587</v>
       </c>
-      <c r="F118" t="s">
+      <c r="G118" t="s">
         <v>679</v>
       </c>
-      <c r="H118" t="s">
+      <c r="I118" t="s">
         <v>744</v>
       </c>
     </row>
-    <row r="119" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A119" t="s">
         <v>224</v>
       </c>
@@ -4874,17 +4887,17 @@
       <c r="C119" t="s">
         <v>21</v>
       </c>
-      <c r="E119" t="s">
+      <c r="F119" t="s">
         <v>589</v>
       </c>
-      <c r="F119" t="s">
+      <c r="G119" t="s">
         <v>680</v>
       </c>
-      <c r="H119" t="s">
+      <c r="I119" t="s">
         <v>745</v>
       </c>
     </row>
-    <row r="120" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A120" t="s">
         <v>225</v>
       </c>
@@ -4894,17 +4907,17 @@
       <c r="C120" t="s">
         <v>23</v>
       </c>
-      <c r="E120" t="s">
+      <c r="F120" t="s">
         <v>590</v>
       </c>
-      <c r="F120" t="s">
+      <c r="G120" t="s">
         <v>681</v>
       </c>
-      <c r="H120" t="s">
+      <c r="I120" t="s">
         <v>781</v>
       </c>
     </row>
-    <row r="121" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A121" t="s">
         <v>226</v>
       </c>
@@ -4914,17 +4927,17 @@
       <c r="C121" t="s">
         <v>25</v>
       </c>
-      <c r="E121" t="s">
+      <c r="F121" t="s">
         <v>591</v>
       </c>
-      <c r="F121" t="s">
+      <c r="G121" t="s">
         <v>682</v>
       </c>
-      <c r="H121" t="s">
+      <c r="I121" t="s">
         <v>745</v>
       </c>
     </row>
-    <row r="122" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A122" t="s">
         <v>227</v>
       </c>
@@ -4934,17 +4947,17 @@
       <c r="C122" t="s">
         <v>27</v>
       </c>
-      <c r="E122" t="s">
+      <c r="F122" t="s">
         <v>592</v>
       </c>
-      <c r="F122" t="s">
+      <c r="G122" t="s">
         <v>683</v>
       </c>
-      <c r="H122" t="s">
+      <c r="I122" t="s">
         <v>745</v>
       </c>
     </row>
-    <row r="123" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A123" t="s">
         <v>228</v>
       </c>
@@ -4954,17 +4967,17 @@
       <c r="C123" t="s">
         <v>29</v>
       </c>
-      <c r="E123" t="s">
+      <c r="F123" t="s">
         <v>593</v>
       </c>
-      <c r="F123" t="s">
+      <c r="G123" t="s">
         <v>684</v>
       </c>
-      <c r="H123" t="s">
+      <c r="I123" t="s">
         <v>745</v>
       </c>
     </row>
-    <row r="124" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A124" t="s">
         <v>229</v>
       </c>
@@ -4974,17 +4987,17 @@
       <c r="C124" t="s">
         <v>31</v>
       </c>
-      <c r="E124" t="s">
+      <c r="F124" t="s">
         <v>594</v>
       </c>
-      <c r="F124" t="s">
+      <c r="G124" t="s">
         <v>685</v>
       </c>
-      <c r="H124" t="s">
+      <c r="I124" t="s">
         <v>746</v>
       </c>
     </row>
-    <row r="125" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A125" t="s">
         <v>230</v>
       </c>
@@ -4994,17 +5007,17 @@
       <c r="C125" t="s">
         <v>33</v>
       </c>
-      <c r="E125" t="s">
+      <c r="F125" t="s">
         <v>595</v>
       </c>
-      <c r="F125" t="s">
+      <c r="G125" t="s">
         <v>686</v>
       </c>
-      <c r="H125" t="s">
+      <c r="I125" t="s">
         <v>779</v>
       </c>
     </row>
-    <row r="126" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A126" t="s">
         <v>231</v>
       </c>
@@ -5014,17 +5027,17 @@
       <c r="C126" t="s">
         <v>35</v>
       </c>
-      <c r="E126" t="s">
+      <c r="F126" t="s">
         <v>596</v>
       </c>
-      <c r="F126" t="s">
+      <c r="G126" t="s">
         <v>687</v>
       </c>
-      <c r="H126" t="s">
+      <c r="I126" t="s">
         <v>780</v>
       </c>
     </row>
-    <row r="127" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A127" t="s">
         <v>232</v>
       </c>
@@ -5034,17 +5047,17 @@
       <c r="C127" t="s">
         <v>37</v>
       </c>
-      <c r="E127" t="s">
+      <c r="F127" t="s">
         <v>597</v>
       </c>
-      <c r="F127" t="s">
+      <c r="G127" t="s">
         <v>688</v>
       </c>
-      <c r="H127" t="s">
+      <c r="I127" t="s">
         <v>746</v>
       </c>
     </row>
-    <row r="128" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A128" t="s">
         <v>233</v>
       </c>
@@ -5054,17 +5067,17 @@
       <c r="C128" t="s">
         <v>39</v>
       </c>
-      <c r="E128" t="s">
+      <c r="F128" t="s">
         <v>598</v>
       </c>
-      <c r="F128" t="s">
+      <c r="G128" t="s">
         <v>689</v>
       </c>
-      <c r="H128" t="s">
+      <c r="I128" t="s">
         <v>746</v>
       </c>
     </row>
-    <row r="129" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A129" t="s">
         <v>234</v>
       </c>
@@ -5074,17 +5087,17 @@
       <c r="C129" t="s">
         <v>41</v>
       </c>
-      <c r="E129" t="s">
+      <c r="F129" t="s">
         <v>599</v>
       </c>
-      <c r="F129" t="s">
+      <c r="G129" t="s">
         <v>690</v>
       </c>
-      <c r="H129" t="s">
+      <c r="I129" t="s">
         <v>747</v>
       </c>
     </row>
-    <row r="130" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A130" t="s">
         <v>235</v>
       </c>
@@ -5094,17 +5107,17 @@
       <c r="C130" t="s">
         <v>43</v>
       </c>
-      <c r="E130" t="s">
+      <c r="F130" t="s">
         <v>600</v>
       </c>
-      <c r="F130" t="s">
+      <c r="G130" t="s">
         <v>691</v>
       </c>
-      <c r="H130" t="s">
+      <c r="I130" t="s">
         <v>747</v>
       </c>
     </row>
-    <row r="131" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A131" t="s">
         <v>236</v>
       </c>
@@ -5114,17 +5127,17 @@
       <c r="C131" t="s">
         <v>45</v>
       </c>
-      <c r="E131" t="s">
+      <c r="F131" t="s">
         <v>601</v>
       </c>
-      <c r="F131" t="s">
+      <c r="G131" t="s">
         <v>692</v>
       </c>
-      <c r="H131" t="s">
+      <c r="I131" t="s">
         <v>747</v>
       </c>
     </row>
-    <row r="132" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A132" t="s">
         <v>237</v>
       </c>
@@ -5134,17 +5147,17 @@
       <c r="C132" t="s">
         <v>47</v>
       </c>
-      <c r="E132" t="s">
+      <c r="F132" t="s">
         <v>602</v>
       </c>
-      <c r="F132" t="s">
+      <c r="G132" t="s">
         <v>693</v>
       </c>
-      <c r="H132" t="s">
+      <c r="I132" t="s">
         <v>747</v>
       </c>
     </row>
-    <row r="133" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A133" t="s">
         <v>238</v>
       </c>
@@ -5154,17 +5167,17 @@
       <c r="C133" t="s">
         <v>49</v>
       </c>
-      <c r="E133" t="s">
+      <c r="F133" t="s">
         <v>603</v>
       </c>
-      <c r="F133" t="s">
+      <c r="G133" t="s">
         <v>694</v>
       </c>
-      <c r="H133" t="s">
+      <c r="I133" t="s">
         <v>747</v>
       </c>
     </row>
-    <row r="134" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A134" t="s">
         <v>239</v>
       </c>
@@ -5174,17 +5187,17 @@
       <c r="C134" t="s">
         <v>51</v>
       </c>
-      <c r="E134" t="s">
+      <c r="F134" t="s">
         <v>604</v>
       </c>
-      <c r="F134" t="s">
+      <c r="G134" t="s">
         <v>695</v>
       </c>
-      <c r="H134" t="s">
+      <c r="I134" t="s">
         <v>748</v>
       </c>
     </row>
-    <row r="135" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A135" t="s">
         <v>240</v>
       </c>
@@ -5194,17 +5207,17 @@
       <c r="C135" t="s">
         <v>53</v>
       </c>
-      <c r="E135" t="s">
+      <c r="F135" t="s">
         <v>605</v>
       </c>
-      <c r="F135" t="s">
+      <c r="G135" t="s">
         <v>696</v>
       </c>
-      <c r="H135" t="s">
+      <c r="I135" t="s">
         <v>748</v>
       </c>
     </row>
-    <row r="136" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A136" t="s">
         <v>241</v>
       </c>
@@ -5214,20 +5227,20 @@
       <c r="C136" t="s">
         <v>55</v>
       </c>
-      <c r="E136" t="s">
+      <c r="F136" t="s">
         <v>606</v>
       </c>
-      <c r="F136" t="s">
+      <c r="G136" t="s">
         <v>697</v>
       </c>
-      <c r="G136" t="s">
+      <c r="H136" t="s">
         <v>794</v>
       </c>
-      <c r="H136" t="s">
+      <c r="I136" t="s">
         <v>770</v>
       </c>
     </row>
-    <row r="137" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A137" t="s">
         <v>242</v>
       </c>
@@ -5237,17 +5250,17 @@
       <c r="C137" t="s">
         <v>57</v>
       </c>
-      <c r="E137" t="s">
+      <c r="F137" t="s">
         <v>607</v>
       </c>
-      <c r="F137" t="s">
+      <c r="G137" t="s">
         <v>698</v>
       </c>
-      <c r="H137" t="s">
+      <c r="I137" t="s">
         <v>748</v>
       </c>
     </row>
-    <row r="138" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A138" t="s">
         <v>243</v>
       </c>
@@ -5257,17 +5270,17 @@
       <c r="C138" t="s">
         <v>59</v>
       </c>
-      <c r="E138" t="s">
+      <c r="F138" t="s">
         <v>608</v>
       </c>
-      <c r="F138" t="s">
+      <c r="G138" t="s">
         <v>699</v>
       </c>
-      <c r="H138" t="s">
+      <c r="I138" t="s">
         <v>748</v>
       </c>
     </row>
-    <row r="139" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A139" t="s">
         <v>244</v>
       </c>
@@ -5277,17 +5290,17 @@
       <c r="C139" t="s">
         <v>61</v>
       </c>
-      <c r="E139" t="s">
+      <c r="F139" t="s">
         <v>609</v>
       </c>
-      <c r="F139" t="s">
+      <c r="G139" t="s">
         <v>700</v>
       </c>
-      <c r="H139" t="s">
+      <c r="I139" t="s">
         <v>749</v>
       </c>
     </row>
-    <row r="140" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A140" t="s">
         <v>245</v>
       </c>
@@ -5297,17 +5310,17 @@
       <c r="C140" t="s">
         <v>63</v>
       </c>
-      <c r="E140" t="s">
+      <c r="F140" t="s">
         <v>610</v>
       </c>
-      <c r="F140" t="s">
+      <c r="G140" t="s">
         <v>701</v>
       </c>
-      <c r="H140" t="s">
+      <c r="I140" t="s">
         <v>749</v>
       </c>
     </row>
-    <row r="141" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A141" t="s">
         <v>246</v>
       </c>
@@ -5317,17 +5330,17 @@
       <c r="C141" t="s">
         <v>65</v>
       </c>
-      <c r="E141" t="s">
+      <c r="F141" t="s">
         <v>611</v>
       </c>
-      <c r="F141" t="s">
+      <c r="G141" t="s">
         <v>702</v>
       </c>
-      <c r="H141" t="s">
+      <c r="I141" t="s">
         <v>749</v>
       </c>
     </row>
-    <row r="142" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A142" t="s">
         <v>247</v>
       </c>
@@ -5337,17 +5350,17 @@
       <c r="C142" t="s">
         <v>67</v>
       </c>
-      <c r="E142" t="s">
+      <c r="F142" t="s">
         <v>612</v>
       </c>
-      <c r="F142" t="s">
+      <c r="G142" t="s">
         <v>703</v>
       </c>
-      <c r="H142" t="s">
+      <c r="I142" t="s">
         <v>749</v>
       </c>
     </row>
-    <row r="143" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A143" t="s">
         <v>248</v>
       </c>
@@ -5357,17 +5370,17 @@
       <c r="C143" t="s">
         <v>69</v>
       </c>
-      <c r="E143" t="s">
+      <c r="F143" t="s">
         <v>613</v>
       </c>
-      <c r="F143" t="s">
+      <c r="G143" t="s">
         <v>704</v>
       </c>
-      <c r="H143" t="s">
+      <c r="I143" t="s">
         <v>749</v>
       </c>
     </row>
-    <row r="144" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A144" t="s">
         <v>249</v>
       </c>
@@ -5377,17 +5390,17 @@
       <c r="C144" t="s">
         <v>71</v>
       </c>
-      <c r="E144" t="s">
+      <c r="F144" t="s">
         <v>614</v>
       </c>
-      <c r="F144" t="s">
+      <c r="G144" t="s">
         <v>705</v>
       </c>
-      <c r="H144" t="s">
+      <c r="I144" t="s">
         <v>750</v>
       </c>
     </row>
-    <row r="145" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A145" t="s">
         <v>250</v>
       </c>
@@ -5397,17 +5410,17 @@
       <c r="C145" t="s">
         <v>73</v>
       </c>
-      <c r="E145" t="s">
+      <c r="F145" t="s">
         <v>615</v>
       </c>
-      <c r="F145" t="s">
+      <c r="G145" t="s">
         <v>706</v>
       </c>
-      <c r="H145" t="s">
+      <c r="I145" t="s">
         <v>750</v>
       </c>
     </row>
-    <row r="146" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A146" t="s">
         <v>251</v>
       </c>
@@ -5417,17 +5430,17 @@
       <c r="C146" t="s">
         <v>75</v>
       </c>
-      <c r="E146" t="s">
+      <c r="F146" t="s">
         <v>616</v>
       </c>
-      <c r="F146" t="s">
+      <c r="G146" t="s">
         <v>707</v>
       </c>
-      <c r="H146" t="s">
+      <c r="I146" t="s">
         <v>750</v>
       </c>
     </row>
-    <row r="147" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A147" t="s">
         <v>252</v>
       </c>
@@ -5437,20 +5450,20 @@
       <c r="C147" t="s">
         <v>77</v>
       </c>
-      <c r="E147" t="s">
+      <c r="F147" t="s">
         <v>617</v>
       </c>
-      <c r="F147" t="s">
+      <c r="G147" t="s">
         <v>708</v>
       </c>
-      <c r="G147" t="s">
+      <c r="H147" t="s">
         <v>795</v>
       </c>
-      <c r="H147" t="s">
+      <c r="I147" t="s">
         <v>751</v>
       </c>
     </row>
-    <row r="148" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="148" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A148" t="s">
         <v>253</v>
       </c>
@@ -5460,20 +5473,20 @@
       <c r="C148" t="s">
         <v>79</v>
       </c>
-      <c r="E148" t="s">
+      <c r="F148" t="s">
         <v>618</v>
       </c>
-      <c r="F148" t="s">
+      <c r="G148" t="s">
         <v>709</v>
       </c>
-      <c r="G148" t="s">
+      <c r="H148" t="s">
         <v>795</v>
       </c>
-      <c r="H148" t="s">
+      <c r="I148" t="s">
         <v>751</v>
       </c>
     </row>
-    <row r="149" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="149" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A149" t="s">
         <v>254</v>
       </c>
@@ -5483,20 +5496,20 @@
       <c r="C149" t="s">
         <v>81</v>
       </c>
-      <c r="E149" t="s">
+      <c r="F149" t="s">
         <v>619</v>
       </c>
-      <c r="F149" t="s">
+      <c r="G149" t="s">
         <v>710</v>
       </c>
-      <c r="G149" t="s">
+      <c r="H149" t="s">
         <v>795</v>
       </c>
-      <c r="H149" t="s">
+      <c r="I149" t="s">
         <v>751</v>
       </c>
     </row>
-    <row r="150" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="150" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A150" t="s">
         <v>255</v>
       </c>
@@ -5506,20 +5519,20 @@
       <c r="C150" t="s">
         <v>83</v>
       </c>
-      <c r="E150" t="s">
+      <c r="F150" t="s">
         <v>620</v>
       </c>
-      <c r="F150" t="s">
+      <c r="G150" t="s">
         <v>711</v>
       </c>
-      <c r="G150" t="s">
+      <c r="H150" t="s">
         <v>795</v>
       </c>
-      <c r="H150" t="s">
+      <c r="I150" t="s">
         <v>751</v>
       </c>
     </row>
-    <row r="151" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="151" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A151" t="s">
         <v>256</v>
       </c>
@@ -5529,20 +5542,20 @@
       <c r="C151" t="s">
         <v>85</v>
       </c>
-      <c r="E151" t="s">
+      <c r="F151" t="s">
         <v>621</v>
       </c>
-      <c r="F151" t="s">
+      <c r="G151" t="s">
         <v>712</v>
       </c>
-      <c r="G151" t="s">
+      <c r="H151" t="s">
         <v>795</v>
       </c>
-      <c r="H151" t="s">
+      <c r="I151" t="s">
         <v>751</v>
       </c>
     </row>
-    <row r="152" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="152" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A152" t="s">
         <v>257</v>
       </c>
@@ -5552,17 +5565,17 @@
       <c r="C152" t="s">
         <v>87</v>
       </c>
-      <c r="E152" t="s">
+      <c r="F152" t="s">
         <v>622</v>
       </c>
-      <c r="F152" t="s">
+      <c r="G152" t="s">
         <v>713</v>
       </c>
-      <c r="H152" t="s">
+      <c r="I152" t="s">
         <v>752</v>
       </c>
     </row>
-    <row r="153" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="153" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A153" t="s">
         <v>258</v>
       </c>
@@ -5575,11 +5588,11 @@
       <c r="D153">
         <v>1</v>
       </c>
-      <c r="H153" t="s">
+      <c r="I153" t="s">
         <v>752</v>
       </c>
     </row>
-    <row r="154" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="154" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A154" t="s">
         <v>259</v>
       </c>
@@ -5589,20 +5602,20 @@
       <c r="C154" t="s">
         <v>91</v>
       </c>
-      <c r="E154" t="s">
+      <c r="F154" t="s">
         <v>623</v>
       </c>
-      <c r="F154" t="s">
+      <c r="G154" t="s">
         <v>714</v>
       </c>
-      <c r="G154" s="1" t="s">
-        <v>797</v>
-      </c>
-      <c r="H154" t="s">
+      <c r="H154" s="1" t="s">
+        <v>799</v>
+      </c>
+      <c r="I154" t="s">
         <v>752</v>
       </c>
     </row>
-    <row r="155" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="155" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A155" t="s">
         <v>260</v>
       </c>
@@ -5612,11 +5625,11 @@
       <c r="C155" t="s">
         <v>93</v>
       </c>
-      <c r="H155" t="s">
+      <c r="I155" t="s">
         <v>753</v>
       </c>
     </row>
-    <row r="156" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="156" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A156" t="s">
         <v>261</v>
       </c>
@@ -5626,11 +5639,11 @@
       <c r="C156" t="s">
         <v>95</v>
       </c>
-      <c r="H156" t="s">
+      <c r="I156" t="s">
         <v>753</v>
       </c>
     </row>
-    <row r="157" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="157" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A157" t="s">
         <v>262</v>
       </c>
@@ -5640,11 +5653,11 @@
       <c r="C157" t="s">
         <v>97</v>
       </c>
-      <c r="H157" t="s">
+      <c r="I157" t="s">
         <v>753</v>
       </c>
     </row>
-    <row r="158" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="158" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A158" t="s">
         <v>263</v>
       </c>
@@ -5654,11 +5667,11 @@
       <c r="C158" t="s">
         <v>99</v>
       </c>
-      <c r="H158" t="s">
+      <c r="I158" t="s">
         <v>753</v>
       </c>
     </row>
-    <row r="159" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="159" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A159" t="s">
         <v>264</v>
       </c>
@@ -5668,11 +5681,11 @@
       <c r="C159" t="s">
         <v>101</v>
       </c>
-      <c r="H159" t="s">
+      <c r="I159" t="s">
         <v>753</v>
       </c>
     </row>
-    <row r="160" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="160" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A160" t="s">
         <v>265</v>
       </c>
@@ -5682,11 +5695,14 @@
       <c r="C160" t="s">
         <v>103</v>
       </c>
-      <c r="H160" t="s">
+      <c r="E160" t="s">
+        <v>798</v>
+      </c>
+      <c r="I160" t="s">
         <v>754</v>
       </c>
     </row>
-    <row r="161" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="161" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A161" t="s">
         <v>266</v>
       </c>
@@ -5699,11 +5715,11 @@
       <c r="D161">
         <v>1</v>
       </c>
-      <c r="H161" t="s">
+      <c r="I161" t="s">
         <v>790</v>
       </c>
     </row>
-    <row r="162" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="162" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A162" t="s">
         <v>267</v>
       </c>
@@ -5716,11 +5732,11 @@
       <c r="D162">
         <v>1</v>
       </c>
-      <c r="H162" t="s">
+      <c r="I162" t="s">
         <v>754</v>
       </c>
     </row>
-    <row r="163" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="163" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A163" t="s">
         <v>268</v>
       </c>
@@ -5730,11 +5746,11 @@
       <c r="C163" t="s">
         <v>109</v>
       </c>
-      <c r="H163" t="s">
+      <c r="I163" t="s">
         <v>754</v>
       </c>
     </row>
-    <row r="164" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="164" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A164" t="s">
         <v>269</v>
       </c>
@@ -5744,11 +5760,11 @@
       <c r="C164" t="s">
         <v>111</v>
       </c>
-      <c r="H164" t="s">
+      <c r="I164" t="s">
         <v>754</v>
       </c>
     </row>
-    <row r="165" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="165" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A165" t="s">
         <v>270</v>
       </c>
@@ -5758,14 +5774,14 @@
       <c r="C165" t="s">
         <v>113</v>
       </c>
-      <c r="G165" t="s">
+      <c r="H165" t="s">
         <v>796</v>
       </c>
-      <c r="H165" t="s">
+      <c r="I165" t="s">
         <v>755</v>
       </c>
     </row>
-    <row r="166" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="166" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A166" t="s">
         <v>271</v>
       </c>
@@ -5778,11 +5794,11 @@
       <c r="D166">
         <v>1</v>
       </c>
-      <c r="H166" t="s">
+      <c r="I166" t="s">
         <v>755</v>
       </c>
     </row>
-    <row r="167" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="167" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A167" t="s">
         <v>272</v>
       </c>
@@ -5795,11 +5811,11 @@
       <c r="D167">
         <v>1</v>
       </c>
-      <c r="H167" t="s">
+      <c r="I167" t="s">
         <v>755</v>
       </c>
     </row>
-    <row r="168" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="168" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A168" t="s">
         <v>273</v>
       </c>
@@ -5809,14 +5825,14 @@
       <c r="C168" t="s">
         <v>119</v>
       </c>
-      <c r="G168" t="s">
+      <c r="H168" t="s">
         <v>796</v>
       </c>
-      <c r="H168" t="s">
+      <c r="I168" t="s">
         <v>755</v>
       </c>
     </row>
-    <row r="169" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="169" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A169" t="s">
         <v>274</v>
       </c>
@@ -5826,14 +5842,14 @@
       <c r="C169" t="s">
         <v>121</v>
       </c>
-      <c r="G169" t="s">
+      <c r="H169" t="s">
         <v>796</v>
       </c>
-      <c r="H169" t="s">
+      <c r="I169" t="s">
         <v>755</v>
       </c>
     </row>
-    <row r="170" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="170" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A170" t="s">
         <v>275</v>
       </c>
@@ -5843,11 +5859,11 @@
       <c r="C170" t="s">
         <v>123</v>
       </c>
-      <c r="H170" t="s">
+      <c r="I170" t="s">
         <v>756</v>
       </c>
     </row>
-    <row r="171" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="171" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A171" t="s">
         <v>276</v>
       </c>
@@ -5857,11 +5873,11 @@
       <c r="C171" t="s">
         <v>125</v>
       </c>
-      <c r="H171" t="s">
+      <c r="I171" t="s">
         <v>756</v>
       </c>
     </row>
-    <row r="172" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="172" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A172" t="s">
         <v>277</v>
       </c>
@@ -5871,11 +5887,11 @@
       <c r="C172" t="s">
         <v>127</v>
       </c>
-      <c r="H172" t="s">
+      <c r="I172" t="s">
         <v>756</v>
       </c>
     </row>
-    <row r="173" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="173" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A173" t="s">
         <v>278</v>
       </c>
@@ -5885,11 +5901,11 @@
       <c r="C173" t="s">
         <v>129</v>
       </c>
-      <c r="H173" t="s">
+      <c r="I173" t="s">
         <v>756</v>
       </c>
     </row>
-    <row r="174" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="174" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A174" t="s">
         <v>279</v>
       </c>
@@ -5899,11 +5915,11 @@
       <c r="C174" t="s">
         <v>131</v>
       </c>
-      <c r="H174" t="s">
+      <c r="I174" t="s">
         <v>756</v>
       </c>
     </row>
-    <row r="175" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="175" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A175" t="s">
         <v>280</v>
       </c>
@@ -5913,11 +5929,11 @@
       <c r="C175" t="s">
         <v>133</v>
       </c>
-      <c r="H175" t="s">
+      <c r="I175" t="s">
         <v>757</v>
       </c>
     </row>
-    <row r="176" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="176" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A176" t="s">
         <v>281</v>
       </c>
@@ -5927,11 +5943,11 @@
       <c r="C176" t="s">
         <v>135</v>
       </c>
-      <c r="H176" t="s">
+      <c r="I176" t="s">
         <v>757</v>
       </c>
     </row>
-    <row r="177" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="177" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A177" t="s">
         <v>282</v>
       </c>
@@ -5941,11 +5957,11 @@
       <c r="C177" t="s">
         <v>137</v>
       </c>
-      <c r="H177" t="s">
+      <c r="I177" t="s">
         <v>757</v>
       </c>
     </row>
-    <row r="178" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="178" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A178" t="s">
         <v>283</v>
       </c>
@@ -5955,11 +5971,11 @@
       <c r="C178" t="s">
         <v>139</v>
       </c>
-      <c r="H178" t="s">
+      <c r="I178" t="s">
         <v>757</v>
       </c>
     </row>
-    <row r="179" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="179" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A179" t="s">
         <v>284</v>
       </c>
@@ -5969,11 +5985,11 @@
       <c r="C179" t="s">
         <v>141</v>
       </c>
-      <c r="H179" t="s">
+      <c r="I179" t="s">
         <v>757</v>
       </c>
     </row>
-    <row r="180" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="180" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A180" t="s">
         <v>285</v>
       </c>
@@ -5983,11 +5999,11 @@
       <c r="C180" t="s">
         <v>143</v>
       </c>
-      <c r="H180" t="s">
+      <c r="I180" t="s">
         <v>758</v>
       </c>
     </row>
-    <row r="181" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="181" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A181" t="s">
         <v>286</v>
       </c>
@@ -5997,11 +6013,11 @@
       <c r="C181" t="s">
         <v>145</v>
       </c>
-      <c r="H181" t="s">
+      <c r="I181" t="s">
         <v>758</v>
       </c>
     </row>
-    <row r="182" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="182" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A182" t="s">
         <v>287</v>
       </c>
@@ -6011,11 +6027,11 @@
       <c r="C182" t="s">
         <v>147</v>
       </c>
-      <c r="H182" t="s">
+      <c r="I182" t="s">
         <v>758</v>
       </c>
     </row>
-    <row r="183" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="183" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A183" t="s">
         <v>288</v>
       </c>
@@ -6025,11 +6041,11 @@
       <c r="C183" t="s">
         <v>149</v>
       </c>
-      <c r="H183" t="s">
+      <c r="I183" t="s">
         <v>759</v>
       </c>
     </row>
-    <row r="184" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="184" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A184" t="s">
         <v>289</v>
       </c>
@@ -6039,11 +6055,11 @@
       <c r="C184" t="s">
         <v>151</v>
       </c>
-      <c r="H184" t="s">
+      <c r="I184" t="s">
         <v>759</v>
       </c>
     </row>
-    <row r="185" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="185" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A185" t="s">
         <v>290</v>
       </c>
@@ -6053,11 +6069,11 @@
       <c r="C185" t="s">
         <v>153</v>
       </c>
-      <c r="H185" t="s">
+      <c r="I185" t="s">
         <v>759</v>
       </c>
     </row>
-    <row r="186" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="186" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A186" t="s">
         <v>291</v>
       </c>
@@ -6067,11 +6083,11 @@
       <c r="C186" t="s">
         <v>155</v>
       </c>
-      <c r="H186" t="s">
+      <c r="I186" t="s">
         <v>760</v>
       </c>
     </row>
-    <row r="187" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="187" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A187" t="s">
         <v>292</v>
       </c>
@@ -6081,11 +6097,11 @@
       <c r="C187" t="s">
         <v>157</v>
       </c>
-      <c r="H187" t="s">
+      <c r="I187" t="s">
         <v>760</v>
       </c>
     </row>
-    <row r="188" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="188" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A188" t="s">
         <v>293</v>
       </c>
@@ -6095,11 +6111,11 @@
       <c r="C188" t="s">
         <v>159</v>
       </c>
-      <c r="H188" t="s">
+      <c r="I188" t="s">
         <v>760</v>
       </c>
     </row>
-    <row r="189" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="189" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A189" t="s">
         <v>294</v>
       </c>
@@ -6109,11 +6125,11 @@
       <c r="C189" t="s">
         <v>161</v>
       </c>
-      <c r="H189" t="s">
+      <c r="I189" t="s">
         <v>761</v>
       </c>
     </row>
-    <row r="190" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="190" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A190" t="s">
         <v>295</v>
       </c>
@@ -6123,11 +6139,11 @@
       <c r="C190" t="s">
         <v>163</v>
       </c>
-      <c r="H190" t="s">
+      <c r="I190" t="s">
         <v>761</v>
       </c>
     </row>
-    <row r="191" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="191" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A191" t="s">
         <v>296</v>
       </c>
@@ -6137,11 +6153,11 @@
       <c r="C191" t="s">
         <v>165</v>
       </c>
-      <c r="H191" t="s">
+      <c r="I191" t="s">
         <v>761</v>
       </c>
     </row>
-    <row r="192" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="192" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A192" t="s">
         <v>297</v>
       </c>
@@ -6151,11 +6167,11 @@
       <c r="C192" t="s">
         <v>167</v>
       </c>
-      <c r="H192" t="s">
+      <c r="I192" t="s">
         <v>762</v>
       </c>
     </row>
-    <row r="193" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="193" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A193" t="s">
         <v>298</v>
       </c>
@@ -6165,11 +6181,11 @@
       <c r="C193" t="s">
         <v>169</v>
       </c>
-      <c r="H193" t="s">
+      <c r="I193" t="s">
         <v>762</v>
       </c>
     </row>
-    <row r="194" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="194" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A194" t="s">
         <v>299</v>
       </c>
@@ -6179,11 +6195,11 @@
       <c r="C194" t="s">
         <v>171</v>
       </c>
-      <c r="H194" t="s">
+      <c r="I194" t="s">
         <v>762</v>
       </c>
     </row>
-    <row r="195" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="195" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A195" t="s">
         <v>300</v>
       </c>
@@ -6193,11 +6209,11 @@
       <c r="C195" t="s">
         <v>173</v>
       </c>
-      <c r="H195" t="s">
+      <c r="I195" t="s">
         <v>763</v>
       </c>
     </row>
-    <row r="196" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="196" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A196" t="s">
         <v>301</v>
       </c>
@@ -6207,11 +6223,11 @@
       <c r="C196" t="s">
         <v>175</v>
       </c>
-      <c r="H196" t="s">
+      <c r="I196" t="s">
         <v>763</v>
       </c>
     </row>
-    <row r="197" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="197" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A197" t="s">
         <v>302</v>
       </c>
@@ -6221,11 +6237,11 @@
       <c r="C197" t="s">
         <v>177</v>
       </c>
-      <c r="H197" t="s">
+      <c r="I197" t="s">
         <v>763</v>
       </c>
     </row>
-    <row r="198" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="198" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A198" t="s">
         <v>303</v>
       </c>
@@ -6235,11 +6251,11 @@
       <c r="C198" t="s">
         <v>179</v>
       </c>
-      <c r="H198" t="s">
+      <c r="I198" t="s">
         <v>764</v>
       </c>
     </row>
-    <row r="199" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="199" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A199" t="s">
         <v>304</v>
       </c>
@@ -6252,11 +6268,11 @@
       <c r="D199">
         <v>1</v>
       </c>
-      <c r="H199" t="s">
+      <c r="I199" t="s">
         <v>764</v>
       </c>
     </row>
-    <row r="200" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="200" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A200" t="s">
         <v>305</v>
       </c>
@@ -6266,11 +6282,11 @@
       <c r="C200" t="s">
         <v>183</v>
       </c>
-      <c r="H200" t="s">
+      <c r="I200" t="s">
         <v>764</v>
       </c>
     </row>
-    <row r="201" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="201" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A201" t="s">
         <v>306</v>
       </c>
@@ -6280,11 +6296,11 @@
       <c r="C201" t="s">
         <v>185</v>
       </c>
-      <c r="H201" t="s">
+      <c r="I201" t="s">
         <v>765</v>
       </c>
     </row>
-    <row r="202" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="202" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A202" t="s">
         <v>307</v>
       </c>
@@ -6294,11 +6310,11 @@
       <c r="C202" t="s">
         <v>187</v>
       </c>
-      <c r="H202" t="s">
+      <c r="I202" t="s">
         <v>765</v>
       </c>
     </row>
-    <row r="203" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="203" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A203" t="s">
         <v>308</v>
       </c>
@@ -6308,11 +6324,11 @@
       <c r="C203" t="s">
         <v>189</v>
       </c>
-      <c r="H203" t="s">
+      <c r="I203" t="s">
         <v>765</v>
       </c>
     </row>
-    <row r="204" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="204" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A204" t="s">
         <v>309</v>
       </c>
@@ -6325,11 +6341,11 @@
       <c r="D204">
         <v>1</v>
       </c>
-      <c r="H204" t="s">
+      <c r="I204" t="s">
         <v>766</v>
       </c>
     </row>
-    <row r="205" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="205" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A205" t="s">
         <v>310</v>
       </c>
@@ -6342,11 +6358,11 @@
       <c r="D205">
         <v>1</v>
       </c>
-      <c r="H205" t="s">
+      <c r="I205" t="s">
         <v>766</v>
       </c>
     </row>
-    <row r="206" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="206" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A206" t="s">
         <v>311</v>
       </c>
@@ -6359,11 +6375,11 @@
       <c r="D206">
         <v>1</v>
       </c>
-      <c r="H206" t="s">
+      <c r="I206" t="s">
         <v>766</v>
       </c>
     </row>
-    <row r="207" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="207" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A207" t="s">
         <v>312</v>
       </c>
@@ -6376,11 +6392,11 @@
       <c r="D207">
         <v>1</v>
       </c>
-      <c r="H207" t="s">
+      <c r="I207" t="s">
         <v>767</v>
       </c>
     </row>
-    <row r="208" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="208" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A208" t="s">
         <v>313</v>
       </c>
@@ -6393,11 +6409,11 @@
       <c r="D208">
         <v>1</v>
       </c>
-      <c r="H208" t="s">
+      <c r="I208" t="s">
         <v>767</v>
       </c>
     </row>
-    <row r="209" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="209" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A209" t="s">
         <v>314</v>
       </c>
@@ -6410,11 +6426,11 @@
       <c r="D209">
         <v>1</v>
       </c>
-      <c r="H209" t="s">
+      <c r="I209" t="s">
         <v>767</v>
       </c>
     </row>
-    <row r="210" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="210" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A210" t="s">
         <v>315</v>
       </c>
@@ -6424,11 +6440,11 @@
       <c r="C210" t="s">
         <v>203</v>
       </c>
-      <c r="H210" t="s">
+      <c r="I210" t="s">
         <v>768</v>
       </c>
     </row>
-    <row r="211" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="211" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A211" t="s">
         <v>316</v>
       </c>
@@ -6438,11 +6454,11 @@
       <c r="C211" t="s">
         <v>205</v>
       </c>
-      <c r="H211" t="s">
+      <c r="I211" t="s">
         <v>768</v>
       </c>
     </row>
-    <row r="212" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="212" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A212" t="s">
         <v>317</v>
       </c>
@@ -6452,11 +6468,11 @@
       <c r="C212" t="s">
         <v>207</v>
       </c>
-      <c r="H212" t="s">
+      <c r="I212" t="s">
         <v>768</v>
       </c>
     </row>
-    <row r="213" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="213" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A213" t="s">
         <v>318</v>
       </c>
@@ -6466,11 +6482,11 @@
       <c r="C213" t="s">
         <v>209</v>
       </c>
-      <c r="H213" t="s">
+      <c r="I213" t="s">
         <v>769</v>
       </c>
     </row>
-    <row r="214" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="214" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A214" t="s">
         <v>319</v>
       </c>
@@ -6480,11 +6496,11 @@
       <c r="C214" t="s">
         <v>211</v>
       </c>
-      <c r="H214" t="s">
+      <c r="I214" t="s">
         <v>769</v>
       </c>
     </row>
-    <row r="215" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="215" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A215" t="s">
         <v>320</v>
       </c>
@@ -6494,11 +6510,11 @@
       <c r="C215" t="s">
         <v>213</v>
       </c>
-      <c r="H215" t="s">
+      <c r="I215" t="s">
         <v>769</v>
       </c>
     </row>
-    <row r="216" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="216" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A216" t="s">
         <v>321</v>
       </c>
@@ -6508,11 +6524,11 @@
       <c r="D216">
         <v>1</v>
       </c>
-      <c r="H216" t="s">
+      <c r="I216" t="s">
         <v>774</v>
       </c>
     </row>
-    <row r="217" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="217" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A217" t="s">
         <v>323</v>
       </c>
@@ -6522,11 +6538,11 @@
       <c r="D217">
         <v>1</v>
       </c>
-      <c r="H217" t="s">
+      <c r="I217" t="s">
         <v>774</v>
       </c>
     </row>
-    <row r="218" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="218" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A218" t="s">
         <v>325</v>
       </c>
@@ -6536,11 +6552,11 @@
       <c r="D218">
         <v>1</v>
       </c>
-      <c r="H218" t="s">
+      <c r="I218" t="s">
         <v>775</v>
       </c>
     </row>
-    <row r="219" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="219" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A219" t="s">
         <v>327</v>
       </c>
@@ -6550,11 +6566,11 @@
       <c r="D219">
         <v>1</v>
       </c>
-      <c r="H219" t="s">
+      <c r="I219" t="s">
         <v>775</v>
       </c>
     </row>
-    <row r="220" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="220" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A220" t="s">
         <v>329</v>
       </c>
@@ -6564,11 +6580,11 @@
       <c r="D220">
         <v>1</v>
       </c>
-      <c r="H220" t="s">
+      <c r="I220" t="s">
         <v>775</v>
       </c>
     </row>
-    <row r="221" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="221" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A221" t="s">
         <v>331</v>
       </c>
@@ -6581,11 +6597,11 @@
       <c r="D221">
         <v>1</v>
       </c>
-      <c r="H221" t="s">
+      <c r="I221" t="s">
         <v>771</v>
       </c>
     </row>
-    <row r="222" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="222" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A222" t="s">
         <v>333</v>
       </c>
@@ -6598,11 +6614,11 @@
       <c r="D222">
         <v>1</v>
       </c>
-      <c r="H222" t="s">
+      <c r="I222" t="s">
         <v>771</v>
       </c>
     </row>
-    <row r="223" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="223" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A223" t="s">
         <v>335</v>
       </c>
@@ -6612,11 +6628,11 @@
       <c r="D223">
         <v>1</v>
       </c>
-      <c r="H223" t="s">
+      <c r="I223" t="s">
         <v>771</v>
       </c>
     </row>
-    <row r="224" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="224" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A224" t="s">
         <v>337</v>
       </c>
@@ -6629,11 +6645,11 @@
       <c r="D224">
         <v>1</v>
       </c>
-      <c r="H224" t="s">
+      <c r="I224" t="s">
         <v>771</v>
       </c>
     </row>
-    <row r="225" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="225" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A225" t="s">
         <v>339</v>
       </c>
@@ -6646,11 +6662,11 @@
       <c r="D225">
         <v>1</v>
       </c>
-      <c r="H225" t="s">
+      <c r="I225" t="s">
         <v>771</v>
       </c>
     </row>
-    <row r="226" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="226" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A226" t="s">
         <v>341</v>
       </c>
@@ -6660,11 +6676,11 @@
       <c r="D226">
         <v>1</v>
       </c>
-      <c r="H226" t="s">
+      <c r="I226" t="s">
         <v>776</v>
       </c>
     </row>
-    <row r="227" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="227" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A227" t="s">
         <v>343</v>
       </c>
@@ -6677,11 +6693,11 @@
       <c r="D227">
         <v>1</v>
       </c>
-      <c r="H227" t="s">
+      <c r="I227" t="s">
         <v>772</v>
       </c>
     </row>
-    <row r="228" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="228" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A228" t="s">
         <v>345</v>
       </c>
@@ -6691,11 +6707,11 @@
       <c r="D228">
         <v>1</v>
       </c>
-      <c r="H228" t="s">
+      <c r="I228" t="s">
         <v>777</v>
       </c>
     </row>
-    <row r="229" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="229" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A229" t="s">
         <v>347</v>
       </c>
@@ -6708,11 +6724,11 @@
       <c r="D229">
         <v>1</v>
       </c>
-      <c r="H229" t="s">
+      <c r="I229" t="s">
         <v>778</v>
       </c>
     </row>
-    <row r="230" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="230" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A230" t="s">
         <v>349</v>
       </c>
@@ -6725,11 +6741,11 @@
       <c r="D230">
         <v>1</v>
       </c>
-      <c r="H230" t="s">
+      <c r="I230" t="s">
         <v>778</v>
       </c>
     </row>
-    <row r="231" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="231" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A231" t="s">
         <v>351</v>
       </c>
@@ -6742,11 +6758,11 @@
       <c r="D231">
         <v>1</v>
       </c>
-      <c r="H231" t="s">
+      <c r="I231" t="s">
         <v>773</v>
       </c>
     </row>
-    <row r="232" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="232" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A232" t="s">
         <v>353</v>
       </c>
@@ -6759,11 +6775,11 @@
       <c r="D232">
         <v>1</v>
       </c>
-      <c r="H232" t="s">
+      <c r="I232" t="s">
         <v>773</v>
       </c>
     </row>
-    <row r="233" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="233" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A233" t="s">
         <v>355</v>
       </c>
@@ -6776,11 +6792,11 @@
       <c r="D233">
         <v>1</v>
       </c>
-      <c r="H233" t="s">
+      <c r="I233" t="s">
         <v>782</v>
       </c>
     </row>
-    <row r="234" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="234" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A234" t="s">
         <v>357</v>
       </c>
@@ -6790,11 +6806,11 @@
       <c r="D234">
         <v>1</v>
       </c>
-      <c r="H234" t="s">
+      <c r="I234" t="s">
         <v>782</v>
       </c>
     </row>
-    <row r="235" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="235" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A235" t="s">
         <v>359</v>
       </c>
@@ -6807,11 +6823,11 @@
       <c r="D235">
         <v>1</v>
       </c>
-      <c r="H235" t="s">
+      <c r="I235" t="s">
         <v>782</v>
       </c>
     </row>
-    <row r="236" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="236" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A236" t="s">
         <v>361</v>
       </c>
@@ -6824,11 +6840,11 @@
       <c r="D236">
         <v>1</v>
       </c>
-      <c r="H236" t="s">
+      <c r="I236" t="s">
         <v>782</v>
       </c>
     </row>
-    <row r="237" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="237" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A237" t="s">
         <v>363</v>
       </c>
@@ -6841,11 +6857,11 @@
       <c r="D237">
         <v>1</v>
       </c>
-      <c r="H237" t="s">
+      <c r="I237" t="s">
         <v>783</v>
       </c>
     </row>
-    <row r="238" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="238" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A238" t="s">
         <v>365</v>
       </c>
@@ -6858,11 +6874,11 @@
       <c r="D238">
         <v>1</v>
       </c>
-      <c r="H238" t="s">
+      <c r="I238" t="s">
         <v>783</v>
       </c>
     </row>
-    <row r="239" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="239" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A239" t="s">
         <v>367</v>
       </c>
@@ -6875,11 +6891,11 @@
       <c r="D239">
         <v>1</v>
       </c>
-      <c r="H239" t="s">
+      <c r="I239" t="s">
         <v>783</v>
       </c>
     </row>
-    <row r="240" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="240" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A240" t="s">
         <v>369</v>
       </c>
@@ -6892,11 +6908,11 @@
       <c r="D240">
         <v>1</v>
       </c>
-      <c r="H240" t="s">
+      <c r="I240" t="s">
         <v>783</v>
       </c>
     </row>
-    <row r="241" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="241" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A241" t="s">
         <v>371</v>
       </c>
@@ -6906,11 +6922,11 @@
       <c r="D241">
         <v>1</v>
       </c>
-      <c r="H241" t="s">
+      <c r="I241" t="s">
         <v>784</v>
       </c>
     </row>
-    <row r="242" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="242" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A242" t="s">
         <v>373</v>
       </c>
@@ -6920,11 +6936,11 @@
       <c r="D242">
         <v>1</v>
       </c>
-      <c r="H242" t="s">
+      <c r="I242" t="s">
         <v>784</v>
       </c>
     </row>
-    <row r="243" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="243" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A243" t="s">
         <v>375</v>
       </c>
@@ -6934,11 +6950,11 @@
       <c r="D243">
         <v>1</v>
       </c>
-      <c r="H243" t="s">
+      <c r="I243" t="s">
         <v>784</v>
       </c>
     </row>
-    <row r="244" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="244" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A244" t="s">
         <v>377</v>
       </c>
@@ -6948,11 +6964,11 @@
       <c r="D244">
         <v>1</v>
       </c>
-      <c r="H244" t="s">
+      <c r="I244" t="s">
         <v>785</v>
       </c>
     </row>
-    <row r="245" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="245" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A245" t="s">
         <v>379</v>
       </c>
@@ -6965,11 +6981,11 @@
       <c r="D245">
         <v>1</v>
       </c>
-      <c r="H245" t="s">
+      <c r="I245" t="s">
         <v>786</v>
       </c>
     </row>
-    <row r="246" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="246" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A246" t="s">
         <v>380</v>
       </c>
@@ -6979,11 +6995,11 @@
       <c r="D246">
         <v>1</v>
       </c>
-      <c r="H246" t="s">
+      <c r="I246" t="s">
         <v>792</v>
       </c>
     </row>
-    <row r="247" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="247" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A247" t="s">
         <v>382</v>
       </c>
@@ -6993,11 +7009,11 @@
       <c r="D247">
         <v>1</v>
       </c>
-      <c r="H247" t="s">
+      <c r="I247" t="s">
         <v>787</v>
       </c>
     </row>
-    <row r="248" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="248" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A248" t="s">
         <v>384</v>
       </c>
@@ -7007,11 +7023,11 @@
       <c r="D248">
         <v>1</v>
       </c>
-      <c r="H248" t="s">
+      <c r="I248" t="s">
         <v>788</v>
       </c>
     </row>
-    <row r="249" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="249" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A249" t="s">
         <v>386</v>
       </c>
@@ -7021,11 +7037,11 @@
       <c r="D249">
         <v>1</v>
       </c>
-      <c r="H249" t="s">
+      <c r="I249" t="s">
         <v>787</v>
       </c>
     </row>
-    <row r="250" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="250" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A250" t="s">
         <v>388</v>
       </c>
@@ -7035,11 +7051,11 @@
       <c r="D250">
         <v>1</v>
       </c>
-      <c r="H250" t="s">
+      <c r="I250" t="s">
         <v>787</v>
       </c>
     </row>
-    <row r="251" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="251" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A251" t="s">
         <v>390</v>
       </c>
@@ -7049,11 +7065,11 @@
       <c r="D251">
         <v>1</v>
       </c>
-      <c r="H251" t="s">
+      <c r="I251" t="s">
         <v>787</v>
       </c>
     </row>
-    <row r="252" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="252" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A252" t="s">
         <v>392</v>
       </c>
@@ -7063,11 +7079,11 @@
       <c r="D252">
         <v>1</v>
       </c>
-      <c r="H252" t="s">
+      <c r="I252" t="s">
         <v>791</v>
       </c>
     </row>
-    <row r="253" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="253" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A253" t="s">
         <v>394</v>
       </c>
@@ -7077,11 +7093,11 @@
       <c r="D253">
         <v>1</v>
       </c>
-      <c r="H253" t="s">
+      <c r="I253" t="s">
         <v>789</v>
       </c>
     </row>
-    <row r="254" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="254" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A254" t="s">
         <v>395</v>
       </c>
@@ -7091,11 +7107,11 @@
       <c r="D254">
         <v>1</v>
       </c>
-      <c r="H254" t="s">
+      <c r="I254" t="s">
         <v>791</v>
       </c>
     </row>
-    <row r="255" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="255" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A255" t="s">
         <v>397</v>
       </c>
@@ -7105,11 +7121,11 @@
       <c r="D255">
         <v>1</v>
       </c>
-      <c r="H255" t="s">
+      <c r="I255" t="s">
         <v>791</v>
       </c>
     </row>
-    <row r="256" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="256" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A256" t="s">
         <v>399</v>
       </c>
@@ -7119,7 +7135,7 @@
       <c r="D256">
         <v>1</v>
       </c>
-      <c r="H256" t="s">
+      <c r="I256" t="s">
         <v>791</v>
       </c>
     </row>

</xml_diff>